<commit_message>
Have cleaned up .gitignore file so that now, user data that is saved to User_Data folder will not be tracked by git. Finally figured that out.
</commit_message>
<xml_diff>
--- a/Macro_Chartist/Control.xlsx
+++ b/Macro_Chartist/Control.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesbishop/Documents/Python/Bootleg_Macro/Macro_Chartist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A044C5E5-FC80-4D47-9707-91C2D9191BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C51AA7-6411-EA40-98C3-05BFA9EACD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="477">
   <si>
     <t>Index</t>
   </si>
@@ -1599,37 +1599,10 @@
     <t>S &amp; P 500 in real terms</t>
   </si>
   <si>
-    <t>Dolllar dollar bill yo</t>
-  </si>
-  <si>
-    <t>Big rektums</t>
-  </si>
-  <si>
     <t>SPX/CPI</t>
   </si>
   <si>
     <t>U.S M2 Monetary aggregate</t>
-  </si>
-  <si>
-    <t>Rate of cunts what lost jobs, got rekt</t>
-  </si>
-  <si>
-    <t>Gross domestic income (GDI)</t>
-  </si>
-  <si>
-    <t>Still rekt cunts after some time.</t>
-  </si>
-  <si>
-    <t>TLAACBW027SBOG</t>
-  </si>
-  <si>
-    <t>Dunno what did shit id…</t>
-  </si>
-  <si>
-    <t>Dunno bro….............</t>
-  </si>
-  <si>
-    <t>a.u</t>
   </si>
   <si>
     <t>1990-01-01</t>
@@ -2315,29 +2288,125 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2364,21 +2433,21 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2388,119 +2457,23 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2916,7 +2889,7 @@
   <dimension ref="A1:AJ209"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -2982,7 +2955,7 @@
         <v>59</v>
       </c>
       <c r="D2" s="74" t="s">
-        <v>18</v>
+        <v>147</v>
       </c>
       <c r="E2" s="74" t="s">
         <v>19</v>
@@ -2991,7 +2964,7 @@
         <v>20</v>
       </c>
       <c r="G2" s="75" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="H2" s="75" t="s">
         <v>196</v>
@@ -3012,7 +2985,7 @@
         <v>59</v>
       </c>
       <c r="D3" s="74" t="s">
-        <v>18</v>
+        <v>147</v>
       </c>
       <c r="E3" s="74" t="s">
         <v>99</v>
@@ -3042,7 +3015,7 @@
         <v>59</v>
       </c>
       <c r="D4" s="74" t="s">
-        <v>18</v>
+        <v>147</v>
       </c>
       <c r="E4" s="74" t="s">
         <v>282</v>
@@ -3051,7 +3024,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="75" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="H4" s="75" t="s">
         <v>471</v>
@@ -3088,9 +3061,7 @@
       <c r="H5" s="75" t="s">
         <v>460</v>
       </c>
-      <c r="I5" s="78" t="s">
-        <v>469</v>
-      </c>
+      <c r="I5" s="78"/>
       <c r="J5" s="74" t="s">
         <v>43</v>
       </c>
@@ -3115,14 +3086,12 @@
         <v>20</v>
       </c>
       <c r="G6" s="75" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="H6" s="75" t="s">
         <v>460</v>
       </c>
-      <c r="I6" s="78" t="s">
-        <v>469</v>
-      </c>
+      <c r="I6" s="78"/>
       <c r="J6" s="76" t="s">
         <v>43</v>
       </c>
@@ -3131,215 +3100,139 @@
       <c r="A7" s="81">
         <v>6</v>
       </c>
-      <c r="B7" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="C7" s="73" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="74" t="s">
-        <v>147</v>
-      </c>
-      <c r="E7" s="74" t="s">
-        <v>77</v>
-      </c>
-      <c r="F7" s="74" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" s="75" t="s">
-        <v>477</v>
-      </c>
-      <c r="H7" s="75" t="s">
-        <v>221</v>
-      </c>
-      <c r="I7" s="85" t="s">
-        <v>469</v>
-      </c>
-      <c r="J7" s="76" t="s">
-        <v>43</v>
-      </c>
+      <c r="B7" s="37"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="76"/>
     </row>
     <row r="8" spans="1:36" ht="18" customHeight="1">
       <c r="A8" s="82">
         <v>7</v>
       </c>
-      <c r="B8" s="48" t="s">
-        <v>224</v>
-      </c>
-      <c r="C8" s="73" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="74" t="s">
-        <v>147</v>
-      </c>
-      <c r="E8" s="74" t="s">
-        <v>371</v>
-      </c>
-      <c r="F8" s="74" t="s">
-        <v>62</v>
-      </c>
-      <c r="G8" s="75" t="s">
-        <v>478</v>
-      </c>
-      <c r="H8" s="75" t="s">
-        <v>473</v>
-      </c>
-      <c r="I8" s="85" t="s">
-        <v>469</v>
-      </c>
-      <c r="J8" s="76" t="s">
-        <v>43</v>
-      </c>
+      <c r="B8" s="48"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="75"/>
+      <c r="I8" s="85"/>
+      <c r="J8" s="76"/>
     </row>
     <row r="9" spans="1:36" ht="18" customHeight="1">
       <c r="A9" s="81">
         <v>8</v>
       </c>
-      <c r="B9" s="72" t="s">
-        <v>219</v>
-      </c>
-      <c r="C9" s="73" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="74" t="s">
-        <v>147</v>
-      </c>
-      <c r="E9" s="74" t="s">
-        <v>324</v>
-      </c>
-      <c r="F9" s="74" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="75" t="s">
-        <v>479</v>
-      </c>
-      <c r="H9" s="75" t="s">
-        <v>474</v>
-      </c>
-      <c r="I9" s="85" t="s">
-        <v>469</v>
-      </c>
-      <c r="J9" s="76" t="s">
-        <v>43</v>
-      </c>
+      <c r="B9" s="72"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="76"/>
     </row>
     <row r="10" spans="1:36" ht="18" customHeight="1">
       <c r="A10" s="82">
         <v>9</v>
       </c>
-      <c r="B10" s="72" t="s">
-        <v>480</v>
-      </c>
-      <c r="C10" s="73" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="74" t="s">
-        <v>147</v>
-      </c>
+      <c r="B10" s="72"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="74"/>
       <c r="E10" s="74"/>
       <c r="F10" s="74"/>
-      <c r="G10" s="75" t="s">
-        <v>481</v>
-      </c>
-      <c r="H10" s="75" t="s">
-        <v>483</v>
-      </c>
-      <c r="I10" s="85" t="s">
-        <v>469</v>
-      </c>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="85"/>
       <c r="J10" s="76"/>
     </row>
     <row r="11" spans="1:36" ht="18" customHeight="1">
       <c r="A11" s="81">
         <v>10</v>
       </c>
-      <c r="B11" s="72" t="s">
-        <v>242</v>
-      </c>
-      <c r="C11" s="73" t="s">
-        <v>59</v>
-      </c>
+      <c r="B11" s="72"/>
+      <c r="C11" s="73"/>
       <c r="D11" s="74"/>
       <c r="E11" s="74"/>
       <c r="F11" s="74"/>
-      <c r="G11" s="75" t="s">
-        <v>482</v>
-      </c>
-      <c r="H11" s="75" t="s">
-        <v>483</v>
-      </c>
-      <c r="I11" s="85" t="s">
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="85"/>
+      <c r="J11" s="76"/>
+    </row>
+    <row r="12" spans="1:36" ht="18" customHeight="1">
+      <c r="A12" s="133" t="s">
+        <v>445</v>
+      </c>
+      <c r="B12" s="132" t="s">
+        <v>449</v>
+      </c>
+      <c r="C12" s="136" t="s">
+        <v>452</v>
+      </c>
+      <c r="D12" s="132" t="s">
+        <v>432</v>
+      </c>
+      <c r="E12" s="132" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="135" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="132" t="s">
+        <v>451</v>
+      </c>
+      <c r="H12" s="132" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="142" t="s">
         <v>469</v>
       </c>
-      <c r="J11" s="76"/>
-    </row>
-    <row r="12" spans="1:36" ht="18" customHeight="1">
-      <c r="A12" s="102" t="s">
-        <v>445</v>
-      </c>
-      <c r="B12" s="87" t="s">
-        <v>449</v>
-      </c>
-      <c r="C12" s="104" t="s">
-        <v>452</v>
-      </c>
-      <c r="D12" s="87" t="s">
-        <v>432</v>
-      </c>
-      <c r="E12" s="87" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="86" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="87" t="s">
-        <v>451</v>
-      </c>
-      <c r="H12" s="87" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" s="90" t="s">
-        <v>469</v>
-      </c>
-      <c r="J12" s="107" t="s">
+      <c r="J12" s="137" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:36" ht="18" customHeight="1">
-      <c r="A13" s="103"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="104"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="91"/>
-      <c r="J13" s="108"/>
+      <c r="A13" s="134"/>
+      <c r="B13" s="135"/>
+      <c r="C13" s="136"/>
+      <c r="D13" s="132"/>
+      <c r="E13" s="132"/>
+      <c r="F13" s="132"/>
+      <c r="G13" s="132"/>
+      <c r="H13" s="132"/>
+      <c r="I13" s="143"/>
+      <c r="J13" s="138"/>
     </row>
     <row r="14" spans="1:36" ht="18" customHeight="1">
-      <c r="A14" s="103"/>
-      <c r="B14" s="86"/>
-      <c r="C14" s="104"/>
-      <c r="D14" s="87"/>
-      <c r="E14" s="87"/>
-      <c r="F14" s="87"/>
-      <c r="G14" s="87"/>
-      <c r="H14" s="87"/>
-      <c r="I14" s="91"/>
-      <c r="J14" s="108"/>
+      <c r="A14" s="134"/>
+      <c r="B14" s="135"/>
+      <c r="C14" s="136"/>
+      <c r="D14" s="132"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="132"/>
+      <c r="G14" s="132"/>
+      <c r="H14" s="132"/>
+      <c r="I14" s="143"/>
+      <c r="J14" s="138"/>
     </row>
     <row r="15" spans="1:36" ht="25.5" customHeight="1">
-      <c r="A15" s="103"/>
-      <c r="B15" s="86"/>
-      <c r="C15" s="104"/>
-      <c r="D15" s="87"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87"/>
-      <c r="H15" s="87"/>
-      <c r="I15" s="92"/>
-      <c r="J15" s="109"/>
+      <c r="A15" s="134"/>
+      <c r="B15" s="135"/>
+      <c r="C15" s="136"/>
+      <c r="D15" s="132"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="132"/>
+      <c r="G15" s="132"/>
+      <c r="H15" s="132"/>
+      <c r="I15" s="144"/>
+      <c r="J15" s="139"/>
     </row>
     <row r="16" spans="1:36" ht="21" customHeight="1">
       <c r="A16" s="83" t="s">
@@ -3438,9 +3331,7 @@
       <c r="F18" s="6"/>
       <c r="G18" s="7"/>
       <c r="H18" s="6"/>
-      <c r="I18" s="8">
-        <v>34700</v>
-      </c>
+      <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="R18" s="13"/>
       <c r="S18" s="13"/>
@@ -3579,170 +3470,170 @@
       <c r="J26" s="8"/>
     </row>
     <row r="27" spans="1:36" ht="15.75" customHeight="1">
-      <c r="A27" s="129" t="s">
+      <c r="A27" s="123" t="s">
         <v>446</v>
       </c>
-      <c r="B27" s="128" t="s">
+      <c r="B27" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="128" t="s">
+      <c r="C27" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="105" t="s">
+      <c r="D27" s="100" t="s">
         <v>450</v>
       </c>
-      <c r="E27" s="137" t="s">
+      <c r="E27" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="88" t="s">
+      <c r="F27" s="140" t="s">
         <v>447</v>
       </c>
-      <c r="G27" s="89" t="s">
+      <c r="G27" s="141" t="s">
         <v>448</v>
       </c>
-      <c r="H27" s="127" t="s">
+      <c r="H27" s="121" t="s">
         <v>453</v>
       </c>
-      <c r="I27" s="105" t="s">
+      <c r="I27" s="100" t="s">
         <v>434</v>
       </c>
-      <c r="J27" s="105" t="s">
+      <c r="J27" s="100" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="28" spans="1:36" ht="15.75" customHeight="1">
-      <c r="A28" s="129"/>
-      <c r="B28" s="128"/>
-      <c r="C28" s="128"/>
-      <c r="D28" s="106"/>
-      <c r="E28" s="138"/>
-      <c r="F28" s="88"/>
-      <c r="G28" s="89"/>
-      <c r="H28" s="127"/>
-      <c r="I28" s="106"/>
-      <c r="J28" s="106"/>
+      <c r="A28" s="123"/>
+      <c r="B28" s="122"/>
+      <c r="C28" s="122"/>
+      <c r="D28" s="101"/>
+      <c r="E28" s="103"/>
+      <c r="F28" s="140"/>
+      <c r="G28" s="141"/>
+      <c r="H28" s="121"/>
+      <c r="I28" s="101"/>
+      <c r="J28" s="101"/>
     </row>
     <row r="29" spans="1:36" ht="15.75" customHeight="1">
-      <c r="A29" s="129"/>
-      <c r="B29" s="128"/>
-      <c r="C29" s="128"/>
-      <c r="D29" s="106"/>
-      <c r="E29" s="138"/>
-      <c r="F29" s="88"/>
-      <c r="G29" s="89"/>
-      <c r="H29" s="127"/>
-      <c r="I29" s="106"/>
-      <c r="J29" s="106"/>
+      <c r="A29" s="123"/>
+      <c r="B29" s="122"/>
+      <c r="C29" s="122"/>
+      <c r="D29" s="101"/>
+      <c r="E29" s="103"/>
+      <c r="F29" s="140"/>
+      <c r="G29" s="141"/>
+      <c r="H29" s="121"/>
+      <c r="I29" s="101"/>
+      <c r="J29" s="101"/>
     </row>
     <row r="30" spans="1:36" ht="15.75" customHeight="1">
-      <c r="A30" s="129"/>
-      <c r="B30" s="128"/>
-      <c r="C30" s="128"/>
-      <c r="D30" s="106"/>
-      <c r="E30" s="138"/>
-      <c r="F30" s="88"/>
-      <c r="G30" s="89"/>
-      <c r="H30" s="127"/>
-      <c r="I30" s="106"/>
-      <c r="J30" s="106"/>
+      <c r="A30" s="123"/>
+      <c r="B30" s="122"/>
+      <c r="C30" s="122"/>
+      <c r="D30" s="101"/>
+      <c r="E30" s="103"/>
+      <c r="F30" s="140"/>
+      <c r="G30" s="141"/>
+      <c r="H30" s="121"/>
+      <c r="I30" s="101"/>
+      <c r="J30" s="101"/>
     </row>
     <row r="31" spans="1:36" ht="15.75" customHeight="1">
-      <c r="A31" s="129"/>
-      <c r="B31" s="128"/>
-      <c r="C31" s="128"/>
-      <c r="D31" s="106"/>
-      <c r="E31" s="138"/>
-      <c r="F31" s="88"/>
-      <c r="G31" s="89"/>
-      <c r="H31" s="127"/>
-      <c r="I31" s="106"/>
-      <c r="J31" s="106"/>
+      <c r="A31" s="123"/>
+      <c r="B31" s="122"/>
+      <c r="C31" s="122"/>
+      <c r="D31" s="101"/>
+      <c r="E31" s="103"/>
+      <c r="F31" s="140"/>
+      <c r="G31" s="141"/>
+      <c r="H31" s="121"/>
+      <c r="I31" s="101"/>
+      <c r="J31" s="101"/>
     </row>
     <row r="32" spans="1:36" ht="15.75" customHeight="1">
-      <c r="A32" s="129"/>
-      <c r="B32" s="128"/>
-      <c r="C32" s="128"/>
-      <c r="D32" s="106"/>
-      <c r="E32" s="139"/>
-      <c r="F32" s="88"/>
-      <c r="G32" s="89"/>
-      <c r="H32" s="127"/>
-      <c r="I32" s="106"/>
-      <c r="J32" s="106"/>
+      <c r="A32" s="123"/>
+      <c r="B32" s="122"/>
+      <c r="C32" s="122"/>
+      <c r="D32" s="101"/>
+      <c r="E32" s="104"/>
+      <c r="F32" s="140"/>
+      <c r="G32" s="141"/>
+      <c r="H32" s="121"/>
+      <c r="I32" s="101"/>
+      <c r="J32" s="101"/>
     </row>
     <row r="33" spans="1:13" ht="22.5" customHeight="1">
-      <c r="A33" s="116" t="s">
+      <c r="A33" s="111" t="s">
         <v>461</v>
       </c>
-      <c r="B33" s="116"/>
-      <c r="C33" s="116"/>
-      <c r="D33" s="116"/>
-      <c r="E33" s="116"/>
-      <c r="F33" s="116"/>
-      <c r="G33" s="117"/>
-      <c r="H33" s="127"/>
-      <c r="I33" s="106"/>
-      <c r="J33" s="106"/>
+      <c r="B33" s="111"/>
+      <c r="C33" s="111"/>
+      <c r="D33" s="111"/>
+      <c r="E33" s="111"/>
+      <c r="F33" s="111"/>
+      <c r="G33" s="112"/>
+      <c r="H33" s="121"/>
+      <c r="I33" s="101"/>
+      <c r="J33" s="101"/>
     </row>
     <row r="34" spans="1:13" ht="22.5" customHeight="1">
-      <c r="A34" s="134"/>
-      <c r="B34" s="135"/>
-      <c r="C34" s="135"/>
-      <c r="D34" s="135"/>
-      <c r="E34" s="135"/>
-      <c r="F34" s="135"/>
-      <c r="G34" s="135"/>
-      <c r="H34" s="135"/>
-      <c r="I34" s="135"/>
-      <c r="J34" s="136"/>
+      <c r="A34" s="97"/>
+      <c r="B34" s="98"/>
+      <c r="C34" s="98"/>
+      <c r="D34" s="98"/>
+      <c r="E34" s="98"/>
+      <c r="F34" s="98"/>
+      <c r="G34" s="98"/>
+      <c r="H34" s="98"/>
+      <c r="I34" s="98"/>
+      <c r="J34" s="99"/>
     </row>
     <row r="35" spans="1:13" ht="22.5" customHeight="1">
-      <c r="A35" s="95" t="s">
+      <c r="A35" s="125" t="s">
         <v>456</v>
       </c>
-      <c r="B35" s="95"/>
-      <c r="C35" s="95"/>
-      <c r="D35" s="95"/>
-      <c r="E35" s="95"/>
-      <c r="F35" s="95"/>
-      <c r="G35" s="95"/>
-      <c r="H35" s="95"/>
-      <c r="I35" s="95"/>
-      <c r="J35" s="95"/>
+      <c r="B35" s="125"/>
+      <c r="C35" s="125"/>
+      <c r="D35" s="125"/>
+      <c r="E35" s="125"/>
+      <c r="F35" s="125"/>
+      <c r="G35" s="125"/>
+      <c r="H35" s="125"/>
+      <c r="I35" s="125"/>
+      <c r="J35" s="125"/>
     </row>
     <row r="36" spans="1:13" ht="18.75" customHeight="1">
       <c r="A36" s="14" t="s">
         <v>32</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>484</v>
-      </c>
-      <c r="C36" s="93" t="s">
+        <v>475</v>
+      </c>
+      <c r="C36" s="145" t="s">
         <v>33</v>
       </c>
-      <c r="D36" s="93"/>
-      <c r="E36" s="98"/>
-      <c r="F36" s="99"/>
-      <c r="G36" s="99"/>
-      <c r="H36" s="99"/>
-      <c r="I36" s="99"/>
-      <c r="J36" s="99"/>
+      <c r="D36" s="145"/>
+      <c r="E36" s="128"/>
+      <c r="F36" s="129"/>
+      <c r="G36" s="129"/>
+      <c r="H36" s="129"/>
+      <c r="I36" s="129"/>
+      <c r="J36" s="129"/>
     </row>
     <row r="37" spans="1:13" ht="16">
       <c r="A37" s="14" t="s">
         <v>34</v>
       </c>
       <c r="B37" s="15"/>
-      <c r="C37" s="96" t="s">
+      <c r="C37" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="D37" s="97"/>
-      <c r="E37" s="100"/>
-      <c r="F37" s="101"/>
-      <c r="G37" s="101"/>
-      <c r="H37" s="101"/>
-      <c r="I37" s="101"/>
-      <c r="J37" s="101"/>
+      <c r="D37" s="127"/>
+      <c r="E37" s="130"/>
+      <c r="F37" s="131"/>
+      <c r="G37" s="131"/>
+      <c r="H37" s="131"/>
+      <c r="I37" s="131"/>
+      <c r="J37" s="131"/>
       <c r="K37" s="13"/>
       <c r="L37" s="13"/>
     </row>
@@ -3750,17 +3641,17 @@
       <c r="A38" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="94"/>
-      <c r="C38" s="94"/>
-      <c r="D38" s="94"/>
-      <c r="E38" s="115" t="s">
+      <c r="B38" s="124"/>
+      <c r="C38" s="124"/>
+      <c r="D38" s="124"/>
+      <c r="E38" s="110" t="s">
         <v>435</v>
       </c>
-      <c r="F38" s="115"/>
-      <c r="G38" s="115"/>
-      <c r="H38" s="115"/>
-      <c r="I38" s="115"/>
-      <c r="J38" s="115"/>
+      <c r="F38" s="110"/>
+      <c r="G38" s="110"/>
+      <c r="H38" s="110"/>
+      <c r="I38" s="110"/>
+      <c r="J38" s="110"/>
       <c r="K38" s="65"/>
       <c r="L38" s="65"/>
     </row>
@@ -3768,21 +3659,21 @@
       <c r="A39" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="130" t="s">
+      <c r="B39" s="93" t="s">
         <v>472</v>
       </c>
-      <c r="C39" s="130"/>
-      <c r="D39" s="130"/>
-      <c r="E39" s="131"/>
-      <c r="F39" s="132" t="s">
+      <c r="C39" s="93"/>
+      <c r="D39" s="93"/>
+      <c r="E39" s="94"/>
+      <c r="F39" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="G39" s="133"/>
-      <c r="H39" s="113" t="s">
+      <c r="G39" s="96"/>
+      <c r="H39" s="108" t="s">
         <v>437</v>
       </c>
-      <c r="I39" s="114"/>
-      <c r="J39" s="114"/>
+      <c r="I39" s="109"/>
+      <c r="J39" s="109"/>
       <c r="K39" s="64"/>
       <c r="L39" s="64"/>
       <c r="M39" s="64"/>
@@ -3794,80 +3685,80 @@
       <c r="B40" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="118" t="s">
+      <c r="C40" s="113" t="s">
         <v>41</v>
       </c>
-      <c r="D40" s="118"/>
-      <c r="E40" s="118"/>
-      <c r="F40" s="118"/>
+      <c r="D40" s="113"/>
+      <c r="E40" s="113"/>
+      <c r="F40" s="113"/>
       <c r="G40" s="63"/>
-      <c r="H40" s="112" t="s">
+      <c r="H40" s="107" t="s">
         <v>455</v>
       </c>
-      <c r="I40" s="112"/>
-      <c r="J40" s="112"/>
+      <c r="I40" s="107"/>
+      <c r="J40" s="107"/>
       <c r="K40" s="64"/>
       <c r="L40" s="64"/>
       <c r="M40" s="64"/>
     </row>
     <row r="41" spans="1:13" ht="13" customHeight="1">
-      <c r="A41" s="126"/>
-      <c r="B41" s="126"/>
-      <c r="C41" s="126"/>
-      <c r="D41" s="126"/>
-      <c r="E41" s="126"/>
-      <c r="F41" s="126"/>
-      <c r="G41" s="126"/>
-      <c r="H41" s="112"/>
-      <c r="I41" s="112"/>
-      <c r="J41" s="112"/>
+      <c r="A41" s="120"/>
+      <c r="B41" s="120"/>
+      <c r="C41" s="120"/>
+      <c r="D41" s="120"/>
+      <c r="E41" s="120"/>
+      <c r="F41" s="120"/>
+      <c r="G41" s="120"/>
+      <c r="H41" s="107"/>
+      <c r="I41" s="107"/>
+      <c r="J41" s="107"/>
       <c r="K41" s="64"/>
       <c r="L41" s="64"/>
       <c r="M41" s="64"/>
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A42" s="126"/>
-      <c r="B42" s="126"/>
-      <c r="C42" s="126"/>
-      <c r="D42" s="126"/>
-      <c r="E42" s="126"/>
-      <c r="F42" s="126"/>
-      <c r="G42" s="126"/>
-      <c r="H42" s="112"/>
-      <c r="I42" s="112"/>
-      <c r="J42" s="112"/>
+      <c r="A42" s="120"/>
+      <c r="B42" s="120"/>
+      <c r="C42" s="120"/>
+      <c r="D42" s="120"/>
+      <c r="E42" s="120"/>
+      <c r="F42" s="120"/>
+      <c r="G42" s="120"/>
+      <c r="H42" s="107"/>
+      <c r="I42" s="107"/>
+      <c r="J42" s="107"/>
       <c r="K42" s="64"/>
       <c r="L42" s="64"/>
       <c r="M42" s="64"/>
     </row>
     <row r="43" spans="1:13" ht="13" customHeight="1">
-      <c r="A43" s="126"/>
-      <c r="B43" s="126"/>
-      <c r="C43" s="126"/>
-      <c r="D43" s="126"/>
-      <c r="E43" s="126"/>
-      <c r="F43" s="126"/>
-      <c r="G43" s="126"/>
-      <c r="H43" s="112"/>
-      <c r="I43" s="112"/>
-      <c r="J43" s="112"/>
+      <c r="A43" s="120"/>
+      <c r="B43" s="120"/>
+      <c r="C43" s="120"/>
+      <c r="D43" s="120"/>
+      <c r="E43" s="120"/>
+      <c r="F43" s="120"/>
+      <c r="G43" s="120"/>
+      <c r="H43" s="107"/>
+      <c r="I43" s="107"/>
+      <c r="J43" s="107"/>
       <c r="K43" s="64"/>
       <c r="L43" s="64"/>
       <c r="M43" s="64"/>
     </row>
     <row r="44" spans="1:13" ht="18">
-      <c r="A44" s="122" t="s">
+      <c r="A44" s="117" t="s">
         <v>454</v>
       </c>
-      <c r="B44" s="123"/>
-      <c r="C44" s="123"/>
-      <c r="D44" s="123"/>
-      <c r="E44" s="123"/>
-      <c r="F44" s="123"/>
-      <c r="G44" s="123"/>
-      <c r="H44" s="112"/>
-      <c r="I44" s="112"/>
-      <c r="J44" s="112"/>
+      <c r="B44" s="118"/>
+      <c r="C44" s="118"/>
+      <c r="D44" s="118"/>
+      <c r="E44" s="118"/>
+      <c r="F44" s="118"/>
+      <c r="G44" s="118"/>
+      <c r="H44" s="107"/>
+      <c r="I44" s="107"/>
+      <c r="J44" s="107"/>
       <c r="K44" s="64"/>
       <c r="L44" s="64"/>
       <c r="M44" s="64"/>
@@ -3879,16 +3770,16 @@
       <c r="B45" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="124" t="s">
+      <c r="C45" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="D45" s="125"/>
-      <c r="E45" s="125"/>
-      <c r="F45" s="125"/>
-      <c r="G45" s="125"/>
-      <c r="H45" s="112"/>
-      <c r="I45" s="112"/>
-      <c r="J45" s="112"/>
+      <c r="D45" s="119"/>
+      <c r="E45" s="119"/>
+      <c r="F45" s="119"/>
+      <c r="G45" s="119"/>
+      <c r="H45" s="107"/>
+      <c r="I45" s="107"/>
+      <c r="J45" s="107"/>
       <c r="K45" s="64"/>
       <c r="L45" s="64"/>
       <c r="M45" s="64"/>
@@ -3898,16 +3789,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="19"/>
-      <c r="C46" s="119" t="s">
+      <c r="C46" s="114" t="s">
         <v>46</v>
       </c>
-      <c r="D46" s="119"/>
-      <c r="E46" s="119"/>
-      <c r="F46" s="119"/>
-      <c r="G46" s="120"/>
-      <c r="H46" s="112"/>
-      <c r="I46" s="112"/>
-      <c r="J46" s="112"/>
+      <c r="D46" s="114"/>
+      <c r="E46" s="114"/>
+      <c r="F46" s="114"/>
+      <c r="G46" s="115"/>
+      <c r="H46" s="107"/>
+      <c r="I46" s="107"/>
+      <c r="J46" s="107"/>
       <c r="K46" s="64"/>
       <c r="L46" s="64"/>
       <c r="M46" s="64"/>
@@ -3917,41 +3808,41 @@
         <v>47</v>
       </c>
       <c r="B47" s="19"/>
-      <c r="C47" s="119" t="s">
+      <c r="C47" s="114" t="s">
         <v>48</v>
       </c>
-      <c r="D47" s="119"/>
-      <c r="E47" s="119"/>
-      <c r="F47" s="119"/>
-      <c r="G47" s="120"/>
-      <c r="H47" s="112"/>
-      <c r="I47" s="112"/>
-      <c r="J47" s="112"/>
+      <c r="D47" s="114"/>
+      <c r="E47" s="114"/>
+      <c r="F47" s="114"/>
+      <c r="G47" s="115"/>
+      <c r="H47" s="107"/>
+      <c r="I47" s="107"/>
+      <c r="J47" s="107"/>
       <c r="K47" s="64"/>
       <c r="L47" s="64"/>
       <c r="M47" s="64"/>
     </row>
     <row r="48" spans="1:13" ht="13" customHeight="1">
-      <c r="H48" s="112"/>
-      <c r="I48" s="112"/>
-      <c r="J48" s="112"/>
+      <c r="H48" s="107"/>
+      <c r="I48" s="107"/>
+      <c r="J48" s="107"/>
       <c r="K48" s="64"/>
       <c r="L48" s="64"/>
       <c r="M48" s="64"/>
     </row>
     <row r="49" spans="1:14" ht="25" customHeight="1">
-      <c r="A49" s="110" t="s">
+      <c r="A49" s="105" t="s">
         <v>436</v>
       </c>
-      <c r="B49" s="110"/>
-      <c r="C49" s="110"/>
-      <c r="D49" s="110"/>
-      <c r="E49" s="110"/>
-      <c r="F49" s="110"/>
-      <c r="G49" s="111"/>
-      <c r="H49" s="112"/>
-      <c r="I49" s="112"/>
-      <c r="J49" s="112"/>
+      <c r="B49" s="105"/>
+      <c r="C49" s="105"/>
+      <c r="D49" s="105"/>
+      <c r="E49" s="105"/>
+      <c r="F49" s="105"/>
+      <c r="G49" s="106"/>
+      <c r="H49" s="107"/>
+      <c r="I49" s="107"/>
+      <c r="J49" s="107"/>
       <c r="K49" s="64"/>
       <c r="L49" s="64"/>
       <c r="M49" s="64"/>
@@ -3963,16 +3854,16 @@
       <c r="B50" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C50" s="118" t="s">
+      <c r="C50" s="113" t="s">
         <v>50</v>
       </c>
-      <c r="D50" s="118"/>
-      <c r="E50" s="118"/>
-      <c r="F50" s="118"/>
-      <c r="G50" s="121"/>
-      <c r="H50" s="112"/>
-      <c r="I50" s="112"/>
-      <c r="J50" s="112"/>
+      <c r="D50" s="113"/>
+      <c r="E50" s="113"/>
+      <c r="F50" s="113"/>
+      <c r="G50" s="116"/>
+      <c r="H50" s="107"/>
+      <c r="I50" s="107"/>
+      <c r="J50" s="107"/>
       <c r="K50" s="64"/>
       <c r="L50" s="64"/>
       <c r="M50" s="64"/>
@@ -3985,25 +3876,25 @@
       <c r="B51" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C51" s="145" t="s">
+      <c r="C51" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="D51" s="145"/>
-      <c r="E51" s="145"/>
-      <c r="F51" s="145"/>
-      <c r="G51" s="124"/>
-      <c r="H51" s="112"/>
-      <c r="I51" s="112"/>
-      <c r="J51" s="112"/>
+      <c r="D51" s="91"/>
+      <c r="E51" s="91"/>
+      <c r="F51" s="91"/>
+      <c r="G51" s="92"/>
+      <c r="H51" s="107"/>
+      <c r="I51" s="107"/>
+      <c r="J51" s="107"/>
       <c r="K51" s="64"/>
       <c r="L51" s="64"/>
       <c r="M51" s="64"/>
       <c r="N51" s="13"/>
     </row>
     <row r="52" spans="1:14" ht="13" customHeight="1">
-      <c r="H52" s="112"/>
-      <c r="I52" s="112"/>
-      <c r="J52" s="112"/>
+      <c r="H52" s="107"/>
+      <c r="I52" s="107"/>
+      <c r="J52" s="107"/>
       <c r="K52" s="64"/>
       <c r="L52" s="64"/>
       <c r="M52" s="64"/>
@@ -4013,19 +3904,19 @@
       <c r="A53" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="143" t="s">
+      <c r="B53" s="89" t="s">
         <v>428</v>
       </c>
-      <c r="C53" s="143"/>
-      <c r="D53" s="143"/>
-      <c r="E53" s="144"/>
-      <c r="F53" s="141" t="s">
+      <c r="C53" s="89"/>
+      <c r="D53" s="89"/>
+      <c r="E53" s="90"/>
+      <c r="F53" s="87" t="s">
         <v>438</v>
       </c>
-      <c r="G53" s="142"/>
-      <c r="H53" s="142"/>
-      <c r="I53" s="142"/>
-      <c r="J53" s="142"/>
+      <c r="G53" s="88"/>
+      <c r="H53" s="88"/>
+      <c r="I53" s="88"/>
+      <c r="J53" s="88"/>
       <c r="K53" s="66"/>
       <c r="L53" s="66"/>
       <c r="M53" s="66"/>
@@ -4037,28 +3928,28 @@
       <c r="C54" s="13"/>
       <c r="D54" s="13"/>
       <c r="E54" s="13"/>
-      <c r="F54" s="142"/>
-      <c r="G54" s="142"/>
-      <c r="H54" s="142"/>
-      <c r="I54" s="142"/>
-      <c r="J54" s="142"/>
+      <c r="F54" s="88"/>
+      <c r="G54" s="88"/>
+      <c r="H54" s="88"/>
+      <c r="I54" s="88"/>
+      <c r="J54" s="88"/>
       <c r="K54" s="66"/>
       <c r="L54" s="66"/>
       <c r="M54" s="66"/>
     </row>
     <row r="55" spans="1:14">
-      <c r="F55" s="142"/>
-      <c r="G55" s="142"/>
-      <c r="H55" s="142"/>
-      <c r="I55" s="142"/>
-      <c r="J55" s="142"/>
+      <c r="F55" s="88"/>
+      <c r="G55" s="88"/>
+      <c r="H55" s="88"/>
+      <c r="I55" s="88"/>
+      <c r="J55" s="88"/>
     </row>
     <row r="56" spans="1:14">
-      <c r="F56" s="142"/>
-      <c r="G56" s="142"/>
-      <c r="H56" s="142"/>
-      <c r="I56" s="142"/>
-      <c r="J56" s="142"/>
+      <c r="F56" s="88"/>
+      <c r="G56" s="88"/>
+      <c r="H56" s="88"/>
+      <c r="I56" s="88"/>
+      <c r="J56" s="88"/>
       <c r="N56" s="13"/>
     </row>
     <row r="57" spans="1:14">
@@ -4176,14 +4067,14 @@
     <row r="64" spans="1:14" ht="13" customHeight="1">
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
-      <c r="C64" s="140"/>
-      <c r="D64" s="140"/>
-      <c r="E64" s="140"/>
-      <c r="F64" s="140"/>
-      <c r="G64" s="140"/>
-      <c r="H64" s="140"/>
-      <c r="I64" s="140"/>
-      <c r="J64" s="140"/>
+      <c r="C64" s="86"/>
+      <c r="D64" s="86"/>
+      <c r="E64" s="86"/>
+      <c r="F64" s="86"/>
+      <c r="G64" s="86"/>
+      <c r="H64" s="86"/>
+      <c r="I64" s="86"/>
+      <c r="J64" s="86"/>
       <c r="K64" s="13"/>
       <c r="L64" s="13"/>
       <c r="M64" s="13"/>
@@ -4245,14 +4136,14 @@
       <c r="N68" s="13"/>
     </row>
     <row r="69" spans="1:14">
-      <c r="C69" s="140"/>
-      <c r="D69" s="140"/>
-      <c r="E69" s="140"/>
-      <c r="F69" s="140"/>
-      <c r="G69" s="140"/>
-      <c r="H69" s="140"/>
-      <c r="I69" s="140"/>
-      <c r="J69" s="140"/>
+      <c r="C69" s="86"/>
+      <c r="D69" s="86"/>
+      <c r="E69" s="86"/>
+      <c r="F69" s="86"/>
+      <c r="G69" s="86"/>
+      <c r="H69" s="86"/>
+      <c r="I69" s="86"/>
+      <c r="J69" s="86"/>
       <c r="K69" s="13"/>
       <c r="L69" s="13"/>
       <c r="M69" s="13"/>
@@ -5800,16 +5691,18 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="C64:J64"/>
-    <mergeCell ref="C69:J69"/>
-    <mergeCell ref="F53:J56"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="C51:G51"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="A34:J34"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="E12:E15"/>
     <mergeCell ref="A49:G49"/>
     <mergeCell ref="H40:J52"/>
     <mergeCell ref="H39:J39"/>
@@ -5826,25 +5719,23 @@
     <mergeCell ref="C27:C32"/>
     <mergeCell ref="B27:B32"/>
     <mergeCell ref="A27:A32"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="A34:J34"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="E27:E32"/>
     <mergeCell ref="B38:D38"/>
     <mergeCell ref="A35:J35"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="E36:J37"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="E12:E15"/>
     <mergeCell ref="I27:I33"/>
     <mergeCell ref="J27:J33"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="I12:I15"/>
     <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C64:J64"/>
+    <mergeCell ref="C69:J69"/>
+    <mergeCell ref="F53:J56"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="C51:G51"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B40 B45" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>

<commit_message>
Get ABS series via subprocess using R implemented. Eliminated reiance upon python rpy2 package which does not work on windows.
</commit_message>
<xml_diff>
--- a/Macro_Chartist/Control.xlsx
+++ b/Macro_Chartist/Control.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesbishop/Documents/Python/Bootleg_Macro/Macro_Chartist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADA8EA2-6C6A-184F-A6EB-2CB6C29C3F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D9A856-9EA5-5445-885C-3799C9669F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="480">
   <si>
     <t>Index</t>
   </si>
@@ -1613,10 +1613,16 @@
     <t>Interest Paid on home loans in Australia</t>
   </si>
   <si>
-    <t>A2422351V</t>
-  </si>
-  <si>
     <t>Consumption of Fixed Capital (Aus)</t>
+  </si>
+  <si>
+    <t>A130118747J</t>
+  </si>
+  <si>
+    <t>A3605929A</t>
+  </si>
+  <si>
+    <t>Rent price expenditures..</t>
   </si>
 </sst>
 </file>
@@ -2221,6 +2227,75 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -2233,9 +2308,6 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2255,69 +2327,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2326,9 +2335,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2594,7 +2600,7 @@
   <dimension ref="A1:AJ209"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -2685,7 +2691,7 @@
         <v>468</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>90</v>
+        <v>467</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>12</v>
@@ -2710,10 +2716,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>90</v>
+        <v>467</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>12</v>
@@ -2725,7 +2731,7 @@
         <v>14</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>473</v>
@@ -2737,13 +2743,27 @@
       <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
+      <c r="B5" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>473</v>
+      </c>
       <c r="I5" s="11"/>
       <c r="J5" s="9"/>
     </row>
@@ -2832,72 +2852,72 @@
       <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:36" ht="18" customHeight="1">
-      <c r="A12" s="115" t="s">
+      <c r="A12" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="90" t="s">
+      <c r="B12" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="116" t="s">
+      <c r="C12" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="90" t="s">
+      <c r="D12" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="90" t="s">
+      <c r="E12" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="114" t="s">
+      <c r="F12" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="90" t="s">
+      <c r="G12" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="90" t="s">
+      <c r="H12" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="110" t="s">
+      <c r="I12" s="91" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="90" t="s">
+      <c r="J12" s="88" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:36" ht="18" customHeight="1">
-      <c r="A13" s="115"/>
-      <c r="B13" s="90"/>
-      <c r="C13" s="116"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="90"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="90"/>
-      <c r="I13" s="110"/>
-      <c r="J13" s="90"/>
+      <c r="A13" s="87"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="88"/>
+      <c r="G13" s="88"/>
+      <c r="H13" s="88"/>
+      <c r="I13" s="91"/>
+      <c r="J13" s="88"/>
     </row>
     <row r="14" spans="1:36" ht="18" customHeight="1">
-      <c r="A14" s="115"/>
-      <c r="B14" s="90"/>
-      <c r="C14" s="116"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="90"/>
-      <c r="I14" s="110"/>
-      <c r="J14" s="90"/>
+      <c r="A14" s="87"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="88"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="91"/>
+      <c r="J14" s="88"/>
     </row>
     <row r="15" spans="1:36" ht="25.5" customHeight="1">
-      <c r="A15" s="115"/>
-      <c r="B15" s="90"/>
-      <c r="C15" s="116"/>
-      <c r="D15" s="90"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="90"/>
-      <c r="G15" s="90"/>
-      <c r="H15" s="90"/>
-      <c r="I15" s="110"/>
-      <c r="J15" s="90"/>
+      <c r="A15" s="87"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="88"/>
+      <c r="G15" s="88"/>
+      <c r="H15" s="88"/>
+      <c r="I15" s="91"/>
+      <c r="J15" s="88"/>
     </row>
     <row r="16" spans="1:36" ht="21" customHeight="1">
       <c r="A16" s="18" t="s">
@@ -3129,136 +3149,136 @@
       <c r="J26" s="25"/>
     </row>
     <row r="27" spans="1:36" ht="15.75" customHeight="1">
-      <c r="A27" s="112" t="s">
+      <c r="A27" s="96" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="113" t="s">
+      <c r="B27" s="97" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="113" t="s">
+      <c r="C27" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="110" t="s">
+      <c r="D27" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="109" t="s">
+      <c r="E27" s="94" t="s">
         <v>51</v>
       </c>
-      <c r="F27" s="107" t="s">
+      <c r="F27" s="92" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="108" t="s">
+      <c r="G27" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="H27" s="109" t="s">
+      <c r="H27" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="I27" s="110" t="s">
+      <c r="I27" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="J27" s="110" t="s">
+      <c r="J27" s="91" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:36" ht="15.75" customHeight="1">
-      <c r="A28" s="112"/>
-      <c r="B28" s="113"/>
-      <c r="C28" s="113"/>
-      <c r="D28" s="110"/>
-      <c r="E28" s="109"/>
-      <c r="F28" s="107"/>
-      <c r="G28" s="108"/>
-      <c r="H28" s="109"/>
-      <c r="I28" s="110"/>
-      <c r="J28" s="110"/>
+      <c r="A28" s="96"/>
+      <c r="B28" s="97"/>
+      <c r="C28" s="97"/>
+      <c r="D28" s="91"/>
+      <c r="E28" s="94"/>
+      <c r="F28" s="92"/>
+      <c r="G28" s="93"/>
+      <c r="H28" s="94"/>
+      <c r="I28" s="91"/>
+      <c r="J28" s="91"/>
     </row>
     <row r="29" spans="1:36" ht="15.75" customHeight="1">
-      <c r="A29" s="112"/>
-      <c r="B29" s="113"/>
-      <c r="C29" s="113"/>
-      <c r="D29" s="110"/>
-      <c r="E29" s="109"/>
-      <c r="F29" s="107"/>
-      <c r="G29" s="108"/>
-      <c r="H29" s="109"/>
-      <c r="I29" s="110"/>
-      <c r="J29" s="110"/>
+      <c r="A29" s="96"/>
+      <c r="B29" s="97"/>
+      <c r="C29" s="97"/>
+      <c r="D29" s="91"/>
+      <c r="E29" s="94"/>
+      <c r="F29" s="92"/>
+      <c r="G29" s="93"/>
+      <c r="H29" s="94"/>
+      <c r="I29" s="91"/>
+      <c r="J29" s="91"/>
     </row>
     <row r="30" spans="1:36" ht="15.75" customHeight="1">
-      <c r="A30" s="112"/>
-      <c r="B30" s="113"/>
-      <c r="C30" s="113"/>
-      <c r="D30" s="110"/>
-      <c r="E30" s="109"/>
-      <c r="F30" s="107"/>
-      <c r="G30" s="108"/>
-      <c r="H30" s="109"/>
-      <c r="I30" s="110"/>
-      <c r="J30" s="110"/>
+      <c r="A30" s="96"/>
+      <c r="B30" s="97"/>
+      <c r="C30" s="97"/>
+      <c r="D30" s="91"/>
+      <c r="E30" s="94"/>
+      <c r="F30" s="92"/>
+      <c r="G30" s="93"/>
+      <c r="H30" s="94"/>
+      <c r="I30" s="91"/>
+      <c r="J30" s="91"/>
     </row>
     <row r="31" spans="1:36" ht="15.75" customHeight="1">
-      <c r="A31" s="112"/>
-      <c r="B31" s="113"/>
-      <c r="C31" s="113"/>
-      <c r="D31" s="110"/>
-      <c r="E31" s="109"/>
-      <c r="F31" s="107"/>
-      <c r="G31" s="108"/>
-      <c r="H31" s="109"/>
-      <c r="I31" s="110"/>
-      <c r="J31" s="110"/>
+      <c r="A31" s="96"/>
+      <c r="B31" s="97"/>
+      <c r="C31" s="97"/>
+      <c r="D31" s="91"/>
+      <c r="E31" s="94"/>
+      <c r="F31" s="92"/>
+      <c r="G31" s="93"/>
+      <c r="H31" s="94"/>
+      <c r="I31" s="91"/>
+      <c r="J31" s="91"/>
     </row>
     <row r="32" spans="1:36" ht="15.75" customHeight="1">
-      <c r="A32" s="112"/>
-      <c r="B32" s="113"/>
-      <c r="C32" s="113"/>
-      <c r="D32" s="110"/>
-      <c r="E32" s="109"/>
-      <c r="F32" s="107"/>
-      <c r="G32" s="108"/>
-      <c r="H32" s="109"/>
-      <c r="I32" s="110"/>
-      <c r="J32" s="110"/>
+      <c r="A32" s="96"/>
+      <c r="B32" s="97"/>
+      <c r="C32" s="97"/>
+      <c r="D32" s="91"/>
+      <c r="E32" s="94"/>
+      <c r="F32" s="92"/>
+      <c r="G32" s="93"/>
+      <c r="H32" s="94"/>
+      <c r="I32" s="91"/>
+      <c r="J32" s="91"/>
     </row>
     <row r="33" spans="1:13" ht="22.5" customHeight="1">
-      <c r="A33" s="111" t="s">
+      <c r="A33" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="111"/>
-      <c r="C33" s="111"/>
-      <c r="D33" s="111"/>
-      <c r="E33" s="111"/>
-      <c r="F33" s="111"/>
-      <c r="G33" s="111"/>
-      <c r="H33" s="109"/>
-      <c r="I33" s="110"/>
-      <c r="J33" s="110"/>
+      <c r="B33" s="95"/>
+      <c r="C33" s="95"/>
+      <c r="D33" s="95"/>
+      <c r="E33" s="95"/>
+      <c r="F33" s="95"/>
+      <c r="G33" s="95"/>
+      <c r="H33" s="94"/>
+      <c r="I33" s="91"/>
+      <c r="J33" s="91"/>
     </row>
     <row r="34" spans="1:13" ht="22.5" customHeight="1">
-      <c r="A34" s="102"/>
-      <c r="B34" s="102"/>
-      <c r="C34" s="102"/>
-      <c r="D34" s="102"/>
-      <c r="E34" s="102"/>
-      <c r="F34" s="102"/>
-      <c r="G34" s="102"/>
-      <c r="H34" s="102"/>
-      <c r="I34" s="102"/>
-      <c r="J34" s="102"/>
+      <c r="A34" s="98"/>
+      <c r="B34" s="98"/>
+      <c r="C34" s="98"/>
+      <c r="D34" s="98"/>
+      <c r="E34" s="98"/>
+      <c r="F34" s="98"/>
+      <c r="G34" s="98"/>
+      <c r="H34" s="98"/>
+      <c r="I34" s="98"/>
+      <c r="J34" s="98"/>
     </row>
     <row r="35" spans="1:13" ht="22.5" customHeight="1">
-      <c r="A35" s="103" t="s">
+      <c r="A35" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="103"/>
-      <c r="C35" s="103"/>
-      <c r="D35" s="103"/>
-      <c r="E35" s="103"/>
-      <c r="F35" s="103"/>
-      <c r="G35" s="103"/>
-      <c r="H35" s="103"/>
-      <c r="I35" s="103"/>
-      <c r="J35" s="103"/>
+      <c r="B35" s="99"/>
+      <c r="C35" s="99"/>
+      <c r="D35" s="99"/>
+      <c r="E35" s="99"/>
+      <c r="F35" s="99"/>
+      <c r="G35" s="99"/>
+      <c r="H35" s="99"/>
+      <c r="I35" s="99"/>
+      <c r="J35" s="99"/>
     </row>
     <row r="36" spans="1:13" ht="18.75" customHeight="1">
       <c r="A36" s="30" t="s">
@@ -3267,32 +3287,32 @@
       <c r="B36" s="31" t="s">
         <v>474</v>
       </c>
-      <c r="C36" s="104" t="s">
+      <c r="C36" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="D36" s="104"/>
-      <c r="E36" s="105"/>
-      <c r="F36" s="105"/>
-      <c r="G36" s="105"/>
-      <c r="H36" s="105"/>
-      <c r="I36" s="105"/>
-      <c r="J36" s="105"/>
+      <c r="D36" s="100"/>
+      <c r="E36" s="101"/>
+      <c r="F36" s="101"/>
+      <c r="G36" s="101"/>
+      <c r="H36" s="101"/>
+      <c r="I36" s="101"/>
+      <c r="J36" s="101"/>
     </row>
     <row r="37" spans="1:13" ht="16">
       <c r="A37" s="30" t="s">
         <v>61</v>
       </c>
       <c r="B37" s="31"/>
-      <c r="C37" s="106" t="s">
+      <c r="C37" s="102" t="s">
         <v>62</v>
       </c>
-      <c r="D37" s="106"/>
-      <c r="E37" s="105"/>
-      <c r="F37" s="105"/>
-      <c r="G37" s="105"/>
-      <c r="H37" s="105"/>
-      <c r="I37" s="105"/>
-      <c r="J37" s="105"/>
+      <c r="D37" s="102"/>
+      <c r="E37" s="101"/>
+      <c r="F37" s="101"/>
+      <c r="G37" s="101"/>
+      <c r="H37" s="101"/>
+      <c r="I37" s="101"/>
+      <c r="J37" s="101"/>
       <c r="K37" s="20"/>
       <c r="L37" s="20"/>
     </row>
@@ -3300,17 +3320,17 @@
       <c r="A38" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="B38" s="97"/>
-      <c r="C38" s="97"/>
-      <c r="D38" s="97"/>
-      <c r="E38" s="98" t="s">
+      <c r="B38" s="103"/>
+      <c r="C38" s="103"/>
+      <c r="D38" s="103"/>
+      <c r="E38" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="F38" s="98"/>
-      <c r="G38" s="98"/>
-      <c r="H38" s="98"/>
-      <c r="I38" s="98"/>
-      <c r="J38" s="98"/>
+      <c r="F38" s="104"/>
+      <c r="G38" s="104"/>
+      <c r="H38" s="104"/>
+      <c r="I38" s="104"/>
+      <c r="J38" s="104"/>
       <c r="K38" s="33"/>
       <c r="L38" s="33"/>
     </row>
@@ -3318,21 +3338,21 @@
       <c r="A39" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="B39" s="99" t="s">
+      <c r="B39" s="105" t="s">
         <v>475</v>
       </c>
-      <c r="C39" s="99"/>
-      <c r="D39" s="99"/>
-      <c r="E39" s="99"/>
-      <c r="F39" s="100" t="s">
+      <c r="C39" s="105"/>
+      <c r="D39" s="105"/>
+      <c r="E39" s="105"/>
+      <c r="F39" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="G39" s="100"/>
-      <c r="H39" s="101" t="s">
+      <c r="G39" s="106"/>
+      <c r="H39" s="107" t="s">
         <v>67</v>
       </c>
-      <c r="I39" s="101"/>
-      <c r="J39" s="101"/>
+      <c r="I39" s="107"/>
+      <c r="J39" s="107"/>
       <c r="K39" s="34"/>
       <c r="L39" s="34"/>
       <c r="M39" s="34"/>
@@ -3344,80 +3364,80 @@
       <c r="B40" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="89" t="s">
+      <c r="C40" s="111" t="s">
         <v>69</v>
       </c>
-      <c r="D40" s="89"/>
-      <c r="E40" s="89"/>
-      <c r="F40" s="89"/>
+      <c r="D40" s="111"/>
+      <c r="E40" s="111"/>
+      <c r="F40" s="111"/>
       <c r="G40" s="37"/>
-      <c r="H40" s="90" t="s">
+      <c r="H40" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="I40" s="90"/>
-      <c r="J40" s="90"/>
+      <c r="I40" s="88"/>
+      <c r="J40" s="88"/>
       <c r="K40" s="34"/>
       <c r="L40" s="34"/>
       <c r="M40" s="34"/>
     </row>
     <row r="41" spans="1:13" ht="12.75" customHeight="1">
-      <c r="A41" s="91"/>
-      <c r="B41" s="91"/>
-      <c r="C41" s="91"/>
-      <c r="D41" s="91"/>
-      <c r="E41" s="91"/>
-      <c r="F41" s="91"/>
-      <c r="G41" s="91"/>
-      <c r="H41" s="90"/>
-      <c r="I41" s="90"/>
-      <c r="J41" s="90"/>
+      <c r="A41" s="112"/>
+      <c r="B41" s="112"/>
+      <c r="C41" s="112"/>
+      <c r="D41" s="112"/>
+      <c r="E41" s="112"/>
+      <c r="F41" s="112"/>
+      <c r="G41" s="112"/>
+      <c r="H41" s="88"/>
+      <c r="I41" s="88"/>
+      <c r="J41" s="88"/>
       <c r="K41" s="34"/>
       <c r="L41" s="34"/>
       <c r="M41" s="34"/>
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A42" s="91"/>
-      <c r="B42" s="91"/>
-      <c r="C42" s="91"/>
-      <c r="D42" s="91"/>
-      <c r="E42" s="91"/>
-      <c r="F42" s="91"/>
-      <c r="G42" s="91"/>
-      <c r="H42" s="90"/>
-      <c r="I42" s="90"/>
-      <c r="J42" s="90"/>
+      <c r="A42" s="112"/>
+      <c r="B42" s="112"/>
+      <c r="C42" s="112"/>
+      <c r="D42" s="112"/>
+      <c r="E42" s="112"/>
+      <c r="F42" s="112"/>
+      <c r="G42" s="112"/>
+      <c r="H42" s="88"/>
+      <c r="I42" s="88"/>
+      <c r="J42" s="88"/>
       <c r="K42" s="34"/>
       <c r="L42" s="34"/>
       <c r="M42" s="34"/>
     </row>
     <row r="43" spans="1:13" ht="12.75" customHeight="1">
-      <c r="A43" s="91"/>
-      <c r="B43" s="91"/>
-      <c r="C43" s="91"/>
-      <c r="D43" s="91"/>
-      <c r="E43" s="91"/>
-      <c r="F43" s="91"/>
-      <c r="G43" s="91"/>
-      <c r="H43" s="90"/>
-      <c r="I43" s="90"/>
-      <c r="J43" s="90"/>
+      <c r="A43" s="112"/>
+      <c r="B43" s="112"/>
+      <c r="C43" s="112"/>
+      <c r="D43" s="112"/>
+      <c r="E43" s="112"/>
+      <c r="F43" s="112"/>
+      <c r="G43" s="112"/>
+      <c r="H43" s="88"/>
+      <c r="I43" s="88"/>
+      <c r="J43" s="88"/>
       <c r="K43" s="34"/>
       <c r="L43" s="34"/>
       <c r="M43" s="34"/>
     </row>
     <row r="44" spans="1:13" ht="18">
-      <c r="A44" s="92" t="s">
+      <c r="A44" s="113" t="s">
         <v>71</v>
       </c>
-      <c r="B44" s="92"/>
-      <c r="C44" s="92"/>
-      <c r="D44" s="92"/>
-      <c r="E44" s="92"/>
-      <c r="F44" s="92"/>
-      <c r="G44" s="92"/>
-      <c r="H44" s="90"/>
-      <c r="I44" s="90"/>
-      <c r="J44" s="90"/>
+      <c r="B44" s="113"/>
+      <c r="C44" s="113"/>
+      <c r="D44" s="113"/>
+      <c r="E44" s="113"/>
+      <c r="F44" s="113"/>
+      <c r="G44" s="113"/>
+      <c r="H44" s="88"/>
+      <c r="I44" s="88"/>
+      <c r="J44" s="88"/>
       <c r="K44" s="34"/>
       <c r="L44" s="34"/>
       <c r="M44" s="34"/>
@@ -3429,16 +3449,16 @@
       <c r="B45" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="93" t="s">
+      <c r="C45" s="114" t="s">
         <v>73</v>
       </c>
-      <c r="D45" s="93"/>
-      <c r="E45" s="93"/>
-      <c r="F45" s="93"/>
-      <c r="G45" s="93"/>
-      <c r="H45" s="90"/>
-      <c r="I45" s="90"/>
-      <c r="J45" s="90"/>
+      <c r="D45" s="114"/>
+      <c r="E45" s="114"/>
+      <c r="F45" s="114"/>
+      <c r="G45" s="114"/>
+      <c r="H45" s="88"/>
+      <c r="I45" s="88"/>
+      <c r="J45" s="88"/>
       <c r="K45" s="34"/>
       <c r="L45" s="34"/>
       <c r="M45" s="34"/>
@@ -3448,16 +3468,16 @@
         <v>74</v>
       </c>
       <c r="B46" s="40"/>
-      <c r="C46" s="94" t="s">
+      <c r="C46" s="115" t="s">
         <v>75</v>
       </c>
-      <c r="D46" s="94"/>
-      <c r="E46" s="94"/>
-      <c r="F46" s="94"/>
-      <c r="G46" s="94"/>
-      <c r="H46" s="90"/>
-      <c r="I46" s="90"/>
-      <c r="J46" s="90"/>
+      <c r="D46" s="115"/>
+      <c r="E46" s="115"/>
+      <c r="F46" s="115"/>
+      <c r="G46" s="115"/>
+      <c r="H46" s="88"/>
+      <c r="I46" s="88"/>
+      <c r="J46" s="88"/>
       <c r="K46" s="34"/>
       <c r="L46" s="34"/>
       <c r="M46" s="34"/>
@@ -3467,41 +3487,41 @@
         <v>76</v>
       </c>
       <c r="B47" s="40"/>
-      <c r="C47" s="94" t="s">
+      <c r="C47" s="115" t="s">
         <v>77</v>
       </c>
-      <c r="D47" s="94"/>
-      <c r="E47" s="94"/>
-      <c r="F47" s="94"/>
-      <c r="G47" s="94"/>
-      <c r="H47" s="90"/>
-      <c r="I47" s="90"/>
-      <c r="J47" s="90"/>
+      <c r="D47" s="115"/>
+      <c r="E47" s="115"/>
+      <c r="F47" s="115"/>
+      <c r="G47" s="115"/>
+      <c r="H47" s="88"/>
+      <c r="I47" s="88"/>
+      <c r="J47" s="88"/>
       <c r="K47" s="34"/>
       <c r="L47" s="34"/>
       <c r="M47" s="34"/>
     </row>
     <row r="48" spans="1:13" ht="12.75" customHeight="1">
-      <c r="H48" s="90"/>
-      <c r="I48" s="90"/>
-      <c r="J48" s="90"/>
+      <c r="H48" s="88"/>
+      <c r="I48" s="88"/>
+      <c r="J48" s="88"/>
       <c r="K48" s="34"/>
       <c r="L48" s="34"/>
       <c r="M48" s="34"/>
     </row>
     <row r="49" spans="1:14" ht="24.75" customHeight="1">
-      <c r="A49" s="95" t="s">
+      <c r="A49" s="116" t="s">
         <v>78</v>
       </c>
-      <c r="B49" s="95"/>
-      <c r="C49" s="95"/>
-      <c r="D49" s="95"/>
-      <c r="E49" s="95"/>
-      <c r="F49" s="95"/>
-      <c r="G49" s="95"/>
-      <c r="H49" s="90"/>
-      <c r="I49" s="90"/>
-      <c r="J49" s="90"/>
+      <c r="B49" s="116"/>
+      <c r="C49" s="116"/>
+      <c r="D49" s="116"/>
+      <c r="E49" s="116"/>
+      <c r="F49" s="116"/>
+      <c r="G49" s="116"/>
+      <c r="H49" s="88"/>
+      <c r="I49" s="88"/>
+      <c r="J49" s="88"/>
       <c r="K49" s="34"/>
       <c r="L49" s="34"/>
       <c r="M49" s="34"/>
@@ -3513,16 +3533,16 @@
       <c r="B50" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="C50" s="96" t="s">
+      <c r="C50" s="117" t="s">
         <v>80</v>
       </c>
-      <c r="D50" s="96"/>
-      <c r="E50" s="96"/>
-      <c r="F50" s="96"/>
-      <c r="G50" s="96"/>
-      <c r="H50" s="90"/>
-      <c r="I50" s="90"/>
-      <c r="J50" s="90"/>
+      <c r="D50" s="117"/>
+      <c r="E50" s="117"/>
+      <c r="F50" s="117"/>
+      <c r="G50" s="117"/>
+      <c r="H50" s="88"/>
+      <c r="I50" s="88"/>
+      <c r="J50" s="88"/>
       <c r="K50" s="34"/>
       <c r="L50" s="34"/>
       <c r="M50" s="34"/>
@@ -3535,25 +3555,25 @@
       <c r="B51" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C51" s="93" t="s">
+      <c r="C51" s="114" t="s">
         <v>82</v>
       </c>
-      <c r="D51" s="93"/>
-      <c r="E51" s="93"/>
-      <c r="F51" s="93"/>
-      <c r="G51" s="93"/>
-      <c r="H51" s="90"/>
-      <c r="I51" s="90"/>
-      <c r="J51" s="90"/>
+      <c r="D51" s="114"/>
+      <c r="E51" s="114"/>
+      <c r="F51" s="114"/>
+      <c r="G51" s="114"/>
+      <c r="H51" s="88"/>
+      <c r="I51" s="88"/>
+      <c r="J51" s="88"/>
       <c r="K51" s="34"/>
       <c r="L51" s="34"/>
       <c r="M51" s="34"/>
       <c r="N51" s="20"/>
     </row>
     <row r="52" spans="1:14" ht="12.75" customHeight="1">
-      <c r="H52" s="90"/>
-      <c r="I52" s="90"/>
-      <c r="J52" s="90"/>
+      <c r="H52" s="88"/>
+      <c r="I52" s="88"/>
+      <c r="J52" s="88"/>
       <c r="K52" s="34"/>
       <c r="L52" s="34"/>
       <c r="M52" s="34"/>
@@ -3563,19 +3583,19 @@
       <c r="A53" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="B53" s="86" t="s">
+      <c r="B53" s="108" t="s">
         <v>84</v>
       </c>
-      <c r="C53" s="86"/>
-      <c r="D53" s="86"/>
-      <c r="E53" s="86"/>
-      <c r="F53" s="87" t="s">
+      <c r="C53" s="108"/>
+      <c r="D53" s="108"/>
+      <c r="E53" s="108"/>
+      <c r="F53" s="109" t="s">
         <v>85</v>
       </c>
-      <c r="G53" s="87"/>
-      <c r="H53" s="87"/>
-      <c r="I53" s="87"/>
-      <c r="J53" s="87"/>
+      <c r="G53" s="109"/>
+      <c r="H53" s="109"/>
+      <c r="I53" s="109"/>
+      <c r="J53" s="109"/>
       <c r="K53" s="44"/>
       <c r="L53" s="44"/>
       <c r="M53" s="44"/>
@@ -3587,28 +3607,28 @@
       <c r="C54" s="20"/>
       <c r="D54" s="20"/>
       <c r="E54" s="20"/>
-      <c r="F54" s="87"/>
-      <c r="G54" s="87"/>
-      <c r="H54" s="87"/>
-      <c r="I54" s="87"/>
-      <c r="J54" s="87"/>
+      <c r="F54" s="109"/>
+      <c r="G54" s="109"/>
+      <c r="H54" s="109"/>
+      <c r="I54" s="109"/>
+      <c r="J54" s="109"/>
       <c r="K54" s="44"/>
       <c r="L54" s="44"/>
       <c r="M54" s="44"/>
     </row>
     <row r="55" spans="1:14">
-      <c r="F55" s="87"/>
-      <c r="G55" s="87"/>
-      <c r="H55" s="87"/>
-      <c r="I55" s="87"/>
-      <c r="J55" s="87"/>
+      <c r="F55" s="109"/>
+      <c r="G55" s="109"/>
+      <c r="H55" s="109"/>
+      <c r="I55" s="109"/>
+      <c r="J55" s="109"/>
     </row>
     <row r="56" spans="1:14">
-      <c r="F56" s="87"/>
-      <c r="G56" s="87"/>
-      <c r="H56" s="87"/>
-      <c r="I56" s="87"/>
-      <c r="J56" s="87"/>
+      <c r="F56" s="109"/>
+      <c r="G56" s="109"/>
+      <c r="H56" s="109"/>
+      <c r="I56" s="109"/>
+      <c r="J56" s="109"/>
       <c r="N56" s="20"/>
     </row>
     <row r="57" spans="1:14">
@@ -3726,14 +3746,14 @@
     <row r="64" spans="1:14" ht="12.75" customHeight="1">
       <c r="A64" s="20"/>
       <c r="B64" s="20"/>
-      <c r="C64" s="88"/>
-      <c r="D64" s="88"/>
-      <c r="E64" s="88"/>
-      <c r="F64" s="88"/>
-      <c r="G64" s="88"/>
-      <c r="H64" s="88"/>
-      <c r="I64" s="88"/>
-      <c r="J64" s="88"/>
+      <c r="C64" s="110"/>
+      <c r="D64" s="110"/>
+      <c r="E64" s="110"/>
+      <c r="F64" s="110"/>
+      <c r="G64" s="110"/>
+      <c r="H64" s="110"/>
+      <c r="I64" s="110"/>
+      <c r="J64" s="110"/>
       <c r="K64" s="20"/>
       <c r="L64" s="20"/>
       <c r="M64" s="20"/>
@@ -3795,14 +3815,14 @@
       <c r="N68" s="20"/>
     </row>
     <row r="69" spans="1:14">
-      <c r="C69" s="88"/>
-      <c r="D69" s="88"/>
-      <c r="E69" s="88"/>
-      <c r="F69" s="88"/>
-      <c r="G69" s="88"/>
-      <c r="H69" s="88"/>
-      <c r="I69" s="88"/>
-      <c r="J69" s="88"/>
+      <c r="C69" s="110"/>
+      <c r="D69" s="110"/>
+      <c r="E69" s="110"/>
+      <c r="F69" s="110"/>
+      <c r="G69" s="110"/>
+      <c r="H69" s="110"/>
+      <c r="I69" s="110"/>
+      <c r="J69" s="110"/>
       <c r="K69" s="20"/>
       <c r="L69" s="20"/>
       <c r="M69" s="20"/>
@@ -5350,37 +5370,6 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="H27:H33"/>
-    <mergeCell ref="I27:I33"/>
-    <mergeCell ref="J27:J33"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="A34:J34"/>
-    <mergeCell ref="A35:J35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:J37"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="E38:J38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H39:J39"/>
     <mergeCell ref="B53:E53"/>
     <mergeCell ref="F53:J56"/>
     <mergeCell ref="C64:J64"/>
@@ -5395,6 +5384,37 @@
     <mergeCell ref="A49:G49"/>
     <mergeCell ref="C50:G50"/>
     <mergeCell ref="C51:G51"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="A34:J34"/>
+    <mergeCell ref="A35:J35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:J37"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="H27:H33"/>
+    <mergeCell ref="I27:I33"/>
+    <mergeCell ref="J27:J33"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="E12:E15"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B40 B45" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -7011,13 +7031,13 @@
       <c r="I43" s="15"/>
       <c r="J43" s="62"/>
       <c r="K43" s="62"/>
-      <c r="L43" s="117" t="s">
+      <c r="L43" s="118" t="s">
         <v>210</v>
       </c>
-      <c r="M43" s="117"/>
-      <c r="N43" s="117"/>
-      <c r="O43" s="117"/>
-      <c r="P43" s="117"/>
+      <c r="M43" s="118"/>
+      <c r="N43" s="118"/>
+      <c r="O43" s="118"/>
+      <c r="P43" s="118"/>
       <c r="Q43" s="66"/>
       <c r="R43" s="66"/>
       <c r="S43" s="66"/>
@@ -7049,13 +7069,13 @@
       <c r="I44" s="15"/>
       <c r="J44" s="62"/>
       <c r="K44" s="62"/>
-      <c r="L44" s="118" t="s">
+      <c r="L44" s="119" t="s">
         <v>212</v>
       </c>
-      <c r="M44" s="118"/>
-      <c r="N44" s="118"/>
-      <c r="O44" s="118"/>
-      <c r="P44" s="118"/>
+      <c r="M44" s="119"/>
+      <c r="N44" s="119"/>
+      <c r="O44" s="119"/>
+      <c r="P44" s="119"/>
       <c r="Q44" s="66"/>
       <c r="R44" s="66"/>
       <c r="S44" s="66"/>
@@ -7087,11 +7107,11 @@
       <c r="I45" s="15"/>
       <c r="J45" s="62"/>
       <c r="K45" s="62"/>
-      <c r="L45" s="118"/>
-      <c r="M45" s="118"/>
-      <c r="N45" s="118"/>
-      <c r="O45" s="118"/>
-      <c r="P45" s="118"/>
+      <c r="L45" s="119"/>
+      <c r="M45" s="119"/>
+      <c r="N45" s="119"/>
+      <c r="O45" s="119"/>
+      <c r="P45" s="119"/>
       <c r="Q45" s="66"/>
       <c r="R45" s="66"/>
       <c r="S45" s="66"/>
@@ -7123,11 +7143,11 @@
       <c r="I46" s="15"/>
       <c r="J46" s="62"/>
       <c r="K46" s="62"/>
-      <c r="L46" s="118"/>
-      <c r="M46" s="118"/>
-      <c r="N46" s="118"/>
-      <c r="O46" s="118"/>
-      <c r="P46" s="118"/>
+      <c r="L46" s="119"/>
+      <c r="M46" s="119"/>
+      <c r="N46" s="119"/>
+      <c r="O46" s="119"/>
+      <c r="P46" s="119"/>
       <c r="Q46" s="66"/>
       <c r="R46" s="66"/>
       <c r="S46" s="66"/>
@@ -7159,11 +7179,11 @@
       <c r="I47" s="15"/>
       <c r="J47" s="62"/>
       <c r="K47" s="62"/>
-      <c r="L47" s="118"/>
-      <c r="M47" s="118"/>
-      <c r="N47" s="118"/>
-      <c r="O47" s="118"/>
-      <c r="P47" s="118"/>
+      <c r="L47" s="119"/>
+      <c r="M47" s="119"/>
+      <c r="N47" s="119"/>
+      <c r="O47" s="119"/>
+      <c r="P47" s="119"/>
       <c r="Q47" s="66"/>
       <c r="R47" s="66"/>
       <c r="S47" s="66"/>
@@ -7189,11 +7209,11 @@
       <c r="I48" s="15"/>
       <c r="J48" s="62"/>
       <c r="K48" s="62"/>
-      <c r="L48" s="118"/>
-      <c r="M48" s="118"/>
-      <c r="N48" s="118"/>
-      <c r="O48" s="118"/>
-      <c r="P48" s="118"/>
+      <c r="L48" s="119"/>
+      <c r="M48" s="119"/>
+      <c r="N48" s="119"/>
+      <c r="O48" s="119"/>
+      <c r="P48" s="119"/>
       <c r="Q48" s="66"/>
       <c r="R48" s="66"/>
       <c r="S48" s="66"/>
@@ -7231,11 +7251,11 @@
       <c r="I49" s="15"/>
       <c r="J49" s="62"/>
       <c r="K49" s="62"/>
-      <c r="L49" s="118"/>
-      <c r="M49" s="118"/>
-      <c r="N49" s="118"/>
-      <c r="O49" s="118"/>
-      <c r="P49" s="118"/>
+      <c r="L49" s="119"/>
+      <c r="M49" s="119"/>
+      <c r="N49" s="119"/>
+      <c r="O49" s="119"/>
+      <c r="P49" s="119"/>
       <c r="Q49" s="66"/>
       <c r="R49" s="66"/>
       <c r="S49" s="66"/>
@@ -7265,11 +7285,11 @@
       <c r="I50" s="15"/>
       <c r="J50" s="62"/>
       <c r="K50" s="62"/>
-      <c r="L50" s="118"/>
-      <c r="M50" s="118"/>
-      <c r="N50" s="118"/>
-      <c r="O50" s="118"/>
-      <c r="P50" s="118"/>
+      <c r="L50" s="119"/>
+      <c r="M50" s="119"/>
+      <c r="N50" s="119"/>
+      <c r="O50" s="119"/>
+      <c r="P50" s="119"/>
       <c r="Q50" s="66"/>
       <c r="R50" s="66"/>
       <c r="S50" s="66"/>
@@ -7299,11 +7319,11 @@
       <c r="I51" s="15"/>
       <c r="J51" s="62"/>
       <c r="K51" s="62"/>
-      <c r="L51" s="118"/>
-      <c r="M51" s="118"/>
-      <c r="N51" s="118"/>
-      <c r="O51" s="118"/>
-      <c r="P51" s="118"/>
+      <c r="L51" s="119"/>
+      <c r="M51" s="119"/>
+      <c r="N51" s="119"/>
+      <c r="O51" s="119"/>
+      <c r="P51" s="119"/>
       <c r="Q51" s="66"/>
       <c r="R51" s="66"/>
       <c r="S51" s="66"/>
@@ -7343,11 +7363,11 @@
       </c>
       <c r="J52" s="62"/>
       <c r="K52" s="62"/>
-      <c r="L52" s="118"/>
-      <c r="M52" s="118"/>
-      <c r="N52" s="118"/>
-      <c r="O52" s="118"/>
-      <c r="P52" s="118"/>
+      <c r="L52" s="119"/>
+      <c r="M52" s="119"/>
+      <c r="N52" s="119"/>
+      <c r="O52" s="119"/>
+      <c r="P52" s="119"/>
       <c r="Q52" s="66"/>
       <c r="R52" s="66"/>
       <c r="S52" s="66"/>
@@ -7387,11 +7407,11 @@
       </c>
       <c r="J53" s="62"/>
       <c r="K53" s="62"/>
-      <c r="L53" s="118"/>
-      <c r="M53" s="118"/>
-      <c r="N53" s="118"/>
-      <c r="O53" s="118"/>
-      <c r="P53" s="118"/>
+      <c r="L53" s="119"/>
+      <c r="M53" s="119"/>
+      <c r="N53" s="119"/>
+      <c r="O53" s="119"/>
+      <c r="P53" s="119"/>
       <c r="Q53" s="66"/>
       <c r="R53" s="66"/>
       <c r="S53" s="66"/>
@@ -7432,11 +7452,11 @@
       </c>
       <c r="J54" s="62"/>
       <c r="K54" s="62"/>
-      <c r="L54" s="118"/>
-      <c r="M54" s="118"/>
-      <c r="N54" s="118"/>
-      <c r="O54" s="118"/>
-      <c r="P54" s="118"/>
+      <c r="L54" s="119"/>
+      <c r="M54" s="119"/>
+      <c r="N54" s="119"/>
+      <c r="O54" s="119"/>
+      <c r="P54" s="119"/>
       <c r="Q54" s="66"/>
       <c r="R54" s="66"/>
       <c r="S54" s="66"/>
@@ -7474,11 +7494,11 @@
       <c r="I55" s="15"/>
       <c r="J55" s="62"/>
       <c r="K55" s="62"/>
-      <c r="L55" s="118"/>
-      <c r="M55" s="118"/>
-      <c r="N55" s="118"/>
-      <c r="O55" s="118"/>
-      <c r="P55" s="118"/>
+      <c r="L55" s="119"/>
+      <c r="M55" s="119"/>
+      <c r="N55" s="119"/>
+      <c r="O55" s="119"/>
+      <c r="P55" s="119"/>
       <c r="Q55" s="66"/>
       <c r="R55" s="66"/>
       <c r="S55" s="66"/>
@@ -7516,11 +7536,11 @@
       <c r="I56" s="15"/>
       <c r="J56" s="62"/>
       <c r="K56" s="62"/>
-      <c r="L56" s="118"/>
-      <c r="M56" s="118"/>
-      <c r="N56" s="118"/>
-      <c r="O56" s="118"/>
-      <c r="P56" s="118"/>
+      <c r="L56" s="119"/>
+      <c r="M56" s="119"/>
+      <c r="N56" s="119"/>
+      <c r="O56" s="119"/>
+      <c r="P56" s="119"/>
       <c r="Q56" s="66"/>
       <c r="R56" s="66"/>
       <c r="S56" s="66"/>
@@ -7556,11 +7576,11 @@
       <c r="I57" s="15"/>
       <c r="J57" s="62"/>
       <c r="K57" s="62"/>
-      <c r="L57" s="118"/>
-      <c r="M57" s="118"/>
-      <c r="N57" s="118"/>
-      <c r="O57" s="118"/>
-      <c r="P57" s="118"/>
+      <c r="L57" s="119"/>
+      <c r="M57" s="119"/>
+      <c r="N57" s="119"/>
+      <c r="O57" s="119"/>
+      <c r="P57" s="119"/>
       <c r="Q57" s="66"/>
       <c r="R57" s="66"/>
       <c r="S57" s="66"/>
@@ -7598,11 +7618,11 @@
       <c r="I58" s="15"/>
       <c r="J58" s="62"/>
       <c r="K58" s="62"/>
-      <c r="L58" s="118"/>
-      <c r="M58" s="118"/>
-      <c r="N58" s="118"/>
-      <c r="O58" s="118"/>
-      <c r="P58" s="118"/>
+      <c r="L58" s="119"/>
+      <c r="M58" s="119"/>
+      <c r="N58" s="119"/>
+      <c r="O58" s="119"/>
+      <c r="P58" s="119"/>
       <c r="Q58" s="66"/>
       <c r="R58" s="66"/>
       <c r="S58" s="66"/>
@@ -7638,11 +7658,11 @@
       <c r="I59" s="15"/>
       <c r="J59" s="62"/>
       <c r="K59" s="62"/>
-      <c r="L59" s="118"/>
-      <c r="M59" s="118"/>
-      <c r="N59" s="118"/>
-      <c r="O59" s="118"/>
-      <c r="P59" s="118"/>
+      <c r="L59" s="119"/>
+      <c r="M59" s="119"/>
+      <c r="N59" s="119"/>
+      <c r="O59" s="119"/>
+      <c r="P59" s="119"/>
       <c r="Q59" s="66"/>
       <c r="R59" s="66"/>
       <c r="S59" s="66"/>
@@ -7680,11 +7700,11 @@
       <c r="I60" s="15"/>
       <c r="J60" s="62"/>
       <c r="K60" s="62"/>
-      <c r="L60" s="118"/>
-      <c r="M60" s="118"/>
-      <c r="N60" s="118"/>
-      <c r="O60" s="118"/>
-      <c r="P60" s="118"/>
+      <c r="L60" s="119"/>
+      <c r="M60" s="119"/>
+      <c r="N60" s="119"/>
+      <c r="O60" s="119"/>
+      <c r="P60" s="119"/>
       <c r="Q60" s="66"/>
       <c r="R60" s="66"/>
       <c r="S60" s="66"/>
@@ -7722,11 +7742,11 @@
       <c r="I61" s="15"/>
       <c r="J61" s="62"/>
       <c r="K61" s="62"/>
-      <c r="L61" s="118"/>
-      <c r="M61" s="118"/>
-      <c r="N61" s="118"/>
-      <c r="O61" s="118"/>
-      <c r="P61" s="118"/>
+      <c r="L61" s="119"/>
+      <c r="M61" s="119"/>
+      <c r="N61" s="119"/>
+      <c r="O61" s="119"/>
+      <c r="P61" s="119"/>
       <c r="Q61" s="66"/>
       <c r="R61" s="66"/>
       <c r="S61" s="66"/>
@@ -7764,11 +7784,11 @@
       <c r="I62" s="15"/>
       <c r="J62" s="62"/>
       <c r="K62" s="62"/>
-      <c r="L62" s="118"/>
-      <c r="M62" s="118"/>
-      <c r="N62" s="118"/>
-      <c r="O62" s="118"/>
-      <c r="P62" s="118"/>
+      <c r="L62" s="119"/>
+      <c r="M62" s="119"/>
+      <c r="N62" s="119"/>
+      <c r="O62" s="119"/>
+      <c r="P62" s="119"/>
       <c r="Q62" s="66"/>
       <c r="R62" s="66"/>
       <c r="S62" s="66"/>
@@ -7806,11 +7826,11 @@
       <c r="I63" s="15"/>
       <c r="J63" s="62"/>
       <c r="K63" s="62"/>
-      <c r="L63" s="118"/>
-      <c r="M63" s="118"/>
-      <c r="N63" s="118"/>
-      <c r="O63" s="118"/>
-      <c r="P63" s="118"/>
+      <c r="L63" s="119"/>
+      <c r="M63" s="119"/>
+      <c r="N63" s="119"/>
+      <c r="O63" s="119"/>
+      <c r="P63" s="119"/>
       <c r="Q63" s="66"/>
       <c r="R63" s="66"/>
       <c r="S63" s="66"/>
@@ -7846,11 +7866,11 @@
         <v>227</v>
       </c>
       <c r="I64" s="60"/>
-      <c r="L64" s="118"/>
-      <c r="M64" s="118"/>
-      <c r="N64" s="118"/>
-      <c r="O64" s="118"/>
-      <c r="P64" s="118"/>
+      <c r="L64" s="119"/>
+      <c r="M64" s="119"/>
+      <c r="N64" s="119"/>
+      <c r="O64" s="119"/>
+      <c r="P64" s="119"/>
       <c r="Q64" s="66"/>
       <c r="R64" s="66"/>
       <c r="S64" s="66"/>
@@ -7886,11 +7906,11 @@
         <v>230</v>
       </c>
       <c r="I65" s="60"/>
-      <c r="L65" s="118"/>
-      <c r="M65" s="118"/>
-      <c r="N65" s="118"/>
-      <c r="O65" s="118"/>
-      <c r="P65" s="118"/>
+      <c r="L65" s="119"/>
+      <c r="M65" s="119"/>
+      <c r="N65" s="119"/>
+      <c r="O65" s="119"/>
+      <c r="P65" s="119"/>
       <c r="Q65" s="66"/>
       <c r="R65" s="66"/>
       <c r="S65" s="66"/>
@@ -7926,11 +7946,11 @@
         <v>234</v>
       </c>
       <c r="I66" s="60"/>
-      <c r="L66" s="118"/>
-      <c r="M66" s="118"/>
-      <c r="N66" s="118"/>
-      <c r="O66" s="118"/>
-      <c r="P66" s="118"/>
+      <c r="L66" s="119"/>
+      <c r="M66" s="119"/>
+      <c r="N66" s="119"/>
+      <c r="O66" s="119"/>
+      <c r="P66" s="119"/>
       <c r="Q66" s="66"/>
       <c r="R66" s="66"/>
       <c r="S66" s="66"/>
@@ -7958,11 +7978,11 @@
       </c>
       <c r="H67" s="60"/>
       <c r="I67" s="60"/>
-      <c r="L67" s="118"/>
-      <c r="M67" s="118"/>
-      <c r="N67" s="118"/>
-      <c r="O67" s="118"/>
-      <c r="P67" s="118"/>
+      <c r="L67" s="119"/>
+      <c r="M67" s="119"/>
+      <c r="N67" s="119"/>
+      <c r="O67" s="119"/>
+      <c r="P67" s="119"/>
       <c r="Q67" s="66"/>
       <c r="R67" s="66"/>
       <c r="S67" s="66"/>
@@ -7990,11 +8010,11 @@
       </c>
       <c r="H68" s="60"/>
       <c r="I68" s="60"/>
-      <c r="L68" s="118"/>
-      <c r="M68" s="118"/>
-      <c r="N68" s="118"/>
-      <c r="O68" s="118"/>
-      <c r="P68" s="118"/>
+      <c r="L68" s="119"/>
+      <c r="M68" s="119"/>
+      <c r="N68" s="119"/>
+      <c r="O68" s="119"/>
+      <c r="P68" s="119"/>
       <c r="Q68" s="66"/>
       <c r="R68" s="66"/>
       <c r="S68" s="66"/>
@@ -8020,11 +8040,11 @@
       <c r="G69" s="60"/>
       <c r="H69" s="60"/>
       <c r="I69" s="60"/>
-      <c r="L69" s="118"/>
-      <c r="M69" s="118"/>
-      <c r="N69" s="118"/>
-      <c r="O69" s="118"/>
-      <c r="P69" s="118"/>
+      <c r="L69" s="119"/>
+      <c r="M69" s="119"/>
+      <c r="N69" s="119"/>
+      <c r="O69" s="119"/>
+      <c r="P69" s="119"/>
       <c r="Q69" s="66"/>
       <c r="R69" s="66"/>
       <c r="S69" s="66"/>
@@ -8060,11 +8080,11 @@
         <v>15</v>
       </c>
       <c r="I70" s="60"/>
-      <c r="L70" s="118"/>
-      <c r="M70" s="118"/>
-      <c r="N70" s="118"/>
-      <c r="O70" s="118"/>
-      <c r="P70" s="118"/>
+      <c r="L70" s="119"/>
+      <c r="M70" s="119"/>
+      <c r="N70" s="119"/>
+      <c r="O70" s="119"/>
+      <c r="P70" s="119"/>
       <c r="Q70" s="66"/>
       <c r="R70" s="66"/>
       <c r="S70" s="66"/>
@@ -8100,11 +8120,11 @@
         <v>15</v>
       </c>
       <c r="I71" s="60"/>
-      <c r="L71" s="118"/>
-      <c r="M71" s="118"/>
-      <c r="N71" s="118"/>
-      <c r="O71" s="118"/>
-      <c r="P71" s="118"/>
+      <c r="L71" s="119"/>
+      <c r="M71" s="119"/>
+      <c r="N71" s="119"/>
+      <c r="O71" s="119"/>
+      <c r="P71" s="119"/>
       <c r="Q71" s="66"/>
       <c r="R71" s="66"/>
       <c r="S71" s="66"/>
@@ -8128,11 +8148,11 @@
       <c r="G72" s="60"/>
       <c r="H72" s="60"/>
       <c r="I72" s="60"/>
-      <c r="L72" s="118"/>
-      <c r="M72" s="118"/>
-      <c r="N72" s="118"/>
-      <c r="O72" s="118"/>
-      <c r="P72" s="118"/>
+      <c r="L72" s="119"/>
+      <c r="M72" s="119"/>
+      <c r="N72" s="119"/>
+      <c r="O72" s="119"/>
+      <c r="P72" s="119"/>
       <c r="Q72" s="66"/>
       <c r="R72" s="66"/>
       <c r="S72" s="66"/>
@@ -8168,11 +8188,11 @@
         <v>244</v>
       </c>
       <c r="I73" s="60"/>
-      <c r="L73" s="118"/>
-      <c r="M73" s="118"/>
-      <c r="N73" s="118"/>
-      <c r="O73" s="118"/>
-      <c r="P73" s="118"/>
+      <c r="L73" s="119"/>
+      <c r="M73" s="119"/>
+      <c r="N73" s="119"/>
+      <c r="O73" s="119"/>
+      <c r="P73" s="119"/>
       <c r="Q73" s="66"/>
       <c r="R73" s="66"/>
       <c r="S73" s="66"/>
@@ -8200,11 +8220,11 @@
         <v>247</v>
       </c>
       <c r="I74" s="60"/>
-      <c r="L74" s="118"/>
-      <c r="M74" s="118"/>
-      <c r="N74" s="118"/>
-      <c r="O74" s="118"/>
-      <c r="P74" s="118"/>
+      <c r="L74" s="119"/>
+      <c r="M74" s="119"/>
+      <c r="N74" s="119"/>
+      <c r="O74" s="119"/>
+      <c r="P74" s="119"/>
       <c r="Q74" s="66"/>
       <c r="R74" s="66"/>
       <c r="S74" s="66"/>
@@ -8238,11 +8258,11 @@
       </c>
       <c r="H75" s="57"/>
       <c r="I75" s="57"/>
-      <c r="L75" s="118"/>
-      <c r="M75" s="118"/>
-      <c r="N75" s="118"/>
-      <c r="O75" s="118"/>
-      <c r="P75" s="118"/>
+      <c r="L75" s="119"/>
+      <c r="M75" s="119"/>
+      <c r="N75" s="119"/>
+      <c r="O75" s="119"/>
+      <c r="P75" s="119"/>
       <c r="Q75" s="66"/>
       <c r="R75" s="66"/>
       <c r="S75" s="66"/>
@@ -8276,11 +8296,11 @@
       </c>
       <c r="H76" s="57"/>
       <c r="I76" s="57"/>
-      <c r="L76" s="118"/>
-      <c r="M76" s="118"/>
-      <c r="N76" s="118"/>
-      <c r="O76" s="118"/>
-      <c r="P76" s="118"/>
+      <c r="L76" s="119"/>
+      <c r="M76" s="119"/>
+      <c r="N76" s="119"/>
+      <c r="O76" s="119"/>
+      <c r="P76" s="119"/>
       <c r="Q76" s="66"/>
       <c r="R76" s="66"/>
       <c r="S76" s="66"/>
@@ -8316,11 +8336,11 @@
         <v>254</v>
       </c>
       <c r="I77" s="57"/>
-      <c r="L77" s="118"/>
-      <c r="M77" s="118"/>
-      <c r="N77" s="118"/>
-      <c r="O77" s="118"/>
-      <c r="P77" s="118"/>
+      <c r="L77" s="119"/>
+      <c r="M77" s="119"/>
+      <c r="N77" s="119"/>
+      <c r="O77" s="119"/>
+      <c r="P77" s="119"/>
       <c r="Q77" s="66"/>
       <c r="R77" s="66"/>
       <c r="S77" s="66"/>
@@ -8355,11 +8375,11 @@
       <c r="H78" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="L78" s="118"/>
-      <c r="M78" s="118"/>
-      <c r="N78" s="118"/>
-      <c r="O78" s="118"/>
-      <c r="P78" s="118"/>
+      <c r="L78" s="119"/>
+      <c r="M78" s="119"/>
+      <c r="N78" s="119"/>
+      <c r="O78" s="119"/>
+      <c r="P78" s="119"/>
       <c r="Q78" s="66"/>
       <c r="R78" s="66"/>
       <c r="S78" s="66"/>
@@ -8394,11 +8414,11 @@
       <c r="H79" s="62" t="s">
         <v>257</v>
       </c>
-      <c r="L79" s="118"/>
-      <c r="M79" s="118"/>
-      <c r="N79" s="118"/>
-      <c r="O79" s="118"/>
-      <c r="P79" s="118"/>
+      <c r="L79" s="119"/>
+      <c r="M79" s="119"/>
+      <c r="N79" s="119"/>
+      <c r="O79" s="119"/>
+      <c r="P79" s="119"/>
       <c r="Q79" s="66"/>
       <c r="R79" s="66"/>
       <c r="S79" s="66"/>
@@ -8433,11 +8453,11 @@
       <c r="H80" s="62" t="s">
         <v>257</v>
       </c>
-      <c r="L80" s="118"/>
-      <c r="M80" s="118"/>
-      <c r="N80" s="118"/>
-      <c r="O80" s="118"/>
-      <c r="P80" s="118"/>
+      <c r="L80" s="119"/>
+      <c r="M80" s="119"/>
+      <c r="N80" s="119"/>
+      <c r="O80" s="119"/>
+      <c r="P80" s="119"/>
       <c r="Q80" s="66"/>
       <c r="R80" s="66"/>
       <c r="S80" s="66"/>
@@ -8472,11 +8492,11 @@
       <c r="H81" s="62" t="s">
         <v>262</v>
       </c>
-      <c r="L81" s="118"/>
-      <c r="M81" s="118"/>
-      <c r="N81" s="118"/>
-      <c r="O81" s="118"/>
-      <c r="P81" s="118"/>
+      <c r="L81" s="119"/>
+      <c r="M81" s="119"/>
+      <c r="N81" s="119"/>
+      <c r="O81" s="119"/>
+      <c r="P81" s="119"/>
       <c r="Q81" s="66"/>
       <c r="R81" s="66"/>
       <c r="S81" s="66"/>
@@ -8505,11 +8525,11 @@
       <c r="H82" s="62" t="s">
         <v>262</v>
       </c>
-      <c r="L82" s="118"/>
-      <c r="M82" s="118"/>
-      <c r="N82" s="118"/>
-      <c r="O82" s="118"/>
-      <c r="P82" s="118"/>
+      <c r="L82" s="119"/>
+      <c r="M82" s="119"/>
+      <c r="N82" s="119"/>
+      <c r="O82" s="119"/>
+      <c r="P82" s="119"/>
       <c r="Q82" s="66"/>
       <c r="R82" s="66"/>
       <c r="S82" s="66"/>
@@ -8544,11 +8564,11 @@
       <c r="H83" t="s">
         <v>267</v>
       </c>
-      <c r="L83" s="118"/>
-      <c r="M83" s="118"/>
-      <c r="N83" s="118"/>
-      <c r="O83" s="118"/>
-      <c r="P83" s="118"/>
+      <c r="L83" s="119"/>
+      <c r="M83" s="119"/>
+      <c r="N83" s="119"/>
+      <c r="O83" s="119"/>
+      <c r="P83" s="119"/>
       <c r="Q83" s="66"/>
       <c r="R83" s="66"/>
       <c r="S83" s="66"/>
@@ -8583,11 +8603,11 @@
       <c r="H84" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="L84" s="118"/>
-      <c r="M84" s="118"/>
-      <c r="N84" s="118"/>
-      <c r="O84" s="118"/>
-      <c r="P84" s="118"/>
+      <c r="L84" s="119"/>
+      <c r="M84" s="119"/>
+      <c r="N84" s="119"/>
+      <c r="O84" s="119"/>
+      <c r="P84" s="119"/>
       <c r="Q84" s="66"/>
       <c r="R84" s="66"/>
       <c r="S84" s="66"/>
@@ -8625,14 +8645,14 @@
       <c r="I85" s="22"/>
       <c r="J85" s="22"/>
       <c r="K85" s="77"/>
-      <c r="L85" s="118"/>
-      <c r="M85" s="118"/>
-      <c r="N85" s="118"/>
-      <c r="O85" s="118">
+      <c r="L85" s="119"/>
+      <c r="M85" s="119"/>
+      <c r="N85" s="119"/>
+      <c r="O85" s="119">
         <f>10^3</f>
         <v>1000</v>
       </c>
-      <c r="P85" s="118"/>
+      <c r="P85" s="119"/>
       <c r="Q85" s="66"/>
       <c r="R85" s="66"/>
       <c r="S85" s="66"/>
@@ -8646,11 +8666,11 @@
       <c r="AA85" s="66"/>
     </row>
     <row r="86" spans="2:27" ht="12.75" customHeight="1">
-      <c r="L86" s="118"/>
-      <c r="M86" s="118"/>
-      <c r="N86" s="118"/>
-      <c r="O86" s="118"/>
-      <c r="P86" s="118"/>
+      <c r="L86" s="119"/>
+      <c r="M86" s="119"/>
+      <c r="N86" s="119"/>
+      <c r="O86" s="119"/>
+      <c r="P86" s="119"/>
       <c r="Q86" s="66"/>
       <c r="R86" s="66"/>
       <c r="S86" s="66"/>
@@ -8664,11 +8684,11 @@
       <c r="AA86" s="66"/>
     </row>
     <row r="87" spans="2:27" ht="12.75" customHeight="1">
-      <c r="L87" s="118"/>
-      <c r="M87" s="118"/>
-      <c r="N87" s="118"/>
-      <c r="O87" s="118"/>
-      <c r="P87" s="118"/>
+      <c r="L87" s="119"/>
+      <c r="M87" s="119"/>
+      <c r="N87" s="119"/>
+      <c r="O87" s="119"/>
+      <c r="P87" s="119"/>
       <c r="Q87" s="66"/>
       <c r="R87" s="66"/>
       <c r="S87" s="66"/>
@@ -8763,267 +8783,267 @@
       </c>
     </row>
     <row r="3" spans="2:21" ht="12.75" customHeight="1">
-      <c r="B3" s="119" t="s">
+      <c r="B3" s="120" t="s">
         <v>272</v>
       </c>
-      <c r="C3" s="119"/>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="119"/>
-      <c r="I3" s="119"/>
-      <c r="J3" s="119"/>
-      <c r="K3" s="119"/>
-      <c r="L3" s="119"/>
-      <c r="M3" s="119"/>
-      <c r="N3" s="119"/>
-      <c r="O3" s="119"/>
-      <c r="P3" s="119"/>
-      <c r="Q3" s="119"/>
-      <c r="R3" s="119"/>
-      <c r="S3" s="119"/>
-      <c r="T3" s="119"/>
-      <c r="U3" s="119"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
+      <c r="M3" s="120"/>
+      <c r="N3" s="120"/>
+      <c r="O3" s="120"/>
+      <c r="P3" s="120"/>
+      <c r="Q3" s="120"/>
+      <c r="R3" s="120"/>
+      <c r="S3" s="120"/>
+      <c r="T3" s="120"/>
+      <c r="U3" s="120"/>
     </row>
     <row r="4" spans="2:21">
-      <c r="B4" s="119"/>
-      <c r="C4" s="119"/>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="119"/>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
-      <c r="J4" s="119"/>
-      <c r="K4" s="119"/>
-      <c r="L4" s="119"/>
-      <c r="M4" s="119"/>
-      <c r="N4" s="119"/>
-      <c r="O4" s="119"/>
-      <c r="P4" s="119"/>
-      <c r="Q4" s="119"/>
-      <c r="R4" s="119"/>
-      <c r="S4" s="119"/>
-      <c r="T4" s="119"/>
-      <c r="U4" s="119"/>
+      <c r="B4" s="120"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
+      <c r="G4" s="120"/>
+      <c r="H4" s="120"/>
+      <c r="I4" s="120"/>
+      <c r="J4" s="120"/>
+      <c r="K4" s="120"/>
+      <c r="L4" s="120"/>
+      <c r="M4" s="120"/>
+      <c r="N4" s="120"/>
+      <c r="O4" s="120"/>
+      <c r="P4" s="120"/>
+      <c r="Q4" s="120"/>
+      <c r="R4" s="120"/>
+      <c r="S4" s="120"/>
+      <c r="T4" s="120"/>
+      <c r="U4" s="120"/>
     </row>
     <row r="5" spans="2:21">
-      <c r="B5" s="119"/>
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
-      <c r="J5" s="119"/>
-      <c r="K5" s="119"/>
-      <c r="L5" s="119"/>
-      <c r="M5" s="119"/>
-      <c r="N5" s="119"/>
-      <c r="O5" s="119"/>
-      <c r="P5" s="119"/>
-      <c r="Q5" s="119"/>
-      <c r="R5" s="119"/>
-      <c r="S5" s="119"/>
-      <c r="T5" s="119"/>
-      <c r="U5" s="119"/>
+      <c r="B5" s="120"/>
+      <c r="C5" s="120"/>
+      <c r="D5" s="120"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="120"/>
+      <c r="G5" s="120"/>
+      <c r="H5" s="120"/>
+      <c r="I5" s="120"/>
+      <c r="J5" s="120"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="120"/>
+      <c r="M5" s="120"/>
+      <c r="N5" s="120"/>
+      <c r="O5" s="120"/>
+      <c r="P5" s="120"/>
+      <c r="Q5" s="120"/>
+      <c r="R5" s="120"/>
+      <c r="S5" s="120"/>
+      <c r="T5" s="120"/>
+      <c r="U5" s="120"/>
     </row>
     <row r="6" spans="2:21">
-      <c r="B6" s="119"/>
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
-      <c r="E6" s="119"/>
-      <c r="F6" s="119"/>
-      <c r="G6" s="119"/>
-      <c r="H6" s="119"/>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="119"/>
-      <c r="O6" s="119"/>
-      <c r="P6" s="119"/>
-      <c r="Q6" s="119"/>
-      <c r="R6" s="119"/>
-      <c r="S6" s="119"/>
-      <c r="T6" s="119"/>
-      <c r="U6" s="119"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="120"/>
+      <c r="D6" s="120"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="120"/>
+      <c r="G6" s="120"/>
+      <c r="H6" s="120"/>
+      <c r="I6" s="120"/>
+      <c r="J6" s="120"/>
+      <c r="K6" s="120"/>
+      <c r="L6" s="120"/>
+      <c r="M6" s="120"/>
+      <c r="N6" s="120"/>
+      <c r="O6" s="120"/>
+      <c r="P6" s="120"/>
+      <c r="Q6" s="120"/>
+      <c r="R6" s="120"/>
+      <c r="S6" s="120"/>
+      <c r="T6" s="120"/>
+      <c r="U6" s="120"/>
     </row>
     <row r="7" spans="2:21">
-      <c r="B7" s="119"/>
-      <c r="C7" s="119"/>
-      <c r="D7" s="119"/>
-      <c r="E7" s="119"/>
-      <c r="F7" s="119"/>
-      <c r="G7" s="119"/>
-      <c r="H7" s="119"/>
-      <c r="I7" s="119"/>
-      <c r="J7" s="119"/>
-      <c r="K7" s="119"/>
-      <c r="L7" s="119"/>
-      <c r="M7" s="119"/>
-      <c r="N7" s="119"/>
-      <c r="O7" s="119"/>
-      <c r="P7" s="119"/>
-      <c r="Q7" s="119"/>
-      <c r="R7" s="119"/>
-      <c r="S7" s="119"/>
-      <c r="T7" s="119"/>
-      <c r="U7" s="119"/>
+      <c r="B7" s="120"/>
+      <c r="C7" s="120"/>
+      <c r="D7" s="120"/>
+      <c r="E7" s="120"/>
+      <c r="F7" s="120"/>
+      <c r="G7" s="120"/>
+      <c r="H7" s="120"/>
+      <c r="I7" s="120"/>
+      <c r="J7" s="120"/>
+      <c r="K7" s="120"/>
+      <c r="L7" s="120"/>
+      <c r="M7" s="120"/>
+      <c r="N7" s="120"/>
+      <c r="O7" s="120"/>
+      <c r="P7" s="120"/>
+      <c r="Q7" s="120"/>
+      <c r="R7" s="120"/>
+      <c r="S7" s="120"/>
+      <c r="T7" s="120"/>
+      <c r="U7" s="120"/>
     </row>
     <row r="8" spans="2:21">
-      <c r="B8" s="119"/>
-      <c r="C8" s="119"/>
-      <c r="D8" s="119"/>
-      <c r="E8" s="119"/>
-      <c r="F8" s="119"/>
-      <c r="G8" s="119"/>
-      <c r="H8" s="119"/>
-      <c r="I8" s="119"/>
-      <c r="J8" s="119"/>
-      <c r="K8" s="119"/>
-      <c r="L8" s="119"/>
-      <c r="M8" s="119"/>
-      <c r="N8" s="119"/>
-      <c r="O8" s="119"/>
-      <c r="P8" s="119"/>
-      <c r="Q8" s="119"/>
-      <c r="R8" s="119"/>
-      <c r="S8" s="119"/>
-      <c r="T8" s="119"/>
-      <c r="U8" s="119"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="120"/>
+      <c r="D8" s="120"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="120"/>
+      <c r="G8" s="120"/>
+      <c r="H8" s="120"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="120"/>
+      <c r="K8" s="120"/>
+      <c r="L8" s="120"/>
+      <c r="M8" s="120"/>
+      <c r="N8" s="120"/>
+      <c r="O8" s="120"/>
+      <c r="P8" s="120"/>
+      <c r="Q8" s="120"/>
+      <c r="R8" s="120"/>
+      <c r="S8" s="120"/>
+      <c r="T8" s="120"/>
+      <c r="U8" s="120"/>
     </row>
     <row r="9" spans="2:21">
-      <c r="B9" s="119"/>
-      <c r="C9" s="119"/>
-      <c r="D9" s="119"/>
-      <c r="E9" s="119"/>
-      <c r="F9" s="119"/>
-      <c r="G9" s="119"/>
-      <c r="H9" s="119"/>
-      <c r="I9" s="119"/>
-      <c r="J9" s="119"/>
-      <c r="K9" s="119"/>
-      <c r="L9" s="119"/>
-      <c r="M9" s="119"/>
-      <c r="N9" s="119"/>
-      <c r="O9" s="119"/>
-      <c r="P9" s="119"/>
-      <c r="Q9" s="119"/>
-      <c r="R9" s="119"/>
-      <c r="S9" s="119"/>
-      <c r="T9" s="119"/>
-      <c r="U9" s="119"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="120"/>
+      <c r="D9" s="120"/>
+      <c r="E9" s="120"/>
+      <c r="F9" s="120"/>
+      <c r="G9" s="120"/>
+      <c r="H9" s="120"/>
+      <c r="I9" s="120"/>
+      <c r="J9" s="120"/>
+      <c r="K9" s="120"/>
+      <c r="L9" s="120"/>
+      <c r="M9" s="120"/>
+      <c r="N9" s="120"/>
+      <c r="O9" s="120"/>
+      <c r="P9" s="120"/>
+      <c r="Q9" s="120"/>
+      <c r="R9" s="120"/>
+      <c r="S9" s="120"/>
+      <c r="T9" s="120"/>
+      <c r="U9" s="120"/>
     </row>
     <row r="10" spans="2:21">
-      <c r="B10" s="119"/>
-      <c r="C10" s="119"/>
-      <c r="D10" s="119"/>
-      <c r="E10" s="119"/>
-      <c r="F10" s="119"/>
-      <c r="G10" s="119"/>
-      <c r="H10" s="119"/>
-      <c r="I10" s="119"/>
-      <c r="J10" s="119"/>
-      <c r="K10" s="119"/>
-      <c r="L10" s="119"/>
-      <c r="M10" s="119"/>
-      <c r="N10" s="119"/>
-      <c r="O10" s="119"/>
-      <c r="P10" s="119"/>
-      <c r="Q10" s="119"/>
-      <c r="R10" s="119"/>
-      <c r="S10" s="119"/>
-      <c r="T10" s="119"/>
-      <c r="U10" s="119"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="120"/>
+      <c r="D10" s="120"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="120"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="120"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="120"/>
+      <c r="K10" s="120"/>
+      <c r="L10" s="120"/>
+      <c r="M10" s="120"/>
+      <c r="N10" s="120"/>
+      <c r="O10" s="120"/>
+      <c r="P10" s="120"/>
+      <c r="Q10" s="120"/>
+      <c r="R10" s="120"/>
+      <c r="S10" s="120"/>
+      <c r="T10" s="120"/>
+      <c r="U10" s="120"/>
     </row>
     <row r="11" spans="2:21">
-      <c r="B11" s="119"/>
-      <c r="C11" s="119"/>
-      <c r="D11" s="119"/>
-      <c r="E11" s="119"/>
-      <c r="F11" s="119"/>
-      <c r="G11" s="119"/>
-      <c r="H11" s="119"/>
-      <c r="I11" s="119"/>
-      <c r="J11" s="119"/>
-      <c r="K11" s="119"/>
-      <c r="L11" s="119"/>
-      <c r="M11" s="119"/>
-      <c r="N11" s="119"/>
-      <c r="O11" s="119"/>
-      <c r="P11" s="119"/>
-      <c r="Q11" s="119"/>
-      <c r="R11" s="119"/>
-      <c r="S11" s="119"/>
-      <c r="T11" s="119"/>
-      <c r="U11" s="119"/>
+      <c r="B11" s="120"/>
+      <c r="C11" s="120"/>
+      <c r="D11" s="120"/>
+      <c r="E11" s="120"/>
+      <c r="F11" s="120"/>
+      <c r="G11" s="120"/>
+      <c r="H11" s="120"/>
+      <c r="I11" s="120"/>
+      <c r="J11" s="120"/>
+      <c r="K11" s="120"/>
+      <c r="L11" s="120"/>
+      <c r="M11" s="120"/>
+      <c r="N11" s="120"/>
+      <c r="O11" s="120"/>
+      <c r="P11" s="120"/>
+      <c r="Q11" s="120"/>
+      <c r="R11" s="120"/>
+      <c r="S11" s="120"/>
+      <c r="T11" s="120"/>
+      <c r="U11" s="120"/>
     </row>
     <row r="12" spans="2:21">
-      <c r="B12" s="119"/>
-      <c r="C12" s="119"/>
-      <c r="D12" s="119"/>
-      <c r="E12" s="119"/>
-      <c r="F12" s="119"/>
-      <c r="G12" s="119"/>
-      <c r="H12" s="119"/>
-      <c r="I12" s="119"/>
-      <c r="J12" s="119"/>
-      <c r="K12" s="119"/>
-      <c r="L12" s="119"/>
-      <c r="M12" s="119"/>
-      <c r="N12" s="119"/>
-      <c r="O12" s="119"/>
-      <c r="P12" s="119"/>
-      <c r="Q12" s="119"/>
-      <c r="R12" s="119"/>
-      <c r="S12" s="119"/>
-      <c r="T12" s="119"/>
-      <c r="U12" s="119"/>
+      <c r="B12" s="120"/>
+      <c r="C12" s="120"/>
+      <c r="D12" s="120"/>
+      <c r="E12" s="120"/>
+      <c r="F12" s="120"/>
+      <c r="G12" s="120"/>
+      <c r="H12" s="120"/>
+      <c r="I12" s="120"/>
+      <c r="J12" s="120"/>
+      <c r="K12" s="120"/>
+      <c r="L12" s="120"/>
+      <c r="M12" s="120"/>
+      <c r="N12" s="120"/>
+      <c r="O12" s="120"/>
+      <c r="P12" s="120"/>
+      <c r="Q12" s="120"/>
+      <c r="R12" s="120"/>
+      <c r="S12" s="120"/>
+      <c r="T12" s="120"/>
+      <c r="U12" s="120"/>
     </row>
     <row r="15" spans="2:21" ht="12.75" customHeight="1">
       <c r="B15" t="s">
         <v>273</v>
       </c>
-      <c r="F15" s="118" t="s">
+      <c r="F15" s="119" t="s">
         <v>274</v>
       </c>
-      <c r="G15" s="118"/>
-      <c r="H15" s="118"/>
-      <c r="I15" s="118"/>
-      <c r="J15" s="118"/>
-      <c r="K15" s="118"/>
-      <c r="L15" s="118"/>
-      <c r="M15" s="118"/>
-      <c r="N15" s="118"/>
-      <c r="O15" s="118"/>
+      <c r="G15" s="119"/>
+      <c r="H15" s="119"/>
+      <c r="I15" s="119"/>
+      <c r="J15" s="119"/>
+      <c r="K15" s="119"/>
+      <c r="L15" s="119"/>
+      <c r="M15" s="119"/>
+      <c r="N15" s="119"/>
+      <c r="O15" s="119"/>
     </row>
     <row r="16" spans="2:21">
-      <c r="F16" s="118"/>
-      <c r="G16" s="118"/>
-      <c r="H16" s="118"/>
-      <c r="I16" s="118"/>
-      <c r="J16" s="118"/>
-      <c r="K16" s="118"/>
-      <c r="L16" s="118"/>
-      <c r="M16" s="118"/>
-      <c r="N16" s="118"/>
-      <c r="O16" s="118"/>
+      <c r="F16" s="119"/>
+      <c r="G16" s="119"/>
+      <c r="H16" s="119"/>
+      <c r="I16" s="119"/>
+      <c r="J16" s="119"/>
+      <c r="K16" s="119"/>
+      <c r="L16" s="119"/>
+      <c r="M16" s="119"/>
+      <c r="N16" s="119"/>
+      <c r="O16" s="119"/>
     </row>
     <row r="17" spans="2:15">
-      <c r="F17" s="118"/>
-      <c r="G17" s="118"/>
-      <c r="H17" s="118"/>
-      <c r="I17" s="118"/>
-      <c r="J17" s="118"/>
-      <c r="K17" s="118"/>
-      <c r="L17" s="118"/>
-      <c r="M17" s="118"/>
-      <c r="N17" s="118"/>
-      <c r="O17" s="118"/>
+      <c r="F17" s="119"/>
+      <c r="G17" s="119"/>
+      <c r="H17" s="119"/>
+      <c r="I17" s="119"/>
+      <c r="J17" s="119"/>
+      <c r="K17" s="119"/>
+      <c r="L17" s="119"/>
+      <c r="M17" s="119"/>
+      <c r="N17" s="119"/>
+      <c r="O17" s="119"/>
     </row>
     <row r="18" spans="2:15">
       <c r="B18" s="49" t="s">
@@ -9038,16 +9058,16 @@
       <c r="E18" s="49" t="s">
         <v>277</v>
       </c>
-      <c r="F18" s="118"/>
-      <c r="G18" s="118"/>
-      <c r="H18" s="118"/>
-      <c r="I18" s="118"/>
-      <c r="J18" s="118"/>
-      <c r="K18" s="118"/>
-      <c r="L18" s="118"/>
-      <c r="M18" s="118"/>
-      <c r="N18" s="118"/>
-      <c r="O18" s="118"/>
+      <c r="F18" s="119"/>
+      <c r="G18" s="119"/>
+      <c r="H18" s="119"/>
+      <c r="I18" s="119"/>
+      <c r="J18" s="119"/>
+      <c r="K18" s="119"/>
+      <c r="L18" s="119"/>
+      <c r="M18" s="119"/>
+      <c r="N18" s="119"/>
+      <c r="O18" s="119"/>
     </row>
     <row r="19" spans="2:15">
       <c r="B19" t="s">
@@ -9062,16 +9082,16 @@
       <c r="E19" t="s">
         <v>280</v>
       </c>
-      <c r="F19" s="118"/>
-      <c r="G19" s="118"/>
-      <c r="H19" s="118"/>
-      <c r="I19" s="118"/>
-      <c r="J19" s="118"/>
-      <c r="K19" s="118"/>
-      <c r="L19" s="118"/>
-      <c r="M19" s="118"/>
-      <c r="N19" s="118"/>
-      <c r="O19" s="118"/>
+      <c r="F19" s="119"/>
+      <c r="G19" s="119"/>
+      <c r="H19" s="119"/>
+      <c r="I19" s="119"/>
+      <c r="J19" s="119"/>
+      <c r="K19" s="119"/>
+      <c r="L19" s="119"/>
+      <c r="M19" s="119"/>
+      <c r="N19" s="119"/>
+      <c r="O19" s="119"/>
     </row>
     <row r="20" spans="2:15">
       <c r="C20" t="s">
@@ -9083,16 +9103,16 @@
       <c r="E20" t="s">
         <v>283</v>
       </c>
-      <c r="F20" s="118"/>
-      <c r="G20" s="118"/>
-      <c r="H20" s="118"/>
-      <c r="I20" s="118"/>
-      <c r="J20" s="118"/>
-      <c r="K20" s="118"/>
-      <c r="L20" s="118"/>
-      <c r="M20" s="118"/>
-      <c r="N20" s="118"/>
-      <c r="O20" s="118"/>
+      <c r="F20" s="119"/>
+      <c r="G20" s="119"/>
+      <c r="H20" s="119"/>
+      <c r="I20" s="119"/>
+      <c r="J20" s="119"/>
+      <c r="K20" s="119"/>
+      <c r="L20" s="119"/>
+      <c r="M20" s="119"/>
+      <c r="N20" s="119"/>
+      <c r="O20" s="119"/>
     </row>
     <row r="21" spans="2:15">
       <c r="B21" t="s">
@@ -9104,16 +9124,16 @@
       <c r="D21" t="s">
         <v>285</v>
       </c>
-      <c r="F21" s="118"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="118"/>
-      <c r="I21" s="118"/>
-      <c r="J21" s="118"/>
-      <c r="K21" s="118"/>
-      <c r="L21" s="118"/>
-      <c r="M21" s="118"/>
-      <c r="N21" s="118"/>
-      <c r="O21" s="118"/>
+      <c r="F21" s="119"/>
+      <c r="G21" s="119"/>
+      <c r="H21" s="119"/>
+      <c r="I21" s="119"/>
+      <c r="J21" s="119"/>
+      <c r="K21" s="119"/>
+      <c r="L21" s="119"/>
+      <c r="M21" s="119"/>
+      <c r="N21" s="119"/>
+      <c r="O21" s="119"/>
     </row>
     <row r="22" spans="2:15">
       <c r="C22" t="s">
@@ -9125,16 +9145,16 @@
       <c r="E22" t="s">
         <v>287</v>
       </c>
-      <c r="F22" s="118"/>
-      <c r="G22" s="118"/>
-      <c r="H22" s="118"/>
-      <c r="I22" s="118"/>
-      <c r="J22" s="118"/>
-      <c r="K22" s="118"/>
-      <c r="L22" s="118"/>
-      <c r="M22" s="118"/>
-      <c r="N22" s="118"/>
-      <c r="O22" s="118"/>
+      <c r="F22" s="119"/>
+      <c r="G22" s="119"/>
+      <c r="H22" s="119"/>
+      <c r="I22" s="119"/>
+      <c r="J22" s="119"/>
+      <c r="K22" s="119"/>
+      <c r="L22" s="119"/>
+      <c r="M22" s="119"/>
+      <c r="N22" s="119"/>
+      <c r="O22" s="119"/>
     </row>
     <row r="23" spans="2:15">
       <c r="B23" t="s">
@@ -9143,370 +9163,370 @@
       <c r="D23" t="s">
         <v>289</v>
       </c>
-      <c r="F23" s="118"/>
-      <c r="G23" s="118"/>
-      <c r="H23" s="118"/>
-      <c r="I23" s="118"/>
-      <c r="J23" s="118"/>
-      <c r="K23" s="118"/>
-      <c r="L23" s="118"/>
-      <c r="M23" s="118"/>
-      <c r="N23" s="118"/>
-      <c r="O23" s="118"/>
+      <c r="F23" s="119"/>
+      <c r="G23" s="119"/>
+      <c r="H23" s="119"/>
+      <c r="I23" s="119"/>
+      <c r="J23" s="119"/>
+      <c r="K23" s="119"/>
+      <c r="L23" s="119"/>
+      <c r="M23" s="119"/>
+      <c r="N23" s="119"/>
+      <c r="O23" s="119"/>
     </row>
     <row r="24" spans="2:15">
-      <c r="F24" s="118"/>
-      <c r="G24" s="118"/>
-      <c r="H24" s="118"/>
-      <c r="I24" s="118"/>
-      <c r="J24" s="118"/>
-      <c r="K24" s="118"/>
-      <c r="L24" s="118"/>
-      <c r="M24" s="118"/>
-      <c r="N24" s="118"/>
-      <c r="O24" s="118"/>
+      <c r="F24" s="119"/>
+      <c r="G24" s="119"/>
+      <c r="H24" s="119"/>
+      <c r="I24" s="119"/>
+      <c r="J24" s="119"/>
+      <c r="K24" s="119"/>
+      <c r="L24" s="119"/>
+      <c r="M24" s="119"/>
+      <c r="N24" s="119"/>
+      <c r="O24" s="119"/>
     </row>
     <row r="25" spans="2:15">
-      <c r="F25" s="118"/>
-      <c r="G25" s="118"/>
-      <c r="H25" s="118"/>
-      <c r="I25" s="118"/>
-      <c r="J25" s="118"/>
-      <c r="K25" s="118"/>
-      <c r="L25" s="118"/>
-      <c r="M25" s="118"/>
-      <c r="N25" s="118"/>
-      <c r="O25" s="118"/>
+      <c r="F25" s="119"/>
+      <c r="G25" s="119"/>
+      <c r="H25" s="119"/>
+      <c r="I25" s="119"/>
+      <c r="J25" s="119"/>
+      <c r="K25" s="119"/>
+      <c r="L25" s="119"/>
+      <c r="M25" s="119"/>
+      <c r="N25" s="119"/>
+      <c r="O25" s="119"/>
     </row>
     <row r="26" spans="2:15">
-      <c r="F26" s="118"/>
-      <c r="G26" s="118"/>
-      <c r="H26" s="118"/>
-      <c r="I26" s="118"/>
-      <c r="J26" s="118"/>
-      <c r="K26" s="118"/>
-      <c r="L26" s="118"/>
-      <c r="M26" s="118"/>
-      <c r="N26" s="118"/>
-      <c r="O26" s="118"/>
+      <c r="F26" s="119"/>
+      <c r="G26" s="119"/>
+      <c r="H26" s="119"/>
+      <c r="I26" s="119"/>
+      <c r="J26" s="119"/>
+      <c r="K26" s="119"/>
+      <c r="L26" s="119"/>
+      <c r="M26" s="119"/>
+      <c r="N26" s="119"/>
+      <c r="O26" s="119"/>
     </row>
     <row r="27" spans="2:15">
-      <c r="F27" s="118"/>
-      <c r="G27" s="118"/>
-      <c r="H27" s="118"/>
-      <c r="I27" s="118"/>
-      <c r="J27" s="118"/>
-      <c r="K27" s="118"/>
-      <c r="L27" s="118"/>
-      <c r="M27" s="118"/>
-      <c r="N27" s="118"/>
-      <c r="O27" s="118"/>
+      <c r="F27" s="119"/>
+      <c r="G27" s="119"/>
+      <c r="H27" s="119"/>
+      <c r="I27" s="119"/>
+      <c r="J27" s="119"/>
+      <c r="K27" s="119"/>
+      <c r="L27" s="119"/>
+      <c r="M27" s="119"/>
+      <c r="N27" s="119"/>
+      <c r="O27" s="119"/>
     </row>
     <row r="28" spans="2:15">
-      <c r="F28" s="118"/>
-      <c r="G28" s="118"/>
-      <c r="H28" s="118"/>
-      <c r="I28" s="118"/>
-      <c r="J28" s="118"/>
-      <c r="K28" s="118"/>
-      <c r="L28" s="118"/>
-      <c r="M28" s="118"/>
-      <c r="N28" s="118"/>
-      <c r="O28" s="118"/>
+      <c r="F28" s="119"/>
+      <c r="G28" s="119"/>
+      <c r="H28" s="119"/>
+      <c r="I28" s="119"/>
+      <c r="J28" s="119"/>
+      <c r="K28" s="119"/>
+      <c r="L28" s="119"/>
+      <c r="M28" s="119"/>
+      <c r="N28" s="119"/>
+      <c r="O28" s="119"/>
     </row>
     <row r="29" spans="2:15">
-      <c r="F29" s="118"/>
-      <c r="G29" s="118"/>
-      <c r="H29" s="118"/>
-      <c r="I29" s="118"/>
-      <c r="J29" s="118"/>
-      <c r="K29" s="118"/>
-      <c r="L29" s="118"/>
-      <c r="M29" s="118"/>
-      <c r="N29" s="118"/>
-      <c r="O29" s="118"/>
+      <c r="F29" s="119"/>
+      <c r="G29" s="119"/>
+      <c r="H29" s="119"/>
+      <c r="I29" s="119"/>
+      <c r="J29" s="119"/>
+      <c r="K29" s="119"/>
+      <c r="L29" s="119"/>
+      <c r="M29" s="119"/>
+      <c r="N29" s="119"/>
+      <c r="O29" s="119"/>
     </row>
     <row r="30" spans="2:15">
-      <c r="F30" s="118"/>
-      <c r="G30" s="118"/>
-      <c r="H30" s="118"/>
-      <c r="I30" s="118"/>
-      <c r="J30" s="118"/>
-      <c r="K30" s="118"/>
-      <c r="L30" s="118"/>
-      <c r="M30" s="118"/>
-      <c r="N30" s="118"/>
-      <c r="O30" s="118"/>
+      <c r="F30" s="119"/>
+      <c r="G30" s="119"/>
+      <c r="H30" s="119"/>
+      <c r="I30" s="119"/>
+      <c r="J30" s="119"/>
+      <c r="K30" s="119"/>
+      <c r="L30" s="119"/>
+      <c r="M30" s="119"/>
+      <c r="N30" s="119"/>
+      <c r="O30" s="119"/>
     </row>
     <row r="31" spans="2:15">
-      <c r="F31" s="118"/>
-      <c r="G31" s="118"/>
-      <c r="H31" s="118"/>
-      <c r="I31" s="118"/>
-      <c r="J31" s="118"/>
-      <c r="K31" s="118"/>
-      <c r="L31" s="118"/>
-      <c r="M31" s="118"/>
-      <c r="N31" s="118"/>
-      <c r="O31" s="118"/>
+      <c r="F31" s="119"/>
+      <c r="G31" s="119"/>
+      <c r="H31" s="119"/>
+      <c r="I31" s="119"/>
+      <c r="J31" s="119"/>
+      <c r="K31" s="119"/>
+      <c r="L31" s="119"/>
+      <c r="M31" s="119"/>
+      <c r="N31" s="119"/>
+      <c r="O31" s="119"/>
     </row>
     <row r="32" spans="2:15">
-      <c r="F32" s="118"/>
-      <c r="G32" s="118"/>
-      <c r="H32" s="118"/>
-      <c r="I32" s="118"/>
-      <c r="J32" s="118"/>
-      <c r="K32" s="118"/>
-      <c r="L32" s="118"/>
-      <c r="M32" s="118"/>
-      <c r="N32" s="118"/>
-      <c r="O32" s="118"/>
+      <c r="F32" s="119"/>
+      <c r="G32" s="119"/>
+      <c r="H32" s="119"/>
+      <c r="I32" s="119"/>
+      <c r="J32" s="119"/>
+      <c r="K32" s="119"/>
+      <c r="L32" s="119"/>
+      <c r="M32" s="119"/>
+      <c r="N32" s="119"/>
+      <c r="O32" s="119"/>
     </row>
     <row r="33" spans="5:15">
-      <c r="F33" s="118"/>
-      <c r="G33" s="118"/>
-      <c r="H33" s="118"/>
-      <c r="I33" s="118"/>
-      <c r="J33" s="118"/>
-      <c r="K33" s="118"/>
-      <c r="L33" s="118"/>
-      <c r="M33" s="118"/>
-      <c r="N33" s="118"/>
-      <c r="O33" s="118"/>
+      <c r="F33" s="119"/>
+      <c r="G33" s="119"/>
+      <c r="H33" s="119"/>
+      <c r="I33" s="119"/>
+      <c r="J33" s="119"/>
+      <c r="K33" s="119"/>
+      <c r="L33" s="119"/>
+      <c r="M33" s="119"/>
+      <c r="N33" s="119"/>
+      <c r="O33" s="119"/>
     </row>
     <row r="34" spans="5:15">
-      <c r="F34" s="118"/>
-      <c r="G34" s="118"/>
-      <c r="H34" s="118"/>
-      <c r="I34" s="118"/>
-      <c r="J34" s="118"/>
-      <c r="K34" s="118"/>
-      <c r="L34" s="118"/>
-      <c r="M34" s="118"/>
-      <c r="N34" s="118"/>
-      <c r="O34" s="118"/>
+      <c r="F34" s="119"/>
+      <c r="G34" s="119"/>
+      <c r="H34" s="119"/>
+      <c r="I34" s="119"/>
+      <c r="J34" s="119"/>
+      <c r="K34" s="119"/>
+      <c r="L34" s="119"/>
+      <c r="M34" s="119"/>
+      <c r="N34" s="119"/>
+      <c r="O34" s="119"/>
     </row>
     <row r="35" spans="5:15">
-      <c r="F35" s="118"/>
-      <c r="G35" s="118"/>
-      <c r="H35" s="118"/>
-      <c r="I35" s="118"/>
-      <c r="J35" s="118"/>
-      <c r="K35" s="118"/>
-      <c r="L35" s="118"/>
-      <c r="M35" s="118"/>
-      <c r="N35" s="118"/>
-      <c r="O35" s="118"/>
+      <c r="F35" s="119"/>
+      <c r="G35" s="119"/>
+      <c r="H35" s="119"/>
+      <c r="I35" s="119"/>
+      <c r="J35" s="119"/>
+      <c r="K35" s="119"/>
+      <c r="L35" s="119"/>
+      <c r="M35" s="119"/>
+      <c r="N35" s="119"/>
+      <c r="O35" s="119"/>
     </row>
     <row r="36" spans="5:15" ht="14">
       <c r="E36" s="23" t="s">
         <v>290</v>
       </c>
-      <c r="F36" s="118"/>
-      <c r="G36" s="118"/>
-      <c r="H36" s="118"/>
-      <c r="I36" s="118"/>
-      <c r="J36" s="118"/>
-      <c r="K36" s="118"/>
-      <c r="L36" s="118"/>
-      <c r="M36" s="118"/>
-      <c r="N36" s="118"/>
-      <c r="O36" s="118"/>
+      <c r="F36" s="119"/>
+      <c r="G36" s="119"/>
+      <c r="H36" s="119"/>
+      <c r="I36" s="119"/>
+      <c r="J36" s="119"/>
+      <c r="K36" s="119"/>
+      <c r="L36" s="119"/>
+      <c r="M36" s="119"/>
+      <c r="N36" s="119"/>
+      <c r="O36" s="119"/>
     </row>
     <row r="37" spans="5:15" ht="14">
       <c r="E37" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="F37" s="118"/>
-      <c r="G37" s="118"/>
-      <c r="H37" s="118"/>
-      <c r="I37" s="118"/>
-      <c r="J37" s="118"/>
-      <c r="K37" s="118"/>
-      <c r="L37" s="118"/>
-      <c r="M37" s="118"/>
-      <c r="N37" s="118"/>
-      <c r="O37" s="118"/>
+      <c r="F37" s="119"/>
+      <c r="G37" s="119"/>
+      <c r="H37" s="119"/>
+      <c r="I37" s="119"/>
+      <c r="J37" s="119"/>
+      <c r="K37" s="119"/>
+      <c r="L37" s="119"/>
+      <c r="M37" s="119"/>
+      <c r="N37" s="119"/>
+      <c r="O37" s="119"/>
     </row>
     <row r="38" spans="5:15">
-      <c r="F38" s="118"/>
-      <c r="G38" s="118"/>
-      <c r="H38" s="118"/>
-      <c r="I38" s="118"/>
-      <c r="J38" s="118"/>
-      <c r="K38" s="118"/>
-      <c r="L38" s="118"/>
-      <c r="M38" s="118"/>
-      <c r="N38" s="118"/>
-      <c r="O38" s="118"/>
+      <c r="F38" s="119"/>
+      <c r="G38" s="119"/>
+      <c r="H38" s="119"/>
+      <c r="I38" s="119"/>
+      <c r="J38" s="119"/>
+      <c r="K38" s="119"/>
+      <c r="L38" s="119"/>
+      <c r="M38" s="119"/>
+      <c r="N38" s="119"/>
+      <c r="O38" s="119"/>
     </row>
     <row r="39" spans="5:15">
-      <c r="F39" s="118"/>
-      <c r="G39" s="118"/>
-      <c r="H39" s="118"/>
-      <c r="I39" s="118"/>
-      <c r="J39" s="118"/>
-      <c r="K39" s="118"/>
-      <c r="L39" s="118"/>
-      <c r="M39" s="118"/>
-      <c r="N39" s="118"/>
-      <c r="O39" s="118"/>
+      <c r="F39" s="119"/>
+      <c r="G39" s="119"/>
+      <c r="H39" s="119"/>
+      <c r="I39" s="119"/>
+      <c r="J39" s="119"/>
+      <c r="K39" s="119"/>
+      <c r="L39" s="119"/>
+      <c r="M39" s="119"/>
+      <c r="N39" s="119"/>
+      <c r="O39" s="119"/>
     </row>
     <row r="40" spans="5:15">
-      <c r="F40" s="118"/>
-      <c r="G40" s="118"/>
-      <c r="H40" s="118"/>
-      <c r="I40" s="118"/>
-      <c r="J40" s="118"/>
-      <c r="K40" s="118"/>
-      <c r="L40" s="118"/>
-      <c r="M40" s="118"/>
-      <c r="N40" s="118"/>
-      <c r="O40" s="118"/>
+      <c r="F40" s="119"/>
+      <c r="G40" s="119"/>
+      <c r="H40" s="119"/>
+      <c r="I40" s="119"/>
+      <c r="J40" s="119"/>
+      <c r="K40" s="119"/>
+      <c r="L40" s="119"/>
+      <c r="M40" s="119"/>
+      <c r="N40" s="119"/>
+      <c r="O40" s="119"/>
     </row>
     <row r="41" spans="5:15">
-      <c r="F41" s="118"/>
-      <c r="G41" s="118"/>
-      <c r="H41" s="118"/>
-      <c r="I41" s="118"/>
-      <c r="J41" s="118"/>
-      <c r="K41" s="118"/>
-      <c r="L41" s="118"/>
-      <c r="M41" s="118"/>
-      <c r="N41" s="118"/>
-      <c r="O41" s="118"/>
+      <c r="F41" s="119"/>
+      <c r="G41" s="119"/>
+      <c r="H41" s="119"/>
+      <c r="I41" s="119"/>
+      <c r="J41" s="119"/>
+      <c r="K41" s="119"/>
+      <c r="L41" s="119"/>
+      <c r="M41" s="119"/>
+      <c r="N41" s="119"/>
+      <c r="O41" s="119"/>
     </row>
     <row r="42" spans="5:15">
-      <c r="F42" s="118"/>
-      <c r="G42" s="118"/>
-      <c r="H42" s="118"/>
-      <c r="I42" s="118"/>
-      <c r="J42" s="118"/>
-      <c r="K42" s="118"/>
-      <c r="L42" s="118"/>
-      <c r="M42" s="118"/>
-      <c r="N42" s="118"/>
-      <c r="O42" s="118"/>
+      <c r="F42" s="119"/>
+      <c r="G42" s="119"/>
+      <c r="H42" s="119"/>
+      <c r="I42" s="119"/>
+      <c r="J42" s="119"/>
+      <c r="K42" s="119"/>
+      <c r="L42" s="119"/>
+      <c r="M42" s="119"/>
+      <c r="N42" s="119"/>
+      <c r="O42" s="119"/>
     </row>
     <row r="43" spans="5:15">
-      <c r="F43" s="118"/>
-      <c r="G43" s="118"/>
-      <c r="H43" s="118"/>
-      <c r="I43" s="118"/>
-      <c r="J43" s="118"/>
-      <c r="K43" s="118"/>
-      <c r="L43" s="118"/>
-      <c r="M43" s="118"/>
-      <c r="N43" s="118"/>
-      <c r="O43" s="118"/>
+      <c r="F43" s="119"/>
+      <c r="G43" s="119"/>
+      <c r="H43" s="119"/>
+      <c r="I43" s="119"/>
+      <c r="J43" s="119"/>
+      <c r="K43" s="119"/>
+      <c r="L43" s="119"/>
+      <c r="M43" s="119"/>
+      <c r="N43" s="119"/>
+      <c r="O43" s="119"/>
     </row>
     <row r="44" spans="5:15">
-      <c r="F44" s="118"/>
-      <c r="G44" s="118"/>
-      <c r="H44" s="118"/>
-      <c r="I44" s="118"/>
-      <c r="J44" s="118"/>
-      <c r="K44" s="118"/>
-      <c r="L44" s="118"/>
-      <c r="M44" s="118"/>
-      <c r="N44" s="118"/>
-      <c r="O44" s="118"/>
+      <c r="F44" s="119"/>
+      <c r="G44" s="119"/>
+      <c r="H44" s="119"/>
+      <c r="I44" s="119"/>
+      <c r="J44" s="119"/>
+      <c r="K44" s="119"/>
+      <c r="L44" s="119"/>
+      <c r="M44" s="119"/>
+      <c r="N44" s="119"/>
+      <c r="O44" s="119"/>
     </row>
     <row r="45" spans="5:15">
-      <c r="F45" s="118"/>
-      <c r="G45" s="118"/>
-      <c r="H45" s="118"/>
-      <c r="I45" s="118"/>
-      <c r="J45" s="118"/>
-      <c r="K45" s="118"/>
-      <c r="L45" s="118"/>
-      <c r="M45" s="118"/>
-      <c r="N45" s="118"/>
-      <c r="O45" s="118"/>
+      <c r="F45" s="119"/>
+      <c r="G45" s="119"/>
+      <c r="H45" s="119"/>
+      <c r="I45" s="119"/>
+      <c r="J45" s="119"/>
+      <c r="K45" s="119"/>
+      <c r="L45" s="119"/>
+      <c r="M45" s="119"/>
+      <c r="N45" s="119"/>
+      <c r="O45" s="119"/>
     </row>
     <row r="46" spans="5:15">
-      <c r="F46" s="118"/>
-      <c r="G46" s="118"/>
-      <c r="H46" s="118"/>
-      <c r="I46" s="118"/>
-      <c r="J46" s="118"/>
-      <c r="K46" s="118"/>
-      <c r="L46" s="118"/>
-      <c r="M46" s="118"/>
-      <c r="N46" s="118"/>
-      <c r="O46" s="118"/>
+      <c r="F46" s="119"/>
+      <c r="G46" s="119"/>
+      <c r="H46" s="119"/>
+      <c r="I46" s="119"/>
+      <c r="J46" s="119"/>
+      <c r="K46" s="119"/>
+      <c r="L46" s="119"/>
+      <c r="M46" s="119"/>
+      <c r="N46" s="119"/>
+      <c r="O46" s="119"/>
     </row>
     <row r="47" spans="5:15">
-      <c r="F47" s="118"/>
-      <c r="G47" s="118"/>
-      <c r="H47" s="118"/>
-      <c r="I47" s="118"/>
-      <c r="J47" s="118"/>
-      <c r="K47" s="118"/>
-      <c r="L47" s="118"/>
-      <c r="M47" s="118"/>
-      <c r="N47" s="118"/>
-      <c r="O47" s="118"/>
+      <c r="F47" s="119"/>
+      <c r="G47" s="119"/>
+      <c r="H47" s="119"/>
+      <c r="I47" s="119"/>
+      <c r="J47" s="119"/>
+      <c r="K47" s="119"/>
+      <c r="L47" s="119"/>
+      <c r="M47" s="119"/>
+      <c r="N47" s="119"/>
+      <c r="O47" s="119"/>
     </row>
     <row r="48" spans="5:15">
-      <c r="F48" s="118"/>
-      <c r="G48" s="118"/>
-      <c r="H48" s="118"/>
-      <c r="I48" s="118"/>
-      <c r="J48" s="118"/>
-      <c r="K48" s="118"/>
-      <c r="L48" s="118"/>
-      <c r="M48" s="118"/>
-      <c r="N48" s="118"/>
-      <c r="O48" s="118"/>
+      <c r="F48" s="119"/>
+      <c r="G48" s="119"/>
+      <c r="H48" s="119"/>
+      <c r="I48" s="119"/>
+      <c r="J48" s="119"/>
+      <c r="K48" s="119"/>
+      <c r="L48" s="119"/>
+      <c r="M48" s="119"/>
+      <c r="N48" s="119"/>
+      <c r="O48" s="119"/>
     </row>
     <row r="49" spans="6:15">
-      <c r="F49" s="118"/>
-      <c r="G49" s="118"/>
-      <c r="H49" s="118"/>
-      <c r="I49" s="118"/>
-      <c r="J49" s="118"/>
-      <c r="K49" s="118"/>
-      <c r="L49" s="118"/>
-      <c r="M49" s="118"/>
-      <c r="N49" s="118"/>
-      <c r="O49" s="118"/>
+      <c r="F49" s="119"/>
+      <c r="G49" s="119"/>
+      <c r="H49" s="119"/>
+      <c r="I49" s="119"/>
+      <c r="J49" s="119"/>
+      <c r="K49" s="119"/>
+      <c r="L49" s="119"/>
+      <c r="M49" s="119"/>
+      <c r="N49" s="119"/>
+      <c r="O49" s="119"/>
     </row>
     <row r="50" spans="6:15">
-      <c r="F50" s="118"/>
-      <c r="G50" s="118"/>
-      <c r="H50" s="118"/>
-      <c r="I50" s="118"/>
-      <c r="J50" s="118"/>
-      <c r="K50" s="118"/>
-      <c r="L50" s="118"/>
-      <c r="M50" s="118"/>
-      <c r="N50" s="118"/>
-      <c r="O50" s="118"/>
+      <c r="F50" s="119"/>
+      <c r="G50" s="119"/>
+      <c r="H50" s="119"/>
+      <c r="I50" s="119"/>
+      <c r="J50" s="119"/>
+      <c r="K50" s="119"/>
+      <c r="L50" s="119"/>
+      <c r="M50" s="119"/>
+      <c r="N50" s="119"/>
+      <c r="O50" s="119"/>
     </row>
     <row r="51" spans="6:15">
-      <c r="F51" s="118"/>
-      <c r="G51" s="118"/>
-      <c r="H51" s="118"/>
-      <c r="I51" s="118"/>
-      <c r="J51" s="118"/>
-      <c r="K51" s="118"/>
-      <c r="L51" s="118"/>
-      <c r="M51" s="118"/>
-      <c r="N51" s="118"/>
-      <c r="O51" s="118"/>
+      <c r="F51" s="119"/>
+      <c r="G51" s="119"/>
+      <c r="H51" s="119"/>
+      <c r="I51" s="119"/>
+      <c r="J51" s="119"/>
+      <c r="K51" s="119"/>
+      <c r="L51" s="119"/>
+      <c r="M51" s="119"/>
+      <c r="N51" s="119"/>
+      <c r="O51" s="119"/>
     </row>
     <row r="52" spans="6:15">
-      <c r="F52" s="118"/>
-      <c r="G52" s="118"/>
-      <c r="H52" s="118"/>
-      <c r="I52" s="118"/>
-      <c r="J52" s="118"/>
-      <c r="K52" s="118"/>
-      <c r="L52" s="118"/>
-      <c r="M52" s="118"/>
-      <c r="N52" s="118"/>
-      <c r="O52" s="118"/>
+      <c r="F52" s="119"/>
+      <c r="G52" s="119"/>
+      <c r="H52" s="119"/>
+      <c r="I52" s="119"/>
+      <c r="J52" s="119"/>
+      <c r="K52" s="119"/>
+      <c r="L52" s="119"/>
+      <c r="M52" s="119"/>
+      <c r="N52" s="119"/>
+      <c r="O52" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -9760,7 +9780,7 @@
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="D11" s="120" t="s">
+      <c r="D11" s="86" t="s">
         <v>467</v>
       </c>
       <c r="E11" s="15" t="s">

</xml_diff>

<commit_message>
Some modificatons of chartist, fixed some bits. GM2 plot as well.
</commit_message>
<xml_diff>
--- a/Macro_Chartist/Control.xlsx
+++ b/Macro_Chartist/Control.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\Code\Bootleg_Macro\Macro_Chartist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182363F5-EE49-4CCF-B11C-A1F8135935BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974BBB32-41BA-4552-B053-D49AAD0A88A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <sheet name="TemplateList" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="473">
   <si>
     <t>Index</t>
   </si>
@@ -1596,10 +1595,13 @@
     <t>Bitcoin price change is fueled by global monetary growth</t>
   </si>
   <si>
-    <t>YoY % change (numbers not right here but shape unchanged)</t>
-  </si>
-  <si>
     <t>2011-06-01</t>
+  </si>
+  <si>
+    <t>GM2_fc_Av3m</t>
+  </si>
+  <si>
+    <t>GM2 Forecast @ last 3 months mean growth rate</t>
   </si>
 </sst>
 </file>
@@ -2207,53 +2209,39 @@
     <xf numFmtId="49" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2273,36 +2261,50 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2576,8 +2578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2654,10 +2656,10 @@
       <c r="G2" s="10" t="s">
         <v>468</v>
       </c>
-      <c r="H2" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="I2" s="11"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="11" t="s">
+        <v>301</v>
+      </c>
       <c r="J2" s="9" t="s">
         <v>25</v>
       </c>
@@ -2666,8 +2668,8 @@
       <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>239</v>
+      <c r="B3" s="12" t="s">
+        <v>471</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>90</v>
@@ -2676,18 +2678,18 @@
         <v>163</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>18</v>
+        <v>345</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>470</v>
-      </c>
-      <c r="I3" s="11"/>
+        <v>472</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11" t="s">
+        <v>301</v>
+      </c>
       <c r="J3" s="9" t="s">
         <v>25</v>
       </c>
@@ -2696,15 +2698,31 @@
       <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
+      <c r="B4" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>124</v>
+      </c>
       <c r="H4" s="10"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="9"/>
+      <c r="I4" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
@@ -2718,7 +2736,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="11"/>
-      <c r="J5" s="9"/>
+      <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
@@ -2738,14 +2756,14 @@
       <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="8"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
-      <c r="I7" s="16"/>
+      <c r="I7" s="11"/>
       <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2805,72 +2823,72 @@
       <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="89" t="s">
+      <c r="C12" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="88" t="s">
+      <c r="D12" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="88" t="s">
+      <c r="E12" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="90" t="s">
+      <c r="F12" s="115" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="88" t="s">
+      <c r="G12" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="88" t="s">
+      <c r="H12" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="91" t="s">
+      <c r="I12" s="111" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="88" t="s">
+      <c r="J12" s="91" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="87"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="89"/>
-      <c r="D13" s="88"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="88"/>
-      <c r="H13" s="88"/>
-      <c r="I13" s="91"/>
-      <c r="J13" s="88"/>
+      <c r="A13" s="116"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="91"/>
     </row>
     <row r="14" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="87"/>
-      <c r="B14" s="88"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="88"/>
-      <c r="H14" s="88"/>
-      <c r="I14" s="91"/>
-      <c r="J14" s="88"/>
+      <c r="A14" s="116"/>
+      <c r="B14" s="91"/>
+      <c r="C14" s="117"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="91"/>
+      <c r="F14" s="91"/>
+      <c r="G14" s="91"/>
+      <c r="H14" s="91"/>
+      <c r="I14" s="111"/>
+      <c r="J14" s="91"/>
     </row>
     <row r="15" spans="1:36" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="87"/>
-      <c r="B15" s="88"/>
-      <c r="C15" s="89"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="88"/>
-      <c r="H15" s="88"/>
-      <c r="I15" s="91"/>
-      <c r="J15" s="88"/>
+      <c r="A15" s="116"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="117"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="91"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="111"/>
+      <c r="J15" s="91"/>
     </row>
     <row r="16" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
@@ -3105,170 +3123,170 @@
       <c r="J26" s="25"/>
     </row>
     <row r="27" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="96" t="s">
+      <c r="A27" s="113" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="97" t="s">
+      <c r="B27" s="114" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="97" t="s">
+      <c r="C27" s="114" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="91" t="s">
+      <c r="D27" s="111" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="94" t="s">
+      <c r="E27" s="110" t="s">
         <v>51</v>
       </c>
-      <c r="F27" s="92" t="s">
+      <c r="F27" s="108" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="93" t="s">
+      <c r="G27" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="H27" s="94" t="s">
+      <c r="H27" s="110" t="s">
         <v>54</v>
       </c>
-      <c r="I27" s="91" t="s">
+      <c r="I27" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="J27" s="91" t="s">
+      <c r="J27" s="111" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="96"/>
-      <c r="B28" s="97"/>
-      <c r="C28" s="97"/>
-      <c r="D28" s="91"/>
-      <c r="E28" s="94"/>
-      <c r="F28" s="92"/>
-      <c r="G28" s="93"/>
-      <c r="H28" s="94"/>
-      <c r="I28" s="91"/>
-      <c r="J28" s="91"/>
+      <c r="A28" s="113"/>
+      <c r="B28" s="114"/>
+      <c r="C28" s="114"/>
+      <c r="D28" s="111"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="108"/>
+      <c r="G28" s="109"/>
+      <c r="H28" s="110"/>
+      <c r="I28" s="111"/>
+      <c r="J28" s="111"/>
     </row>
     <row r="29" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="96"/>
-      <c r="B29" s="97"/>
-      <c r="C29" s="97"/>
-      <c r="D29" s="91"/>
-      <c r="E29" s="94"/>
-      <c r="F29" s="92"/>
-      <c r="G29" s="93"/>
-      <c r="H29" s="94"/>
-      <c r="I29" s="91"/>
-      <c r="J29" s="91"/>
+      <c r="A29" s="113"/>
+      <c r="B29" s="114"/>
+      <c r="C29" s="114"/>
+      <c r="D29" s="111"/>
+      <c r="E29" s="110"/>
+      <c r="F29" s="108"/>
+      <c r="G29" s="109"/>
+      <c r="H29" s="110"/>
+      <c r="I29" s="111"/>
+      <c r="J29" s="111"/>
     </row>
     <row r="30" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="96"/>
-      <c r="B30" s="97"/>
-      <c r="C30" s="97"/>
-      <c r="D30" s="91"/>
-      <c r="E30" s="94"/>
-      <c r="F30" s="92"/>
-      <c r="G30" s="93"/>
-      <c r="H30" s="94"/>
-      <c r="I30" s="91"/>
-      <c r="J30" s="91"/>
+      <c r="A30" s="113"/>
+      <c r="B30" s="114"/>
+      <c r="C30" s="114"/>
+      <c r="D30" s="111"/>
+      <c r="E30" s="110"/>
+      <c r="F30" s="108"/>
+      <c r="G30" s="109"/>
+      <c r="H30" s="110"/>
+      <c r="I30" s="111"/>
+      <c r="J30" s="111"/>
     </row>
     <row r="31" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="96"/>
-      <c r="B31" s="97"/>
-      <c r="C31" s="97"/>
-      <c r="D31" s="91"/>
-      <c r="E31" s="94"/>
-      <c r="F31" s="92"/>
-      <c r="G31" s="93"/>
-      <c r="H31" s="94"/>
-      <c r="I31" s="91"/>
-      <c r="J31" s="91"/>
+      <c r="A31" s="113"/>
+      <c r="B31" s="114"/>
+      <c r="C31" s="114"/>
+      <c r="D31" s="111"/>
+      <c r="E31" s="110"/>
+      <c r="F31" s="108"/>
+      <c r="G31" s="109"/>
+      <c r="H31" s="110"/>
+      <c r="I31" s="111"/>
+      <c r="J31" s="111"/>
     </row>
     <row r="32" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="96"/>
-      <c r="B32" s="97"/>
-      <c r="C32" s="97"/>
-      <c r="D32" s="91"/>
-      <c r="E32" s="94"/>
-      <c r="F32" s="92"/>
-      <c r="G32" s="93"/>
-      <c r="H32" s="94"/>
-      <c r="I32" s="91"/>
-      <c r="J32" s="91"/>
+      <c r="A32" s="113"/>
+      <c r="B32" s="114"/>
+      <c r="C32" s="114"/>
+      <c r="D32" s="111"/>
+      <c r="E32" s="110"/>
+      <c r="F32" s="108"/>
+      <c r="G32" s="109"/>
+      <c r="H32" s="110"/>
+      <c r="I32" s="111"/>
+      <c r="J32" s="111"/>
     </row>
     <row r="33" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="95" t="s">
+      <c r="A33" s="112" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="95"/>
-      <c r="C33" s="95"/>
-      <c r="D33" s="95"/>
-      <c r="E33" s="95"/>
-      <c r="F33" s="95"/>
-      <c r="G33" s="95"/>
-      <c r="H33" s="94"/>
-      <c r="I33" s="91"/>
-      <c r="J33" s="91"/>
+      <c r="B33" s="112"/>
+      <c r="C33" s="112"/>
+      <c r="D33" s="112"/>
+      <c r="E33" s="112"/>
+      <c r="F33" s="112"/>
+      <c r="G33" s="112"/>
+      <c r="H33" s="110"/>
+      <c r="I33" s="111"/>
+      <c r="J33" s="111"/>
     </row>
     <row r="34" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="98"/>
-      <c r="B34" s="98"/>
-      <c r="C34" s="98"/>
-      <c r="D34" s="98"/>
-      <c r="E34" s="98"/>
-      <c r="F34" s="98"/>
-      <c r="G34" s="98"/>
-      <c r="H34" s="98"/>
-      <c r="I34" s="98"/>
-      <c r="J34" s="98"/>
+      <c r="A34" s="103"/>
+      <c r="B34" s="103"/>
+      <c r="C34" s="103"/>
+      <c r="D34" s="103"/>
+      <c r="E34" s="103"/>
+      <c r="F34" s="103"/>
+      <c r="G34" s="103"/>
+      <c r="H34" s="103"/>
+      <c r="I34" s="103"/>
+      <c r="J34" s="103"/>
     </row>
     <row r="35" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="99" t="s">
+      <c r="A35" s="104" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="99"/>
-      <c r="C35" s="99"/>
-      <c r="D35" s="99"/>
-      <c r="E35" s="99"/>
-      <c r="F35" s="99"/>
-      <c r="G35" s="99"/>
-      <c r="H35" s="99"/>
-      <c r="I35" s="99"/>
-      <c r="J35" s="99"/>
+      <c r="B35" s="104"/>
+      <c r="C35" s="104"/>
+      <c r="D35" s="104"/>
+      <c r="E35" s="104"/>
+      <c r="F35" s="104"/>
+      <c r="G35" s="104"/>
+      <c r="H35" s="104"/>
+      <c r="I35" s="104"/>
+      <c r="J35" s="104"/>
     </row>
     <row r="36" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
         <v>59</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>471</v>
-      </c>
-      <c r="C36" s="100" t="s">
+        <v>470</v>
+      </c>
+      <c r="C36" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="D36" s="100"/>
-      <c r="E36" s="101"/>
-      <c r="F36" s="101"/>
-      <c r="G36" s="101"/>
-      <c r="H36" s="101"/>
-      <c r="I36" s="101"/>
-      <c r="J36" s="101"/>
+      <c r="D36" s="105"/>
+      <c r="E36" s="106"/>
+      <c r="F36" s="106"/>
+      <c r="G36" s="106"/>
+      <c r="H36" s="106"/>
+      <c r="I36" s="106"/>
+      <c r="J36" s="106"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="30" t="s">
         <v>61</v>
       </c>
       <c r="B37" s="31"/>
-      <c r="C37" s="102" t="s">
+      <c r="C37" s="107" t="s">
         <v>62</v>
       </c>
-      <c r="D37" s="102"/>
-      <c r="E37" s="101"/>
-      <c r="F37" s="101"/>
-      <c r="G37" s="101"/>
-      <c r="H37" s="101"/>
-      <c r="I37" s="101"/>
-      <c r="J37" s="101"/>
+      <c r="D37" s="107"/>
+      <c r="E37" s="106"/>
+      <c r="F37" s="106"/>
+      <c r="G37" s="106"/>
+      <c r="H37" s="106"/>
+      <c r="I37" s="106"/>
+      <c r="J37" s="106"/>
       <c r="K37" s="20"/>
       <c r="L37" s="20"/>
     </row>
@@ -3276,17 +3294,17 @@
       <c r="A38" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="B38" s="103"/>
-      <c r="C38" s="103"/>
-      <c r="D38" s="103"/>
-      <c r="E38" s="104" t="s">
+      <c r="B38" s="98"/>
+      <c r="C38" s="98"/>
+      <c r="D38" s="98"/>
+      <c r="E38" s="99" t="s">
         <v>64</v>
       </c>
-      <c r="F38" s="104"/>
-      <c r="G38" s="104"/>
-      <c r="H38" s="104"/>
-      <c r="I38" s="104"/>
-      <c r="J38" s="104"/>
+      <c r="F38" s="99"/>
+      <c r="G38" s="99"/>
+      <c r="H38" s="99"/>
+      <c r="I38" s="99"/>
+      <c r="J38" s="99"/>
       <c r="K38" s="33"/>
       <c r="L38" s="33"/>
     </row>
@@ -3294,21 +3312,21 @@
       <c r="A39" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="B39" s="105" t="s">
+      <c r="B39" s="100" t="s">
         <v>469</v>
       </c>
-      <c r="C39" s="105"/>
-      <c r="D39" s="105"/>
-      <c r="E39" s="105"/>
-      <c r="F39" s="106" t="s">
+      <c r="C39" s="100"/>
+      <c r="D39" s="100"/>
+      <c r="E39" s="100"/>
+      <c r="F39" s="101" t="s">
         <v>66</v>
       </c>
-      <c r="G39" s="106"/>
-      <c r="H39" s="107" t="s">
+      <c r="G39" s="101"/>
+      <c r="H39" s="102" t="s">
         <v>67</v>
       </c>
-      <c r="I39" s="107"/>
-      <c r="J39" s="107"/>
+      <c r="I39" s="102"/>
+      <c r="J39" s="102"/>
       <c r="K39" s="34"/>
       <c r="L39" s="34"/>
       <c r="M39" s="34"/>
@@ -3320,80 +3338,80 @@
       <c r="B40" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="111" t="s">
+      <c r="C40" s="90" t="s">
         <v>69</v>
       </c>
-      <c r="D40" s="111"/>
-      <c r="E40" s="111"/>
-      <c r="F40" s="111"/>
+      <c r="D40" s="90"/>
+      <c r="E40" s="90"/>
+      <c r="F40" s="90"/>
       <c r="G40" s="37"/>
-      <c r="H40" s="88" t="s">
+      <c r="H40" s="91" t="s">
         <v>70</v>
       </c>
-      <c r="I40" s="88"/>
-      <c r="J40" s="88"/>
+      <c r="I40" s="91"/>
+      <c r="J40" s="91"/>
       <c r="K40" s="34"/>
       <c r="L40" s="34"/>
       <c r="M40" s="34"/>
     </row>
     <row r="41" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="112"/>
-      <c r="B41" s="112"/>
-      <c r="C41" s="112"/>
-      <c r="D41" s="112"/>
-      <c r="E41" s="112"/>
-      <c r="F41" s="112"/>
-      <c r="G41" s="112"/>
-      <c r="H41" s="88"/>
-      <c r="I41" s="88"/>
-      <c r="J41" s="88"/>
+      <c r="A41" s="92"/>
+      <c r="B41" s="92"/>
+      <c r="C41" s="92"/>
+      <c r="D41" s="92"/>
+      <c r="E41" s="92"/>
+      <c r="F41" s="92"/>
+      <c r="G41" s="92"/>
+      <c r="H41" s="91"/>
+      <c r="I41" s="91"/>
+      <c r="J41" s="91"/>
       <c r="K41" s="34"/>
       <c r="L41" s="34"/>
       <c r="M41" s="34"/>
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="112"/>
-      <c r="B42" s="112"/>
-      <c r="C42" s="112"/>
-      <c r="D42" s="112"/>
-      <c r="E42" s="112"/>
-      <c r="F42" s="112"/>
-      <c r="G42" s="112"/>
-      <c r="H42" s="88"/>
-      <c r="I42" s="88"/>
-      <c r="J42" s="88"/>
+      <c r="A42" s="92"/>
+      <c r="B42" s="92"/>
+      <c r="C42" s="92"/>
+      <c r="D42" s="92"/>
+      <c r="E42" s="92"/>
+      <c r="F42" s="92"/>
+      <c r="G42" s="92"/>
+      <c r="H42" s="91"/>
+      <c r="I42" s="91"/>
+      <c r="J42" s="91"/>
       <c r="K42" s="34"/>
       <c r="L42" s="34"/>
       <c r="M42" s="34"/>
     </row>
     <row r="43" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="112"/>
-      <c r="B43" s="112"/>
-      <c r="C43" s="112"/>
-      <c r="D43" s="112"/>
-      <c r="E43" s="112"/>
-      <c r="F43" s="112"/>
-      <c r="G43" s="112"/>
-      <c r="H43" s="88"/>
-      <c r="I43" s="88"/>
-      <c r="J43" s="88"/>
+      <c r="A43" s="92"/>
+      <c r="B43" s="92"/>
+      <c r="C43" s="92"/>
+      <c r="D43" s="92"/>
+      <c r="E43" s="92"/>
+      <c r="F43" s="92"/>
+      <c r="G43" s="92"/>
+      <c r="H43" s="91"/>
+      <c r="I43" s="91"/>
+      <c r="J43" s="91"/>
       <c r="K43" s="34"/>
       <c r="L43" s="34"/>
       <c r="M43" s="34"/>
     </row>
     <row r="44" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A44" s="113" t="s">
+      <c r="A44" s="93" t="s">
         <v>71</v>
       </c>
-      <c r="B44" s="113"/>
-      <c r="C44" s="113"/>
-      <c r="D44" s="113"/>
-      <c r="E44" s="113"/>
-      <c r="F44" s="113"/>
-      <c r="G44" s="113"/>
-      <c r="H44" s="88"/>
-      <c r="I44" s="88"/>
-      <c r="J44" s="88"/>
+      <c r="B44" s="93"/>
+      <c r="C44" s="93"/>
+      <c r="D44" s="93"/>
+      <c r="E44" s="93"/>
+      <c r="F44" s="93"/>
+      <c r="G44" s="93"/>
+      <c r="H44" s="91"/>
+      <c r="I44" s="91"/>
+      <c r="J44" s="91"/>
       <c r="K44" s="34"/>
       <c r="L44" s="34"/>
       <c r="M44" s="34"/>
@@ -3405,16 +3423,16 @@
       <c r="B45" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="114" t="s">
+      <c r="C45" s="94" t="s">
         <v>73</v>
       </c>
-      <c r="D45" s="114"/>
-      <c r="E45" s="114"/>
-      <c r="F45" s="114"/>
-      <c r="G45" s="114"/>
-      <c r="H45" s="88"/>
-      <c r="I45" s="88"/>
-      <c r="J45" s="88"/>
+      <c r="D45" s="94"/>
+      <c r="E45" s="94"/>
+      <c r="F45" s="94"/>
+      <c r="G45" s="94"/>
+      <c r="H45" s="91"/>
+      <c r="I45" s="91"/>
+      <c r="J45" s="91"/>
       <c r="K45" s="34"/>
       <c r="L45" s="34"/>
       <c r="M45" s="34"/>
@@ -3424,16 +3442,16 @@
         <v>74</v>
       </c>
       <c r="B46" s="40"/>
-      <c r="C46" s="115" t="s">
+      <c r="C46" s="95" t="s">
         <v>75</v>
       </c>
-      <c r="D46" s="115"/>
-      <c r="E46" s="115"/>
-      <c r="F46" s="115"/>
-      <c r="G46" s="115"/>
-      <c r="H46" s="88"/>
-      <c r="I46" s="88"/>
-      <c r="J46" s="88"/>
+      <c r="D46" s="95"/>
+      <c r="E46" s="95"/>
+      <c r="F46" s="95"/>
+      <c r="G46" s="95"/>
+      <c r="H46" s="91"/>
+      <c r="I46" s="91"/>
+      <c r="J46" s="91"/>
       <c r="K46" s="34"/>
       <c r="L46" s="34"/>
       <c r="M46" s="34"/>
@@ -3443,41 +3461,41 @@
         <v>76</v>
       </c>
       <c r="B47" s="40"/>
-      <c r="C47" s="115" t="s">
+      <c r="C47" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="D47" s="115"/>
-      <c r="E47" s="115"/>
-      <c r="F47" s="115"/>
-      <c r="G47" s="115"/>
-      <c r="H47" s="88"/>
-      <c r="I47" s="88"/>
-      <c r="J47" s="88"/>
+      <c r="D47" s="95"/>
+      <c r="E47" s="95"/>
+      <c r="F47" s="95"/>
+      <c r="G47" s="95"/>
+      <c r="H47" s="91"/>
+      <c r="I47" s="91"/>
+      <c r="J47" s="91"/>
       <c r="K47" s="34"/>
       <c r="L47" s="34"/>
       <c r="M47" s="34"/>
     </row>
     <row r="48" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H48" s="88"/>
-      <c r="I48" s="88"/>
-      <c r="J48" s="88"/>
+      <c r="H48" s="91"/>
+      <c r="I48" s="91"/>
+      <c r="J48" s="91"/>
       <c r="K48" s="34"/>
       <c r="L48" s="34"/>
       <c r="M48" s="34"/>
     </row>
     <row r="49" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="116" t="s">
+      <c r="A49" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="B49" s="116"/>
-      <c r="C49" s="116"/>
-      <c r="D49" s="116"/>
-      <c r="E49" s="116"/>
-      <c r="F49" s="116"/>
-      <c r="G49" s="116"/>
-      <c r="H49" s="88"/>
-      <c r="I49" s="88"/>
-      <c r="J49" s="88"/>
+      <c r="B49" s="96"/>
+      <c r="C49" s="96"/>
+      <c r="D49" s="96"/>
+      <c r="E49" s="96"/>
+      <c r="F49" s="96"/>
+      <c r="G49" s="96"/>
+      <c r="H49" s="91"/>
+      <c r="I49" s="91"/>
+      <c r="J49" s="91"/>
       <c r="K49" s="34"/>
       <c r="L49" s="34"/>
       <c r="M49" s="34"/>
@@ -3489,16 +3507,16 @@
       <c r="B50" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="C50" s="117" t="s">
+      <c r="C50" s="97" t="s">
         <v>80</v>
       </c>
-      <c r="D50" s="117"/>
-      <c r="E50" s="117"/>
-      <c r="F50" s="117"/>
-      <c r="G50" s="117"/>
-      <c r="H50" s="88"/>
-      <c r="I50" s="88"/>
-      <c r="J50" s="88"/>
+      <c r="D50" s="97"/>
+      <c r="E50" s="97"/>
+      <c r="F50" s="97"/>
+      <c r="G50" s="97"/>
+      <c r="H50" s="91"/>
+      <c r="I50" s="91"/>
+      <c r="J50" s="91"/>
       <c r="K50" s="34"/>
       <c r="L50" s="34"/>
       <c r="M50" s="34"/>
@@ -3511,25 +3529,25 @@
       <c r="B51" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C51" s="114" t="s">
+      <c r="C51" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="D51" s="114"/>
-      <c r="E51" s="114"/>
-      <c r="F51" s="114"/>
-      <c r="G51" s="114"/>
-      <c r="H51" s="88"/>
-      <c r="I51" s="88"/>
-      <c r="J51" s="88"/>
+      <c r="D51" s="94"/>
+      <c r="E51" s="94"/>
+      <c r="F51" s="94"/>
+      <c r="G51" s="94"/>
+      <c r="H51" s="91"/>
+      <c r="I51" s="91"/>
+      <c r="J51" s="91"/>
       <c r="K51" s="34"/>
       <c r="L51" s="34"/>
       <c r="M51" s="34"/>
       <c r="N51" s="20"/>
     </row>
     <row r="52" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H52" s="88"/>
-      <c r="I52" s="88"/>
-      <c r="J52" s="88"/>
+      <c r="H52" s="91"/>
+      <c r="I52" s="91"/>
+      <c r="J52" s="91"/>
       <c r="K52" s="34"/>
       <c r="L52" s="34"/>
       <c r="M52" s="34"/>
@@ -3539,19 +3557,19 @@
       <c r="A53" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="B53" s="108" t="s">
+      <c r="B53" s="87" t="s">
         <v>462</v>
       </c>
-      <c r="C53" s="108"/>
-      <c r="D53" s="108"/>
-      <c r="E53" s="108"/>
-      <c r="F53" s="109" t="s">
+      <c r="C53" s="87"/>
+      <c r="D53" s="87"/>
+      <c r="E53" s="87"/>
+      <c r="F53" s="88" t="s">
         <v>85</v>
       </c>
-      <c r="G53" s="109"/>
-      <c r="H53" s="109"/>
-      <c r="I53" s="109"/>
-      <c r="J53" s="109"/>
+      <c r="G53" s="88"/>
+      <c r="H53" s="88"/>
+      <c r="I53" s="88"/>
+      <c r="J53" s="88"/>
       <c r="K53" s="44"/>
       <c r="L53" s="44"/>
       <c r="M53" s="44"/>
@@ -3563,28 +3581,28 @@
       <c r="C54" s="20"/>
       <c r="D54" s="20"/>
       <c r="E54" s="20"/>
-      <c r="F54" s="109"/>
-      <c r="G54" s="109"/>
-      <c r="H54" s="109"/>
-      <c r="I54" s="109"/>
-      <c r="J54" s="109"/>
+      <c r="F54" s="88"/>
+      <c r="G54" s="88"/>
+      <c r="H54" s="88"/>
+      <c r="I54" s="88"/>
+      <c r="J54" s="88"/>
       <c r="K54" s="44"/>
       <c r="L54" s="44"/>
       <c r="M54" s="44"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="F55" s="109"/>
-      <c r="G55" s="109"/>
-      <c r="H55" s="109"/>
-      <c r="I55" s="109"/>
-      <c r="J55" s="109"/>
+      <c r="F55" s="88"/>
+      <c r="G55" s="88"/>
+      <c r="H55" s="88"/>
+      <c r="I55" s="88"/>
+      <c r="J55" s="88"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="F56" s="109"/>
-      <c r="G56" s="109"/>
-      <c r="H56" s="109"/>
-      <c r="I56" s="109"/>
-      <c r="J56" s="109"/>
+      <c r="F56" s="88"/>
+      <c r="G56" s="88"/>
+      <c r="H56" s="88"/>
+      <c r="I56" s="88"/>
+      <c r="J56" s="88"/>
       <c r="N56" s="20"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
@@ -3702,14 +3720,14 @@
     <row r="64" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="20"/>
       <c r="B64" s="20"/>
-      <c r="C64" s="110"/>
-      <c r="D64" s="110"/>
-      <c r="E64" s="110"/>
-      <c r="F64" s="110"/>
-      <c r="G64" s="110"/>
-      <c r="H64" s="110"/>
-      <c r="I64" s="110"/>
-      <c r="J64" s="110"/>
+      <c r="C64" s="89"/>
+      <c r="D64" s="89"/>
+      <c r="E64" s="89"/>
+      <c r="F64" s="89"/>
+      <c r="G64" s="89"/>
+      <c r="H64" s="89"/>
+      <c r="I64" s="89"/>
+      <c r="J64" s="89"/>
       <c r="K64" s="20"/>
       <c r="L64" s="20"/>
       <c r="M64" s="20"/>
@@ -3771,14 +3789,14 @@
       <c r="N68" s="20"/>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C69" s="110"/>
-      <c r="D69" s="110"/>
-      <c r="E69" s="110"/>
-      <c r="F69" s="110"/>
-      <c r="G69" s="110"/>
-      <c r="H69" s="110"/>
-      <c r="I69" s="110"/>
-      <c r="J69" s="110"/>
+      <c r="C69" s="89"/>
+      <c r="D69" s="89"/>
+      <c r="E69" s="89"/>
+      <c r="F69" s="89"/>
+      <c r="G69" s="89"/>
+      <c r="H69" s="89"/>
+      <c r="I69" s="89"/>
+      <c r="J69" s="89"/>
       <c r="K69" s="20"/>
       <c r="L69" s="20"/>
       <c r="M69" s="20"/>
@@ -5326,6 +5344,37 @@
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="H27:H33"/>
+    <mergeCell ref="I27:I33"/>
+    <mergeCell ref="J27:J33"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="A34:J34"/>
+    <mergeCell ref="A35:J35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:J37"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:J39"/>
     <mergeCell ref="B53:E53"/>
     <mergeCell ref="F53:J56"/>
     <mergeCell ref="C64:J64"/>
@@ -5340,37 +5389,6 @@
     <mergeCell ref="A49:G49"/>
     <mergeCell ref="C50:G50"/>
     <mergeCell ref="C51:G51"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="E38:J38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="A34:J34"/>
-    <mergeCell ref="A35:J35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:J37"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="H27:H33"/>
-    <mergeCell ref="I27:I33"/>
-    <mergeCell ref="J27:J33"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="E12:E15"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B40 B45" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>

<commit_message>
Just do it cunt.
</commit_message>
<xml_diff>
--- a/Macro_Chartist/Control.xlsx
+++ b/Macro_Chartist/Control.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesbishop/Documents/Python/Bootleg_Macro/Macro_Chartist/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\Code\Bootleg_Macro\Macro_Chartist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F91C3D-3EBC-EA44-B9A0-D96421F5252D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE4F5C5-AD9B-433D-B115-70DE24195D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter_Input" sheetId="1" r:id="rId1"/>
@@ -1620,7 +1620,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2587,31 +2587,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ209"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="31.1640625" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1"/>
     <col min="4" max="4" width="37" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
     <col min="7" max="8" width="44" customWidth="1"/>
-    <col min="9" max="9" width="22.6640625" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" customWidth="1"/>
-    <col min="15" max="15" width="20.33203125" customWidth="1"/>
-    <col min="16" max="16" width="21.33203125" customWidth="1"/>
-    <col min="17" max="17" width="16.83203125" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" customWidth="1"/>
+    <col min="16" max="16" width="21.28515625" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="18" customHeight="1">
+    <row r="1" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="18" customHeight="1">
+    <row r="2" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="18" customHeight="1">
+    <row r="3" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="18" customHeight="1">
+    <row r="4" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="18" customHeight="1">
+    <row r="5" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="J5" s="14"/>
     </row>
-    <row r="6" spans="1:36" ht="18" customHeight="1">
+    <row r="6" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -2789,7 +2789,7 @@
       </c>
       <c r="J6" s="14"/>
     </row>
-    <row r="7" spans="1:36" ht="18" customHeight="1">
+    <row r="7" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -2803,7 +2803,7 @@
       <c r="I7" s="11"/>
       <c r="J7" s="14"/>
     </row>
-    <row r="8" spans="1:36" ht="18" customHeight="1">
+    <row r="8" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -2817,7 +2817,7 @@
       <c r="I8" s="16"/>
       <c r="J8" s="14"/>
     </row>
-    <row r="9" spans="1:36" ht="18" customHeight="1">
+    <row r="9" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -2831,7 +2831,7 @@
       <c r="I9" s="16"/>
       <c r="J9" s="14"/>
     </row>
-    <row r="10" spans="1:36" ht="18" customHeight="1">
+    <row r="10" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>9</v>
       </c>
@@ -2845,7 +2845,7 @@
       <c r="I10" s="16"/>
       <c r="J10" s="14"/>
     </row>
-    <row r="11" spans="1:36" ht="18" customHeight="1">
+    <row r="11" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -2859,7 +2859,7 @@
       <c r="I11" s="16"/>
       <c r="J11" s="14"/>
     </row>
-    <row r="12" spans="1:36" ht="18" customHeight="1">
+    <row r="12" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="87" t="s">
         <v>27</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:36" ht="18" customHeight="1">
+    <row r="13" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="87"/>
       <c r="B13" s="88"/>
       <c r="C13" s="89"/>
@@ -2903,7 +2903,7 @@
       <c r="I13" s="91"/>
       <c r="J13" s="88"/>
     </row>
-    <row r="14" spans="1:36" ht="18" customHeight="1">
+    <row r="14" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="87"/>
       <c r="B14" s="88"/>
       <c r="C14" s="89"/>
@@ -2915,7 +2915,7 @@
       <c r="I14" s="91"/>
       <c r="J14" s="88"/>
     </row>
-    <row r="15" spans="1:36" ht="25.5" customHeight="1">
+    <row r="15" spans="1:36" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="87"/>
       <c r="B15" s="88"/>
       <c r="C15" s="89"/>
@@ -2927,7 +2927,7 @@
       <c r="I15" s="91"/>
       <c r="J15" s="88"/>
     </row>
-    <row r="16" spans="1:36" ht="21" customHeight="1">
+    <row r="16" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>37</v>
       </c>
@@ -2978,16 +2978,12 @@
       <c r="AI16" s="20"/>
       <c r="AJ16" s="20"/>
     </row>
-    <row r="17" spans="1:36" ht="15.75" customHeight="1">
+    <row r="17" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
         <v>11</v>
       </c>
-      <c r="B17" s="22">
-        <v>19.5</v>
-      </c>
-      <c r="C17" s="22">
-        <v>-4.8</v>
-      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="23" t="s">
         <v>477</v>
       </c>
@@ -3017,7 +3013,7 @@
       <c r="AI17" s="20"/>
       <c r="AJ17" s="20"/>
     </row>
-    <row r="18" spans="1:36" ht="15.75" customHeight="1">
+    <row r="18" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21">
         <v>12</v>
       </c>
@@ -3050,7 +3046,7 @@
       <c r="AI18" s="20"/>
       <c r="AJ18" s="20"/>
     </row>
-    <row r="19" spans="1:36" ht="15.75" customHeight="1">
+    <row r="19" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="21">
         <v>13</v>
       </c>
@@ -3064,7 +3060,7 @@
       <c r="I19" s="25"/>
       <c r="J19" s="25"/>
     </row>
-    <row r="20" spans="1:36" ht="15.75" customHeight="1">
+    <row r="20" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21">
         <v>14</v>
       </c>
@@ -3078,16 +3074,12 @@
       <c r="I20" s="25"/>
       <c r="J20" s="25"/>
     </row>
-    <row r="21" spans="1:36" ht="15.75" customHeight="1">
+    <row r="21" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21">
         <v>15</v>
       </c>
-      <c r="B21" s="26">
-        <v>9732</v>
-      </c>
-      <c r="C21" s="26">
-        <v>-83.6</v>
-      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="23" t="s">
         <v>477</v>
       </c>
@@ -3098,7 +3090,7 @@
       <c r="I21" s="25"/>
       <c r="J21" s="25"/>
     </row>
-    <row r="22" spans="1:36" ht="15.75" customHeight="1">
+    <row r="22" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21">
         <v>16</v>
       </c>
@@ -3112,7 +3104,7 @@
       <c r="I22" s="25"/>
       <c r="J22" s="25"/>
     </row>
-    <row r="23" spans="1:36" ht="15.75" customHeight="1">
+    <row r="23" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21">
         <v>17</v>
       </c>
@@ -3126,7 +3118,7 @@
       <c r="I23" s="25"/>
       <c r="J23" s="25"/>
     </row>
-    <row r="24" spans="1:36" ht="15.75" customHeight="1">
+    <row r="24" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21">
         <v>18</v>
       </c>
@@ -3140,7 +3132,7 @@
       <c r="I24" s="25"/>
       <c r="J24" s="25"/>
     </row>
-    <row r="25" spans="1:36" ht="15.75" customHeight="1">
+    <row r="25" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21">
         <v>19</v>
       </c>
@@ -3154,7 +3146,7 @@
       <c r="I25" s="25"/>
       <c r="J25" s="25"/>
     </row>
-    <row r="26" spans="1:36" ht="15.75" customHeight="1">
+    <row r="26" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21">
         <v>20</v>
       </c>
@@ -3168,7 +3160,7 @@
       <c r="I26" s="25"/>
       <c r="J26" s="25"/>
     </row>
-    <row r="27" spans="1:36" ht="15.75" customHeight="1">
+    <row r="27" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="96" t="s">
         <v>47</v>
       </c>
@@ -3200,7 +3192,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:36" ht="15.75" customHeight="1">
+    <row r="28" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="96"/>
       <c r="B28" s="97"/>
       <c r="C28" s="97"/>
@@ -3212,7 +3204,7 @@
       <c r="I28" s="91"/>
       <c r="J28" s="91"/>
     </row>
-    <row r="29" spans="1:36" ht="15.75" customHeight="1">
+    <row r="29" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="96"/>
       <c r="B29" s="97"/>
       <c r="C29" s="97"/>
@@ -3224,7 +3216,7 @@
       <c r="I29" s="91"/>
       <c r="J29" s="91"/>
     </row>
-    <row r="30" spans="1:36" ht="15.75" customHeight="1">
+    <row r="30" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="96"/>
       <c r="B30" s="97"/>
       <c r="C30" s="97"/>
@@ -3236,7 +3228,7 @@
       <c r="I30" s="91"/>
       <c r="J30" s="91"/>
     </row>
-    <row r="31" spans="1:36" ht="15.75" customHeight="1">
+    <row r="31" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="96"/>
       <c r="B31" s="97"/>
       <c r="C31" s="97"/>
@@ -3248,7 +3240,7 @@
       <c r="I31" s="91"/>
       <c r="J31" s="91"/>
     </row>
-    <row r="32" spans="1:36" ht="15.75" customHeight="1">
+    <row r="32" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="96"/>
       <c r="B32" s="97"/>
       <c r="C32" s="97"/>
@@ -3260,7 +3252,7 @@
       <c r="I32" s="91"/>
       <c r="J32" s="91"/>
     </row>
-    <row r="33" spans="1:13" ht="22.5" customHeight="1">
+    <row r="33" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="95" t="s">
         <v>56</v>
       </c>
@@ -3274,7 +3266,7 @@
       <c r="I33" s="91"/>
       <c r="J33" s="91"/>
     </row>
-    <row r="34" spans="1:13" ht="22.5" customHeight="1">
+    <row r="34" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="98"/>
       <c r="B34" s="98"/>
       <c r="C34" s="98"/>
@@ -3286,7 +3278,7 @@
       <c r="I34" s="98"/>
       <c r="J34" s="98"/>
     </row>
-    <row r="35" spans="1:13" ht="22.5" customHeight="1">
+    <row r="35" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="99" t="s">
         <v>57</v>
       </c>
@@ -3300,7 +3292,7 @@
       <c r="I35" s="99"/>
       <c r="J35" s="99"/>
     </row>
-    <row r="36" spans="1:13" ht="18.75" customHeight="1">
+    <row r="36" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
         <v>58</v>
       </c>
@@ -3318,7 +3310,7 @@
       <c r="I36" s="101"/>
       <c r="J36" s="101"/>
     </row>
-    <row r="37" spans="1:13" ht="16">
+    <row r="37" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="30" t="s">
         <v>60</v>
       </c>
@@ -3336,7 +3328,7 @@
       <c r="K37" s="20"/>
       <c r="L37" s="20"/>
     </row>
-    <row r="38" spans="1:13" ht="16">
+    <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="32" t="s">
         <v>62</v>
       </c>
@@ -3354,7 +3346,7 @@
       <c r="K38" s="33"/>
       <c r="L38" s="33"/>
     </row>
-    <row r="39" spans="1:13" ht="19.5" customHeight="1">
+    <row r="39" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="30" t="s">
         <v>64</v>
       </c>
@@ -3377,7 +3369,7 @@
       <c r="L39" s="34"/>
       <c r="M39" s="34"/>
     </row>
-    <row r="40" spans="1:13" ht="15" customHeight="1">
+    <row r="40" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="35" t="s">
         <v>67</v>
       </c>
@@ -3400,7 +3392,7 @@
       <c r="L40" s="34"/>
       <c r="M40" s="34"/>
     </row>
-    <row r="41" spans="1:13" ht="12.75" customHeight="1">
+    <row r="41" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="112"/>
       <c r="B41" s="112"/>
       <c r="C41" s="112"/>
@@ -3415,7 +3407,7 @@
       <c r="L41" s="34"/>
       <c r="M41" s="34"/>
     </row>
-    <row r="42" spans="1:13" ht="15.75" customHeight="1">
+    <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="112"/>
       <c r="B42" s="112"/>
       <c r="C42" s="112"/>
@@ -3430,7 +3422,7 @@
       <c r="L42" s="34"/>
       <c r="M42" s="34"/>
     </row>
-    <row r="43" spans="1:13" ht="12.75" customHeight="1">
+    <row r="43" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="112"/>
       <c r="B43" s="112"/>
       <c r="C43" s="112"/>
@@ -3445,7 +3437,7 @@
       <c r="L43" s="34"/>
       <c r="M43" s="34"/>
     </row>
-    <row r="44" spans="1:13" ht="18">
+    <row r="44" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="113" t="s">
         <v>70</v>
       </c>
@@ -3462,7 +3454,7 @@
       <c r="L44" s="34"/>
       <c r="M44" s="34"/>
     </row>
-    <row r="45" spans="1:13" ht="16">
+    <row r="45" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="35" t="s">
         <v>71</v>
       </c>
@@ -3483,7 +3475,7 @@
       <c r="L45" s="34"/>
       <c r="M45" s="34"/>
     </row>
-    <row r="46" spans="1:13" ht="16">
+    <row r="46" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="39" t="s">
         <v>73</v>
       </c>
@@ -3502,7 +3494,7 @@
       <c r="L46" s="34"/>
       <c r="M46" s="34"/>
     </row>
-    <row r="47" spans="1:13" ht="16">
+    <row r="47" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="39" t="s">
         <v>75</v>
       </c>
@@ -3521,7 +3513,7 @@
       <c r="L47" s="34"/>
       <c r="M47" s="34"/>
     </row>
-    <row r="48" spans="1:13" ht="12.75" customHeight="1">
+    <row r="48" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H48" s="88"/>
       <c r="I48" s="88"/>
       <c r="J48" s="88"/>
@@ -3529,7 +3521,7 @@
       <c r="L48" s="34"/>
       <c r="M48" s="34"/>
     </row>
-    <row r="49" spans="1:14" ht="24.75" customHeight="1">
+    <row r="49" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="116" t="s">
         <v>77</v>
       </c>
@@ -3546,7 +3538,7 @@
       <c r="L49" s="34"/>
       <c r="M49" s="34"/>
     </row>
-    <row r="50" spans="1:14" ht="16">
+    <row r="50" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="41" t="s">
         <v>78</v>
       </c>
@@ -3568,7 +3560,7 @@
       <c r="M50" s="34"/>
       <c r="N50" s="20"/>
     </row>
-    <row r="51" spans="1:14" ht="18" customHeight="1">
+    <row r="51" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="41" t="s">
         <v>80</v>
       </c>
@@ -3590,7 +3582,7 @@
       <c r="M51" s="34"/>
       <c r="N51" s="20"/>
     </row>
-    <row r="52" spans="1:14" ht="12.75" customHeight="1">
+    <row r="52" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H52" s="88"/>
       <c r="I52" s="88"/>
       <c r="J52" s="88"/>
@@ -3599,7 +3591,7 @@
       <c r="M52" s="34"/>
       <c r="N52" s="20"/>
     </row>
-    <row r="53" spans="1:14" ht="19.5" customHeight="1">
+    <row r="53" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="43" t="s">
         <v>82</v>
       </c>
@@ -3621,7 +3613,7 @@
       <c r="M53" s="44"/>
       <c r="N53" s="20"/>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="20"/>
       <c r="B54" s="20"/>
       <c r="C54" s="20"/>
@@ -3636,14 +3628,14 @@
       <c r="L54" s="44"/>
       <c r="M54" s="44"/>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F55" s="109"/>
       <c r="G55" s="109"/>
       <c r="H55" s="109"/>
       <c r="I55" s="109"/>
       <c r="J55" s="109"/>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F56" s="109"/>
       <c r="G56" s="109"/>
       <c r="H56" s="109"/>
@@ -3651,7 +3643,7 @@
       <c r="J56" s="109"/>
       <c r="N56" s="20"/>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="20"/>
       <c r="B57" s="20"/>
       <c r="C57" s="20"/>
@@ -3667,7 +3659,7 @@
       <c r="M57" s="20"/>
       <c r="N57" s="20"/>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="20"/>
       <c r="B58" s="20"/>
       <c r="C58" s="20"/>
@@ -3683,7 +3675,7 @@
       <c r="M58" s="20"/>
       <c r="N58" s="20"/>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="20"/>
       <c r="B59" s="20"/>
       <c r="C59" s="20"/>
@@ -3699,7 +3691,7 @@
       <c r="M59" s="20"/>
       <c r="N59" s="20"/>
     </row>
-    <row r="60" spans="1:14" ht="12.75" customHeight="1">
+    <row r="60" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="20"/>
       <c r="B60" s="20"/>
       <c r="C60" s="46"/>
@@ -3715,7 +3707,7 @@
       <c r="M60" s="20"/>
       <c r="N60" s="20"/>
     </row>
-    <row r="61" spans="1:14" ht="12.75" customHeight="1">
+    <row r="61" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="20"/>
       <c r="B61" s="20"/>
       <c r="C61" s="46"/>
@@ -3731,7 +3723,7 @@
       <c r="M61" s="20"/>
       <c r="N61" s="20"/>
     </row>
-    <row r="62" spans="1:14" ht="12.75" customHeight="1">
+    <row r="62" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="20"/>
       <c r="B62" s="20"/>
       <c r="C62" s="46"/>
@@ -3747,7 +3739,7 @@
       <c r="M62" s="20"/>
       <c r="N62" s="20"/>
     </row>
-    <row r="63" spans="1:14" ht="12.75" customHeight="1">
+    <row r="63" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="20"/>
       <c r="B63" s="20"/>
       <c r="C63" s="46"/>
@@ -3763,7 +3755,7 @@
       <c r="M63" s="20"/>
       <c r="N63" s="20"/>
     </row>
-    <row r="64" spans="1:14" ht="12.75" customHeight="1">
+    <row r="64" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="20"/>
       <c r="B64" s="20"/>
       <c r="C64" s="110"/>
@@ -3779,7 +3771,7 @@
       <c r="M64" s="20"/>
       <c r="N64" s="20"/>
     </row>
-    <row r="65" spans="1:14" ht="12.75" customHeight="1">
+    <row r="65" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="20"/>
       <c r="B65" s="20"/>
       <c r="C65" s="46"/>
@@ -3795,7 +3787,7 @@
       <c r="M65" s="20"/>
       <c r="N65" s="20"/>
     </row>
-    <row r="66" spans="1:14" ht="12.75" customHeight="1">
+    <row r="66" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C66" s="46"/>
       <c r="D66" s="46"/>
       <c r="E66" s="46"/>
@@ -3809,7 +3801,7 @@
       <c r="M66" s="20"/>
       <c r="N66" s="20"/>
     </row>
-    <row r="67" spans="1:14" ht="12.75" customHeight="1">
+    <row r="67" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C67" s="46"/>
       <c r="D67" s="46"/>
       <c r="E67" s="46"/>
@@ -3823,7 +3815,7 @@
       <c r="M67" s="20"/>
       <c r="N67" s="20"/>
     </row>
-    <row r="68" spans="1:14">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F68" s="20"/>
       <c r="G68" s="20"/>
       <c r="H68" s="20"/>
@@ -3834,7 +3826,7 @@
       <c r="M68" s="20"/>
       <c r="N68" s="20"/>
     </row>
-    <row r="69" spans="1:14">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C69" s="110"/>
       <c r="D69" s="110"/>
       <c r="E69" s="110"/>
@@ -3848,7 +3840,7 @@
       <c r="M69" s="20"/>
       <c r="N69" s="20"/>
     </row>
-    <row r="70" spans="1:14">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F70" s="20"/>
       <c r="G70" s="20"/>
       <c r="H70" s="20"/>
@@ -3859,7 +3851,7 @@
       <c r="M70" s="20"/>
       <c r="N70" s="20"/>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F71" s="20"/>
       <c r="G71" s="20"/>
       <c r="H71" s="20"/>
@@ -3870,7 +3862,7 @@
       <c r="M71" s="20"/>
       <c r="N71" s="20"/>
     </row>
-    <row r="72" spans="1:14">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F72" s="20"/>
       <c r="G72" s="20"/>
       <c r="H72" s="20"/>
@@ -3881,7 +3873,7 @@
       <c r="M72" s="20"/>
       <c r="N72" s="20"/>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F73" s="20"/>
       <c r="G73" s="20"/>
       <c r="H73" s="20"/>
@@ -3892,7 +3884,7 @@
       <c r="M73" s="20"/>
       <c r="N73" s="20"/>
     </row>
-    <row r="74" spans="1:14">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F74" s="20"/>
       <c r="G74" s="20"/>
       <c r="H74" s="20"/>
@@ -3903,7 +3895,7 @@
       <c r="M74" s="20"/>
       <c r="N74" s="20"/>
     </row>
-    <row r="75" spans="1:14">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F75" s="20"/>
       <c r="G75" s="20"/>
       <c r="H75" s="20"/>
@@ -3914,7 +3906,7 @@
       <c r="M75" s="20"/>
       <c r="N75" s="20"/>
     </row>
-    <row r="76" spans="1:14">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F76" s="20"/>
       <c r="G76" s="20"/>
       <c r="H76" s="20"/>
@@ -3925,7 +3917,7 @@
       <c r="M76" s="20"/>
       <c r="N76" s="20"/>
     </row>
-    <row r="77" spans="1:14">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F77" s="20"/>
       <c r="G77" s="20"/>
       <c r="H77" s="20"/>
@@ -3936,7 +3928,7 @@
       <c r="M77" s="20"/>
       <c r="N77" s="20"/>
     </row>
-    <row r="78" spans="1:14">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F78" s="20"/>
       <c r="G78" s="20"/>
       <c r="H78" s="20"/>
@@ -3947,7 +3939,7 @@
       <c r="M78" s="20"/>
       <c r="N78" s="20"/>
     </row>
-    <row r="79" spans="1:14">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F79" s="20"/>
       <c r="G79" s="20"/>
       <c r="H79" s="20"/>
@@ -3958,7 +3950,7 @@
       <c r="M79" s="20"/>
       <c r="N79" s="20"/>
     </row>
-    <row r="80" spans="1:14">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F80" s="20"/>
       <c r="G80" s="20"/>
       <c r="H80" s="20"/>
@@ -3969,7 +3961,7 @@
       <c r="M80" s="20"/>
       <c r="N80" s="20"/>
     </row>
-    <row r="81" spans="6:14">
+    <row r="81" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F81" s="20"/>
       <c r="G81" s="20"/>
       <c r="H81" s="20"/>
@@ -3980,7 +3972,7 @@
       <c r="M81" s="20"/>
       <c r="N81" s="20"/>
     </row>
-    <row r="82" spans="6:14">
+    <row r="82" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F82" s="20"/>
       <c r="G82" s="20"/>
       <c r="H82" s="20"/>
@@ -3991,7 +3983,7 @@
       <c r="M82" s="20"/>
       <c r="N82" s="20"/>
     </row>
-    <row r="83" spans="6:14">
+    <row r="83" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F83" s="20"/>
       <c r="G83" s="20"/>
       <c r="H83" s="20"/>
@@ -4002,7 +3994,7 @@
       <c r="M83" s="20"/>
       <c r="N83" s="20"/>
     </row>
-    <row r="84" spans="6:14">
+    <row r="84" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F84" s="20"/>
       <c r="G84" s="20"/>
       <c r="H84" s="20"/>
@@ -4013,7 +4005,7 @@
       <c r="M84" s="20"/>
       <c r="N84" s="20"/>
     </row>
-    <row r="85" spans="6:14">
+    <row r="85" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F85" s="20"/>
       <c r="G85" s="20"/>
       <c r="H85" s="20"/>
@@ -4024,7 +4016,7 @@
       <c r="M85" s="20"/>
       <c r="N85" s="20"/>
     </row>
-    <row r="86" spans="6:14">
+    <row r="86" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F86" s="20"/>
       <c r="G86" s="20"/>
       <c r="H86" s="20"/>
@@ -4035,7 +4027,7 @@
       <c r="M86" s="20"/>
       <c r="N86" s="20"/>
     </row>
-    <row r="87" spans="6:14">
+    <row r="87" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F87" s="20"/>
       <c r="G87" s="20"/>
       <c r="H87" s="20"/>
@@ -4046,7 +4038,7 @@
       <c r="M87" s="20"/>
       <c r="N87" s="20"/>
     </row>
-    <row r="88" spans="6:14">
+    <row r="88" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F88" s="20"/>
       <c r="G88" s="20"/>
       <c r="H88" s="20"/>
@@ -4057,7 +4049,7 @@
       <c r="M88" s="20"/>
       <c r="N88" s="20"/>
     </row>
-    <row r="89" spans="6:14">
+    <row r="89" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F89" s="20"/>
       <c r="G89" s="20"/>
       <c r="H89" s="20"/>
@@ -4068,7 +4060,7 @@
       <c r="M89" s="20"/>
       <c r="N89" s="20"/>
     </row>
-    <row r="90" spans="6:14">
+    <row r="90" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F90" s="20"/>
       <c r="G90" s="20"/>
       <c r="H90" s="20"/>
@@ -4079,7 +4071,7 @@
       <c r="M90" s="20"/>
       <c r="N90" s="20"/>
     </row>
-    <row r="91" spans="6:14">
+    <row r="91" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F91" s="20"/>
       <c r="G91" s="20"/>
       <c r="H91" s="20"/>
@@ -4090,7 +4082,7 @@
       <c r="M91" s="20"/>
       <c r="N91" s="20"/>
     </row>
-    <row r="92" spans="6:14">
+    <row r="92" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F92" s="20"/>
       <c r="G92" s="20"/>
       <c r="H92" s="20"/>
@@ -4101,7 +4093,7 @@
       <c r="M92" s="20"/>
       <c r="N92" s="20"/>
     </row>
-    <row r="93" spans="6:14">
+    <row r="93" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F93" s="20"/>
       <c r="G93" s="20"/>
       <c r="H93" s="20"/>
@@ -4112,7 +4104,7 @@
       <c r="M93" s="20"/>
       <c r="N93" s="20"/>
     </row>
-    <row r="94" spans="6:14">
+    <row r="94" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F94" s="20"/>
       <c r="G94" s="20"/>
       <c r="H94" s="20"/>
@@ -4123,7 +4115,7 @@
       <c r="M94" s="20"/>
       <c r="N94" s="20"/>
     </row>
-    <row r="95" spans="6:14">
+    <row r="95" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F95" s="20"/>
       <c r="G95" s="20"/>
       <c r="H95" s="20"/>
@@ -4134,7 +4126,7 @@
       <c r="M95" s="20"/>
       <c r="N95" s="20"/>
     </row>
-    <row r="96" spans="6:14">
+    <row r="96" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F96" s="20"/>
       <c r="G96" s="20"/>
       <c r="H96" s="20"/>
@@ -4145,7 +4137,7 @@
       <c r="M96" s="20"/>
       <c r="N96" s="20"/>
     </row>
-    <row r="97" spans="6:14">
+    <row r="97" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F97" s="20"/>
       <c r="G97" s="20"/>
       <c r="H97" s="20"/>
@@ -4156,7 +4148,7 @@
       <c r="M97" s="20"/>
       <c r="N97" s="20"/>
     </row>
-    <row r="98" spans="6:14">
+    <row r="98" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F98" s="20"/>
       <c r="G98" s="20"/>
       <c r="H98" s="20"/>
@@ -4167,7 +4159,7 @@
       <c r="M98" s="20"/>
       <c r="N98" s="20"/>
     </row>
-    <row r="99" spans="6:14">
+    <row r="99" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F99" s="20"/>
       <c r="G99" s="20"/>
       <c r="H99" s="20"/>
@@ -4178,7 +4170,7 @@
       <c r="M99" s="20"/>
       <c r="N99" s="20"/>
     </row>
-    <row r="100" spans="6:14">
+    <row r="100" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F100" s="20"/>
       <c r="G100" s="20"/>
       <c r="H100" s="20"/>
@@ -4189,7 +4181,7 @@
       <c r="M100" s="20"/>
       <c r="N100" s="20"/>
     </row>
-    <row r="101" spans="6:14">
+    <row r="101" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F101" s="20"/>
       <c r="G101" s="20"/>
       <c r="H101" s="20"/>
@@ -4200,7 +4192,7 @@
       <c r="M101" s="20"/>
       <c r="N101" s="20"/>
     </row>
-    <row r="102" spans="6:14">
+    <row r="102" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F102" s="20"/>
       <c r="G102" s="20"/>
       <c r="H102" s="20"/>
@@ -4211,7 +4203,7 @@
       <c r="M102" s="20"/>
       <c r="N102" s="20"/>
     </row>
-    <row r="103" spans="6:14">
+    <row r="103" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F103" s="20"/>
       <c r="G103" s="20"/>
       <c r="H103" s="20"/>
@@ -4222,7 +4214,7 @@
       <c r="M103" s="20"/>
       <c r="N103" s="20"/>
     </row>
-    <row r="104" spans="6:14">
+    <row r="104" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F104" s="20"/>
       <c r="G104" s="20"/>
       <c r="H104" s="20"/>
@@ -4233,7 +4225,7 @@
       <c r="M104" s="20"/>
       <c r="N104" s="20"/>
     </row>
-    <row r="105" spans="6:14">
+    <row r="105" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F105" s="20"/>
       <c r="G105" s="20"/>
       <c r="H105" s="20"/>
@@ -4244,7 +4236,7 @@
       <c r="M105" s="20"/>
       <c r="N105" s="20"/>
     </row>
-    <row r="106" spans="6:14">
+    <row r="106" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F106" s="20"/>
       <c r="G106" s="20"/>
       <c r="H106" s="20"/>
@@ -4255,7 +4247,7 @@
       <c r="M106" s="20"/>
       <c r="N106" s="20"/>
     </row>
-    <row r="107" spans="6:14">
+    <row r="107" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F107" s="20"/>
       <c r="G107" s="20"/>
       <c r="H107" s="20"/>
@@ -4266,7 +4258,7 @@
       <c r="M107" s="20"/>
       <c r="N107" s="20"/>
     </row>
-    <row r="108" spans="6:14">
+    <row r="108" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F108" s="20"/>
       <c r="G108" s="20"/>
       <c r="H108" s="20"/>
@@ -4277,7 +4269,7 @@
       <c r="M108" s="20"/>
       <c r="N108" s="20"/>
     </row>
-    <row r="109" spans="6:14">
+    <row r="109" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F109" s="20"/>
       <c r="G109" s="20"/>
       <c r="H109" s="20"/>
@@ -4288,7 +4280,7 @@
       <c r="M109" s="20"/>
       <c r="N109" s="20"/>
     </row>
-    <row r="110" spans="6:14">
+    <row r="110" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F110" s="20"/>
       <c r="G110" s="20"/>
       <c r="H110" s="20"/>
@@ -4299,7 +4291,7 @@
       <c r="M110" s="20"/>
       <c r="N110" s="20"/>
     </row>
-    <row r="111" spans="6:14">
+    <row r="111" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F111" s="20"/>
       <c r="G111" s="20"/>
       <c r="H111" s="20"/>
@@ -4310,7 +4302,7 @@
       <c r="M111" s="20"/>
       <c r="N111" s="20"/>
     </row>
-    <row r="112" spans="6:14">
+    <row r="112" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F112" s="20"/>
       <c r="G112" s="20"/>
       <c r="H112" s="20"/>
@@ -4321,7 +4313,7 @@
       <c r="M112" s="20"/>
       <c r="N112" s="20"/>
     </row>
-    <row r="113" spans="6:14">
+    <row r="113" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F113" s="20"/>
       <c r="G113" s="20"/>
       <c r="H113" s="20"/>
@@ -4332,7 +4324,7 @@
       <c r="M113" s="20"/>
       <c r="N113" s="20"/>
     </row>
-    <row r="114" spans="6:14">
+    <row r="114" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F114" s="20"/>
       <c r="G114" s="20"/>
       <c r="H114" s="20"/>
@@ -4343,7 +4335,7 @@
       <c r="M114" s="20"/>
       <c r="N114" s="20"/>
     </row>
-    <row r="115" spans="6:14">
+    <row r="115" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F115" s="20"/>
       <c r="G115" s="20"/>
       <c r="H115" s="20"/>
@@ -4354,7 +4346,7 @@
       <c r="M115" s="20"/>
       <c r="N115" s="20"/>
     </row>
-    <row r="116" spans="6:14">
+    <row r="116" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F116" s="20"/>
       <c r="G116" s="20"/>
       <c r="H116" s="20"/>
@@ -4365,7 +4357,7 @@
       <c r="M116" s="20"/>
       <c r="N116" s="20"/>
     </row>
-    <row r="117" spans="6:14">
+    <row r="117" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F117" s="20"/>
       <c r="G117" s="20"/>
       <c r="H117" s="20"/>
@@ -4376,7 +4368,7 @@
       <c r="M117" s="20"/>
       <c r="N117" s="20"/>
     </row>
-    <row r="118" spans="6:14">
+    <row r="118" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F118" s="20"/>
       <c r="G118" s="20"/>
       <c r="H118" s="20"/>
@@ -4387,7 +4379,7 @@
       <c r="M118" s="20"/>
       <c r="N118" s="20"/>
     </row>
-    <row r="119" spans="6:14">
+    <row r="119" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F119" s="20"/>
       <c r="G119" s="20"/>
       <c r="H119" s="20"/>
@@ -4398,7 +4390,7 @@
       <c r="M119" s="20"/>
       <c r="N119" s="20"/>
     </row>
-    <row r="120" spans="6:14">
+    <row r="120" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F120" s="20"/>
       <c r="G120" s="20"/>
       <c r="H120" s="20"/>
@@ -4409,7 +4401,7 @@
       <c r="M120" s="20"/>
       <c r="N120" s="20"/>
     </row>
-    <row r="121" spans="6:14">
+    <row r="121" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F121" s="20"/>
       <c r="G121" s="20"/>
       <c r="H121" s="20"/>
@@ -4420,7 +4412,7 @@
       <c r="M121" s="20"/>
       <c r="N121" s="20"/>
     </row>
-    <row r="122" spans="6:14">
+    <row r="122" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F122" s="20"/>
       <c r="G122" s="20"/>
       <c r="H122" s="20"/>
@@ -4431,7 +4423,7 @@
       <c r="M122" s="20"/>
       <c r="N122" s="20"/>
     </row>
-    <row r="123" spans="6:14">
+    <row r="123" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F123" s="20"/>
       <c r="G123" s="20"/>
       <c r="H123" s="20"/>
@@ -4442,7 +4434,7 @@
       <c r="M123" s="20"/>
       <c r="N123" s="20"/>
     </row>
-    <row r="124" spans="6:14">
+    <row r="124" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F124" s="20"/>
       <c r="G124" s="20"/>
       <c r="H124" s="20"/>
@@ -4453,7 +4445,7 @@
       <c r="M124" s="20"/>
       <c r="N124" s="20"/>
     </row>
-    <row r="125" spans="6:14">
+    <row r="125" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F125" s="20"/>
       <c r="G125" s="20"/>
       <c r="H125" s="20"/>
@@ -4464,7 +4456,7 @@
       <c r="M125" s="20"/>
       <c r="N125" s="20"/>
     </row>
-    <row r="126" spans="6:14">
+    <row r="126" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F126" s="20"/>
       <c r="G126" s="20"/>
       <c r="H126" s="20"/>
@@ -4475,7 +4467,7 @@
       <c r="M126" s="20"/>
       <c r="N126" s="20"/>
     </row>
-    <row r="127" spans="6:14">
+    <row r="127" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F127" s="20"/>
       <c r="G127" s="20"/>
       <c r="H127" s="20"/>
@@ -4486,7 +4478,7 @@
       <c r="M127" s="20"/>
       <c r="N127" s="20"/>
     </row>
-    <row r="128" spans="6:14">
+    <row r="128" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F128" s="20"/>
       <c r="G128" s="20"/>
       <c r="H128" s="20"/>
@@ -4497,7 +4489,7 @@
       <c r="M128" s="20"/>
       <c r="N128" s="20"/>
     </row>
-    <row r="129" spans="6:14">
+    <row r="129" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F129" s="20"/>
       <c r="G129" s="20"/>
       <c r="H129" s="20"/>
@@ -4508,7 +4500,7 @@
       <c r="M129" s="20"/>
       <c r="N129" s="20"/>
     </row>
-    <row r="130" spans="6:14">
+    <row r="130" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F130" s="20"/>
       <c r="G130" s="20"/>
       <c r="H130" s="20"/>
@@ -4519,7 +4511,7 @@
       <c r="M130" s="20"/>
       <c r="N130" s="20"/>
     </row>
-    <row r="131" spans="6:14">
+    <row r="131" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F131" s="20"/>
       <c r="G131" s="20"/>
       <c r="H131" s="20"/>
@@ -4530,7 +4522,7 @@
       <c r="M131" s="20"/>
       <c r="N131" s="20"/>
     </row>
-    <row r="132" spans="6:14">
+    <row r="132" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F132" s="20"/>
       <c r="G132" s="20"/>
       <c r="H132" s="20"/>
@@ -4541,7 +4533,7 @@
       <c r="M132" s="20"/>
       <c r="N132" s="20"/>
     </row>
-    <row r="133" spans="6:14">
+    <row r="133" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F133" s="20"/>
       <c r="G133" s="20"/>
       <c r="H133" s="20"/>
@@ -4552,7 +4544,7 @@
       <c r="M133" s="20"/>
       <c r="N133" s="20"/>
     </row>
-    <row r="134" spans="6:14">
+    <row r="134" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F134" s="20"/>
       <c r="G134" s="20"/>
       <c r="H134" s="20"/>
@@ -4563,7 +4555,7 @@
       <c r="M134" s="20"/>
       <c r="N134" s="20"/>
     </row>
-    <row r="135" spans="6:14">
+    <row r="135" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F135" s="20"/>
       <c r="G135" s="20"/>
       <c r="H135" s="20"/>
@@ -4574,7 +4566,7 @@
       <c r="M135" s="20"/>
       <c r="N135" s="20"/>
     </row>
-    <row r="136" spans="6:14">
+    <row r="136" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F136" s="20"/>
       <c r="G136" s="20"/>
       <c r="H136" s="20"/>
@@ -4585,7 +4577,7 @@
       <c r="M136" s="20"/>
       <c r="N136" s="20"/>
     </row>
-    <row r="137" spans="6:14">
+    <row r="137" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F137" s="20"/>
       <c r="G137" s="20"/>
       <c r="H137" s="20"/>
@@ -4596,7 +4588,7 @@
       <c r="M137" s="20"/>
       <c r="N137" s="20"/>
     </row>
-    <row r="138" spans="6:14">
+    <row r="138" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F138" s="20"/>
       <c r="G138" s="20"/>
       <c r="H138" s="20"/>
@@ -4607,7 +4599,7 @@
       <c r="M138" s="20"/>
       <c r="N138" s="20"/>
     </row>
-    <row r="139" spans="6:14">
+    <row r="139" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F139" s="20"/>
       <c r="G139" s="20"/>
       <c r="H139" s="20"/>
@@ -4618,7 +4610,7 @@
       <c r="M139" s="20"/>
       <c r="N139" s="20"/>
     </row>
-    <row r="140" spans="6:14">
+    <row r="140" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F140" s="20"/>
       <c r="G140" s="20"/>
       <c r="H140" s="20"/>
@@ -4629,7 +4621,7 @@
       <c r="M140" s="20"/>
       <c r="N140" s="20"/>
     </row>
-    <row r="141" spans="6:14">
+    <row r="141" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F141" s="20"/>
       <c r="G141" s="20"/>
       <c r="H141" s="20"/>
@@ -4640,7 +4632,7 @@
       <c r="M141" s="20"/>
       <c r="N141" s="20"/>
     </row>
-    <row r="142" spans="6:14">
+    <row r="142" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F142" s="20"/>
       <c r="G142" s="20"/>
       <c r="H142" s="20"/>
@@ -4651,7 +4643,7 @@
       <c r="M142" s="20"/>
       <c r="N142" s="20"/>
     </row>
-    <row r="143" spans="6:14">
+    <row r="143" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F143" s="20"/>
       <c r="G143" s="20"/>
       <c r="H143" s="20"/>
@@ -4662,7 +4654,7 @@
       <c r="M143" s="20"/>
       <c r="N143" s="20"/>
     </row>
-    <row r="144" spans="6:14">
+    <row r="144" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F144" s="20"/>
       <c r="G144" s="20"/>
       <c r="H144" s="20"/>
@@ -4673,7 +4665,7 @@
       <c r="M144" s="20"/>
       <c r="N144" s="20"/>
     </row>
-    <row r="145" spans="6:14">
+    <row r="145" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F145" s="20"/>
       <c r="G145" s="20"/>
       <c r="H145" s="20"/>
@@ -4684,7 +4676,7 @@
       <c r="M145" s="20"/>
       <c r="N145" s="20"/>
     </row>
-    <row r="146" spans="6:14">
+    <row r="146" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F146" s="20"/>
       <c r="G146" s="20"/>
       <c r="H146" s="20"/>
@@ -4695,7 +4687,7 @@
       <c r="M146" s="20"/>
       <c r="N146" s="20"/>
     </row>
-    <row r="147" spans="6:14">
+    <row r="147" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F147" s="20"/>
       <c r="G147" s="20"/>
       <c r="H147" s="20"/>
@@ -4706,7 +4698,7 @@
       <c r="M147" s="20"/>
       <c r="N147" s="20"/>
     </row>
-    <row r="148" spans="6:14">
+    <row r="148" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F148" s="20"/>
       <c r="G148" s="20"/>
       <c r="H148" s="20"/>
@@ -4717,7 +4709,7 @@
       <c r="M148" s="20"/>
       <c r="N148" s="20"/>
     </row>
-    <row r="149" spans="6:14">
+    <row r="149" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F149" s="20"/>
       <c r="G149" s="20"/>
       <c r="H149" s="20"/>
@@ -4728,7 +4720,7 @@
       <c r="M149" s="20"/>
       <c r="N149" s="20"/>
     </row>
-    <row r="150" spans="6:14">
+    <row r="150" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F150" s="20"/>
       <c r="G150" s="20"/>
       <c r="H150" s="20"/>
@@ -4739,7 +4731,7 @@
       <c r="M150" s="20"/>
       <c r="N150" s="20"/>
     </row>
-    <row r="151" spans="6:14">
+    <row r="151" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F151" s="20"/>
       <c r="G151" s="20"/>
       <c r="H151" s="20"/>
@@ -4750,7 +4742,7 @@
       <c r="M151" s="20"/>
       <c r="N151" s="20"/>
     </row>
-    <row r="152" spans="6:14">
+    <row r="152" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F152" s="20"/>
       <c r="G152" s="20"/>
       <c r="H152" s="20"/>
@@ -4761,7 +4753,7 @@
       <c r="M152" s="20"/>
       <c r="N152" s="20"/>
     </row>
-    <row r="153" spans="6:14">
+    <row r="153" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F153" s="20"/>
       <c r="G153" s="20"/>
       <c r="H153" s="20"/>
@@ -4772,7 +4764,7 @@
       <c r="M153" s="20"/>
       <c r="N153" s="20"/>
     </row>
-    <row r="154" spans="6:14">
+    <row r="154" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F154" s="20"/>
       <c r="G154" s="20"/>
       <c r="H154" s="20"/>
@@ -4783,7 +4775,7 @@
       <c r="M154" s="20"/>
       <c r="N154" s="20"/>
     </row>
-    <row r="155" spans="6:14">
+    <row r="155" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F155" s="20"/>
       <c r="G155" s="20"/>
       <c r="H155" s="20"/>
@@ -4794,7 +4786,7 @@
       <c r="M155" s="20"/>
       <c r="N155" s="20"/>
     </row>
-    <row r="156" spans="6:14">
+    <row r="156" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F156" s="20"/>
       <c r="G156" s="20"/>
       <c r="H156" s="20"/>
@@ -4805,7 +4797,7 @@
       <c r="M156" s="20"/>
       <c r="N156" s="20"/>
     </row>
-    <row r="157" spans="6:14">
+    <row r="157" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F157" s="20"/>
       <c r="G157" s="20"/>
       <c r="H157" s="20"/>
@@ -4816,7 +4808,7 @@
       <c r="M157" s="20"/>
       <c r="N157" s="20"/>
     </row>
-    <row r="158" spans="6:14">
+    <row r="158" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F158" s="20"/>
       <c r="G158" s="20"/>
       <c r="H158" s="20"/>
@@ -4827,7 +4819,7 @@
       <c r="M158" s="20"/>
       <c r="N158" s="20"/>
     </row>
-    <row r="159" spans="6:14">
+    <row r="159" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F159" s="20"/>
       <c r="G159" s="20"/>
       <c r="H159" s="20"/>
@@ -4838,7 +4830,7 @@
       <c r="M159" s="20"/>
       <c r="N159" s="20"/>
     </row>
-    <row r="160" spans="6:14">
+    <row r="160" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F160" s="20"/>
       <c r="G160" s="20"/>
       <c r="H160" s="20"/>
@@ -4849,7 +4841,7 @@
       <c r="M160" s="20"/>
       <c r="N160" s="20"/>
     </row>
-    <row r="161" spans="6:14">
+    <row r="161" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F161" s="20"/>
       <c r="G161" s="20"/>
       <c r="H161" s="20"/>
@@ -4860,7 +4852,7 @@
       <c r="M161" s="20"/>
       <c r="N161" s="20"/>
     </row>
-    <row r="162" spans="6:14">
+    <row r="162" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F162" s="20"/>
       <c r="G162" s="20"/>
       <c r="H162" s="20"/>
@@ -4871,7 +4863,7 @@
       <c r="M162" s="20"/>
       <c r="N162" s="20"/>
     </row>
-    <row r="163" spans="6:14">
+    <row r="163" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F163" s="20"/>
       <c r="G163" s="20"/>
       <c r="H163" s="20"/>
@@ -4882,7 +4874,7 @@
       <c r="M163" s="20"/>
       <c r="N163" s="20"/>
     </row>
-    <row r="164" spans="6:14">
+    <row r="164" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F164" s="20"/>
       <c r="G164" s="20"/>
       <c r="H164" s="20"/>
@@ -4893,7 +4885,7 @@
       <c r="M164" s="20"/>
       <c r="N164" s="20"/>
     </row>
-    <row r="165" spans="6:14">
+    <row r="165" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F165" s="20"/>
       <c r="G165" s="20"/>
       <c r="H165" s="20"/>
@@ -4904,7 +4896,7 @@
       <c r="M165" s="20"/>
       <c r="N165" s="20"/>
     </row>
-    <row r="166" spans="6:14">
+    <row r="166" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F166" s="20"/>
       <c r="G166" s="20"/>
       <c r="H166" s="20"/>
@@ -4915,7 +4907,7 @@
       <c r="M166" s="20"/>
       <c r="N166" s="20"/>
     </row>
-    <row r="167" spans="6:14">
+    <row r="167" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F167" s="20"/>
       <c r="G167" s="20"/>
       <c r="H167" s="20"/>
@@ -4926,7 +4918,7 @@
       <c r="M167" s="20"/>
       <c r="N167" s="20"/>
     </row>
-    <row r="168" spans="6:14">
+    <row r="168" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F168" s="20"/>
       <c r="G168" s="20"/>
       <c r="H168" s="20"/>
@@ -4937,7 +4929,7 @@
       <c r="M168" s="20"/>
       <c r="N168" s="20"/>
     </row>
-    <row r="169" spans="6:14">
+    <row r="169" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F169" s="20"/>
       <c r="G169" s="20"/>
       <c r="H169" s="20"/>
@@ -4948,7 +4940,7 @@
       <c r="M169" s="20"/>
       <c r="N169" s="20"/>
     </row>
-    <row r="170" spans="6:14">
+    <row r="170" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F170" s="20"/>
       <c r="G170" s="20"/>
       <c r="H170" s="20"/>
@@ -4959,7 +4951,7 @@
       <c r="M170" s="20"/>
       <c r="N170" s="20"/>
     </row>
-    <row r="171" spans="6:14">
+    <row r="171" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F171" s="20"/>
       <c r="G171" s="20"/>
       <c r="H171" s="20"/>
@@ -4970,7 +4962,7 @@
       <c r="M171" s="20"/>
       <c r="N171" s="20"/>
     </row>
-    <row r="172" spans="6:14">
+    <row r="172" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F172" s="20"/>
       <c r="G172" s="20"/>
       <c r="H172" s="20"/>
@@ -4981,7 +4973,7 @@
       <c r="M172" s="20"/>
       <c r="N172" s="20"/>
     </row>
-    <row r="173" spans="6:14">
+    <row r="173" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F173" s="20"/>
       <c r="G173" s="20"/>
       <c r="H173" s="20"/>
@@ -4992,7 +4984,7 @@
       <c r="M173" s="20"/>
       <c r="N173" s="20"/>
     </row>
-    <row r="174" spans="6:14">
+    <row r="174" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F174" s="20"/>
       <c r="G174" s="20"/>
       <c r="H174" s="20"/>
@@ -5003,7 +4995,7 @@
       <c r="M174" s="20"/>
       <c r="N174" s="20"/>
     </row>
-    <row r="175" spans="6:14">
+    <row r="175" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F175" s="20"/>
       <c r="G175" s="20"/>
       <c r="H175" s="20"/>
@@ -5014,7 +5006,7 @@
       <c r="M175" s="20"/>
       <c r="N175" s="20"/>
     </row>
-    <row r="176" spans="6:14">
+    <row r="176" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F176" s="20"/>
       <c r="G176" s="20"/>
       <c r="H176" s="20"/>
@@ -5025,7 +5017,7 @@
       <c r="M176" s="20"/>
       <c r="N176" s="20"/>
     </row>
-    <row r="177" spans="6:14">
+    <row r="177" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F177" s="20"/>
       <c r="G177" s="20"/>
       <c r="H177" s="20"/>
@@ -5036,7 +5028,7 @@
       <c r="M177" s="20"/>
       <c r="N177" s="20"/>
     </row>
-    <row r="178" spans="6:14">
+    <row r="178" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F178" s="20"/>
       <c r="G178" s="20"/>
       <c r="H178" s="20"/>
@@ -5047,7 +5039,7 @@
       <c r="M178" s="20"/>
       <c r="N178" s="20"/>
     </row>
-    <row r="179" spans="6:14">
+    <row r="179" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F179" s="20"/>
       <c r="G179" s="20"/>
       <c r="H179" s="20"/>
@@ -5058,7 +5050,7 @@
       <c r="M179" s="20"/>
       <c r="N179" s="20"/>
     </row>
-    <row r="180" spans="6:14">
+    <row r="180" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F180" s="20"/>
       <c r="G180" s="20"/>
       <c r="H180" s="20"/>
@@ -5069,7 +5061,7 @@
       <c r="M180" s="20"/>
       <c r="N180" s="20"/>
     </row>
-    <row r="181" spans="6:14">
+    <row r="181" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F181" s="20"/>
       <c r="G181" s="20"/>
       <c r="H181" s="20"/>
@@ -5080,7 +5072,7 @@
       <c r="M181" s="20"/>
       <c r="N181" s="20"/>
     </row>
-    <row r="182" spans="6:14">
+    <row r="182" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F182" s="20"/>
       <c r="G182" s="20"/>
       <c r="H182" s="20"/>
@@ -5091,7 +5083,7 @@
       <c r="M182" s="20"/>
       <c r="N182" s="20"/>
     </row>
-    <row r="183" spans="6:14">
+    <row r="183" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F183" s="20"/>
       <c r="G183" s="20"/>
       <c r="H183" s="20"/>
@@ -5102,7 +5094,7 @@
       <c r="M183" s="20"/>
       <c r="N183" s="20"/>
     </row>
-    <row r="184" spans="6:14">
+    <row r="184" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F184" s="20"/>
       <c r="G184" s="20"/>
       <c r="H184" s="20"/>
@@ -5113,7 +5105,7 @@
       <c r="M184" s="20"/>
       <c r="N184" s="20"/>
     </row>
-    <row r="185" spans="6:14">
+    <row r="185" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F185" s="20"/>
       <c r="G185" s="20"/>
       <c r="H185" s="20"/>
@@ -5124,7 +5116,7 @@
       <c r="M185" s="20"/>
       <c r="N185" s="20"/>
     </row>
-    <row r="186" spans="6:14">
+    <row r="186" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F186" s="20"/>
       <c r="G186" s="20"/>
       <c r="H186" s="20"/>
@@ -5135,7 +5127,7 @@
       <c r="M186" s="20"/>
       <c r="N186" s="20"/>
     </row>
-    <row r="187" spans="6:14">
+    <row r="187" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F187" s="20"/>
       <c r="G187" s="20"/>
       <c r="H187" s="20"/>
@@ -5146,7 +5138,7 @@
       <c r="M187" s="20"/>
       <c r="N187" s="20"/>
     </row>
-    <row r="188" spans="6:14">
+    <row r="188" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F188" s="20"/>
       <c r="G188" s="20"/>
       <c r="H188" s="20"/>
@@ -5157,7 +5149,7 @@
       <c r="M188" s="20"/>
       <c r="N188" s="20"/>
     </row>
-    <row r="189" spans="6:14">
+    <row r="189" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F189" s="20"/>
       <c r="G189" s="20"/>
       <c r="H189" s="20"/>
@@ -5168,7 +5160,7 @@
       <c r="M189" s="20"/>
       <c r="N189" s="20"/>
     </row>
-    <row r="190" spans="6:14">
+    <row r="190" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F190" s="20"/>
       <c r="G190" s="20"/>
       <c r="H190" s="20"/>
@@ -5179,7 +5171,7 @@
       <c r="M190" s="20"/>
       <c r="N190" s="20"/>
     </row>
-    <row r="191" spans="6:14">
+    <row r="191" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F191" s="20"/>
       <c r="G191" s="20"/>
       <c r="H191" s="20"/>
@@ -5190,7 +5182,7 @@
       <c r="M191" s="20"/>
       <c r="N191" s="20"/>
     </row>
-    <row r="192" spans="6:14">
+    <row r="192" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F192" s="20"/>
       <c r="G192" s="20"/>
       <c r="H192" s="20"/>
@@ -5201,7 +5193,7 @@
       <c r="M192" s="20"/>
       <c r="N192" s="20"/>
     </row>
-    <row r="193" spans="6:14">
+    <row r="193" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F193" s="20"/>
       <c r="G193" s="20"/>
       <c r="H193" s="20"/>
@@ -5212,7 +5204,7 @@
       <c r="M193" s="20"/>
       <c r="N193" s="20"/>
     </row>
-    <row r="194" spans="6:14">
+    <row r="194" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F194" s="20"/>
       <c r="G194" s="20"/>
       <c r="H194" s="20"/>
@@ -5223,7 +5215,7 @@
       <c r="M194" s="20"/>
       <c r="N194" s="20"/>
     </row>
-    <row r="195" spans="6:14">
+    <row r="195" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F195" s="20"/>
       <c r="G195" s="20"/>
       <c r="H195" s="20"/>
@@ -5234,7 +5226,7 @@
       <c r="M195" s="20"/>
       <c r="N195" s="20"/>
     </row>
-    <row r="196" spans="6:14">
+    <row r="196" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F196" s="20"/>
       <c r="G196" s="20"/>
       <c r="H196" s="20"/>
@@ -5245,7 +5237,7 @@
       <c r="M196" s="20"/>
       <c r="N196" s="20"/>
     </row>
-    <row r="197" spans="6:14">
+    <row r="197" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F197" s="20"/>
       <c r="G197" s="20"/>
       <c r="H197" s="20"/>
@@ -5256,7 +5248,7 @@
       <c r="M197" s="20"/>
       <c r="N197" s="20"/>
     </row>
-    <row r="198" spans="6:14">
+    <row r="198" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F198" s="20"/>
       <c r="G198" s="20"/>
       <c r="H198" s="20"/>
@@ -5267,7 +5259,7 @@
       <c r="M198" s="20"/>
       <c r="N198" s="20"/>
     </row>
-    <row r="199" spans="6:14">
+    <row r="199" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F199" s="20"/>
       <c r="G199" s="20"/>
       <c r="H199" s="20"/>
@@ -5278,7 +5270,7 @@
       <c r="M199" s="20"/>
       <c r="N199" s="20"/>
     </row>
-    <row r="200" spans="6:14">
+    <row r="200" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F200" s="20"/>
       <c r="G200" s="20"/>
       <c r="H200" s="20"/>
@@ -5289,7 +5281,7 @@
       <c r="M200" s="20"/>
       <c r="N200" s="20"/>
     </row>
-    <row r="201" spans="6:14">
+    <row r="201" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F201" s="20"/>
       <c r="G201" s="20"/>
       <c r="H201" s="20"/>
@@ -5300,7 +5292,7 @@
       <c r="M201" s="20"/>
       <c r="N201" s="20"/>
     </row>
-    <row r="202" spans="6:14">
+    <row r="202" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F202" s="20"/>
       <c r="G202" s="20"/>
       <c r="H202" s="20"/>
@@ -5311,7 +5303,7 @@
       <c r="M202" s="20"/>
       <c r="N202" s="20"/>
     </row>
-    <row r="203" spans="6:14">
+    <row r="203" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F203" s="20"/>
       <c r="G203" s="20"/>
       <c r="H203" s="20"/>
@@ -5322,7 +5314,7 @@
       <c r="M203" s="20"/>
       <c r="N203" s="20"/>
     </row>
-    <row r="204" spans="6:14">
+    <row r="204" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F204" s="20"/>
       <c r="G204" s="20"/>
       <c r="H204" s="20"/>
@@ -5333,7 +5325,7 @@
       <c r="M204" s="20"/>
       <c r="N204" s="20"/>
     </row>
-    <row r="205" spans="6:14">
+    <row r="205" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F205" s="20"/>
       <c r="G205" s="20"/>
       <c r="H205" s="20"/>
@@ -5344,7 +5336,7 @@
       <c r="M205" s="20"/>
       <c r="N205" s="20"/>
     </row>
-    <row r="206" spans="6:14">
+    <row r="206" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F206" s="20"/>
       <c r="G206" s="20"/>
       <c r="H206" s="20"/>
@@ -5355,7 +5347,7 @@
       <c r="M206" s="20"/>
       <c r="N206" s="20"/>
     </row>
-    <row r="207" spans="6:14">
+    <row r="207" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F207" s="20"/>
       <c r="G207" s="20"/>
       <c r="H207" s="20"/>
@@ -5366,7 +5358,7 @@
       <c r="M207" s="20"/>
       <c r="N207" s="20"/>
     </row>
-    <row r="208" spans="6:14">
+    <row r="208" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F208" s="20"/>
       <c r="G208" s="20"/>
       <c r="H208" s="20"/>
@@ -5377,7 +5369,7 @@
       <c r="M208" s="20"/>
       <c r="N208" s="20"/>
     </row>
-    <row r="209" spans="6:14">
+    <row r="209" spans="6:14" x14ac:dyDescent="0.2">
       <c r="F209" s="20"/>
       <c r="G209" s="20"/>
       <c r="H209" s="20"/>
@@ -5537,21 +5529,21 @@
       <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="19.5" customWidth="1"/>
-    <col min="7" max="7" width="46.6640625" customWidth="1"/>
-    <col min="8" max="8" width="35.33203125" customWidth="1"/>
-    <col min="9" max="11" width="12.33203125" customWidth="1"/>
-    <col min="12" max="12" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="46.7109375" customWidth="1"/>
+    <col min="8" max="8" width="35.28515625" customWidth="1"/>
+    <col min="9" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="25.42578125" customWidth="1"/>
     <col min="13" max="13" width="119" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="D1" s="48" t="s">
         <v>85</v>
       </c>
@@ -5571,7 +5563,7 @@
       <c r="Q1" s="52"/>
       <c r="R1" s="52"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="50" t="s">
         <v>0</v>
       </c>
@@ -5610,7 +5602,7 @@
       <c r="Q2" s="58"/>
       <c r="R2" s="59"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B3" s="56" t="s">
         <v>88</v>
       </c>
@@ -5643,7 +5635,7 @@
       <c r="Q3" s="57"/>
       <c r="R3" s="57"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B4" s="56" t="s">
         <v>95</v>
       </c>
@@ -5676,7 +5668,7 @@
       <c r="Q4" s="57"/>
       <c r="R4" s="57"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B5" s="15" t="s">
         <v>100</v>
       </c>
@@ -5709,7 +5701,7 @@
       <c r="Q5" s="57"/>
       <c r="R5" s="57"/>
     </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1">
+    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="56" t="s">
         <v>104</v>
       </c>
@@ -5742,7 +5734,7 @@
       <c r="Q6" s="57"/>
       <c r="R6" s="57"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B7" s="56" t="s">
         <v>10</v>
       </c>
@@ -5775,7 +5767,7 @@
       <c r="Q7" s="57"/>
       <c r="R7" s="57"/>
     </row>
-    <row r="8" spans="1:18" ht="13.5" customHeight="1">
+    <row r="8" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="63" t="s">
         <v>111</v>
       </c>
@@ -5803,7 +5795,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B9" s="56" t="s">
         <v>17</v>
       </c>
@@ -5831,7 +5823,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B10" s="15" t="s">
         <v>118</v>
       </c>
@@ -5862,7 +5854,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B11" s="15" t="s">
         <v>122</v>
       </c>
@@ -5889,7 +5881,7 @@
       </c>
       <c r="M11" s="57"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B12" s="15" t="s">
         <v>100</v>
       </c>
@@ -5918,7 +5910,7 @@
       </c>
       <c r="M12" s="57"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B13" s="15" t="s">
         <v>128</v>
       </c>
@@ -5947,7 +5939,7 @@
       </c>
       <c r="M13" s="57"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B14" s="15" t="s">
         <v>131</v>
       </c>
@@ -5973,7 +5965,7 @@
       </c>
       <c r="M14" s="57"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B15" s="15" t="s">
         <v>133</v>
       </c>
@@ -5993,7 +5985,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
         <v>100</v>
       </c>
@@ -6026,7 +6018,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="2:27">
+    <row r="17" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B17" s="56" t="s">
         <v>139</v>
       </c>
@@ -6058,7 +6050,7 @@
       </c>
       <c r="M17" s="57"/>
     </row>
-    <row r="18" spans="2:27">
+    <row r="18" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B18" s="56" t="s">
         <v>142</v>
       </c>
@@ -6089,7 +6081,7 @@
       </c>
       <c r="M18" s="57"/>
     </row>
-    <row r="19" spans="2:27">
+    <row r="19" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B19" s="56" t="s">
         <v>145</v>
       </c>
@@ -6120,7 +6112,7 @@
       </c>
       <c r="M19" s="57"/>
     </row>
-    <row r="20" spans="2:27" ht="12.75" customHeight="1">
+    <row r="20" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="56" t="s">
         <v>148</v>
       </c>
@@ -6163,7 +6155,7 @@
       <c r="Z20" s="66"/>
       <c r="AA20" s="66"/>
     </row>
-    <row r="21" spans="2:27" ht="12.75" customHeight="1">
+    <row r="21" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="56" t="s">
         <v>152</v>
       </c>
@@ -6198,7 +6190,7 @@
       <c r="Z21" s="66"/>
       <c r="AA21" s="66"/>
     </row>
-    <row r="22" spans="2:27" ht="12.75" customHeight="1">
+    <row r="22" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="15" t="s">
         <v>155</v>
       </c>
@@ -6233,7 +6225,7 @@
       <c r="Z22" s="66"/>
       <c r="AA22" s="66"/>
     </row>
-    <row r="23" spans="2:27" ht="12.75" customHeight="1">
+    <row r="23" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
         <v>158</v>
       </c>
@@ -6276,7 +6268,7 @@
       <c r="Z23" s="66"/>
       <c r="AA23" s="66"/>
     </row>
-    <row r="24" spans="2:27" ht="12.75" customHeight="1">
+    <row r="24" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="15" t="s">
         <v>21</v>
       </c>
@@ -6319,7 +6311,7 @@
       <c r="Z24" s="66"/>
       <c r="AA24" s="66"/>
     </row>
-    <row r="25" spans="2:27" ht="12.75" customHeight="1">
+    <row r="25" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="56" t="s">
         <v>166</v>
       </c>
@@ -6363,7 +6355,7 @@
       <c r="Z25" s="66"/>
       <c r="AA25" s="66"/>
     </row>
-    <row r="26" spans="2:27" ht="12.75" customHeight="1">
+    <row r="26" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="56" t="s">
         <v>170</v>
       </c>
@@ -6407,7 +6399,7 @@
       <c r="Z26" s="66"/>
       <c r="AA26" s="66"/>
     </row>
-    <row r="27" spans="2:27" ht="12.75" customHeight="1">
+    <row r="27" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="67" t="s">
         <v>173</v>
       </c>
@@ -6449,7 +6441,7 @@
       <c r="Z27" s="66"/>
       <c r="AA27" s="66"/>
     </row>
-    <row r="28" spans="2:27" ht="12.75" customHeight="1">
+    <row r="28" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="15" t="s">
         <v>166</v>
       </c>
@@ -6493,7 +6485,7 @@
       <c r="Z28" s="66"/>
       <c r="AA28" s="66"/>
     </row>
-    <row r="29" spans="2:27" ht="12.75" customHeight="1">
+    <row r="29" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="15" t="s">
         <v>178</v>
       </c>
@@ -6533,7 +6525,7 @@
       <c r="Z29" s="66"/>
       <c r="AA29" s="66"/>
     </row>
-    <row r="30" spans="2:27" ht="12.75" customHeight="1">
+    <row r="30" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="15" t="s">
         <v>181</v>
       </c>
@@ -6577,7 +6569,7 @@
       <c r="Z30" s="66"/>
       <c r="AA30" s="66"/>
     </row>
-    <row r="31" spans="2:27" ht="12.75" customHeight="1">
+    <row r="31" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="56" t="s">
         <v>139</v>
       </c>
@@ -6619,7 +6611,7 @@
       <c r="Z31" s="66"/>
       <c r="AA31" s="66"/>
     </row>
-    <row r="32" spans="2:27" ht="12.75" customHeight="1">
+    <row r="32" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="56" t="s">
         <v>184</v>
       </c>
@@ -6651,7 +6643,7 @@
       <c r="Z32" s="66"/>
       <c r="AA32" s="66"/>
     </row>
-    <row r="33" spans="2:27" ht="12.75" customHeight="1">
+    <row r="33" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="56" t="s">
         <v>186</v>
       </c>
@@ -6695,7 +6687,7 @@
       <c r="Z33" s="66"/>
       <c r="AA33" s="66"/>
     </row>
-    <row r="34" spans="2:27" ht="12.75" customHeight="1">
+    <row r="34" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="56" t="s">
         <v>88</v>
       </c>
@@ -6739,7 +6731,7 @@
       <c r="Z34" s="66"/>
       <c r="AA34" s="66"/>
     </row>
-    <row r="35" spans="2:27" ht="12.75" customHeight="1">
+    <row r="35" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="56" t="s">
         <v>133</v>
       </c>
@@ -6781,7 +6773,7 @@
       <c r="Z35" s="66"/>
       <c r="AA35" s="66"/>
     </row>
-    <row r="36" spans="2:27" ht="12.75" customHeight="1">
+    <row r="36" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="56" t="s">
         <v>195</v>
       </c>
@@ -6825,7 +6817,7 @@
       <c r="Z36" s="66"/>
       <c r="AA36" s="66"/>
     </row>
-    <row r="37" spans="2:27" ht="12.75" customHeight="1">
+    <row r="37" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="15" t="s">
         <v>178</v>
       </c>
@@ -6869,7 +6861,7 @@
       <c r="Z37" s="66"/>
       <c r="AA37" s="66"/>
     </row>
-    <row r="38" spans="2:27" ht="12.75" customHeight="1">
+    <row r="38" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="56" t="s">
         <v>202</v>
       </c>
@@ -6913,7 +6905,7 @@
       <c r="Z38" s="66"/>
       <c r="AA38" s="66"/>
     </row>
-    <row r="39" spans="2:27" ht="12.75" customHeight="1">
+    <row r="39" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="15" t="s">
         <v>205</v>
       </c>
@@ -6949,7 +6941,7 @@
       <c r="Z39" s="66"/>
       <c r="AA39" s="66"/>
     </row>
-    <row r="40" spans="2:27" ht="12.75" customHeight="1">
+    <row r="40" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="56"/>
       <c r="C40" s="56"/>
       <c r="D40" s="56"/>
@@ -6978,7 +6970,7 @@
       <c r="Z40" s="66"/>
       <c r="AA40" s="66"/>
     </row>
-    <row r="41" spans="2:27" ht="12.75" customHeight="1">
+    <row r="41" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="56" t="s">
         <v>88</v>
       </c>
@@ -7009,7 +7001,7 @@
       <c r="Z41" s="66"/>
       <c r="AA41" s="66"/>
     </row>
-    <row r="42" spans="2:27" ht="12.75" customHeight="1">
+    <row r="42" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="15" t="s">
         <v>133</v>
       </c>
@@ -7038,7 +7030,7 @@
       <c r="Z42" s="66"/>
       <c r="AA42" s="66"/>
     </row>
-    <row r="43" spans="2:27" ht="27.75" customHeight="1">
+    <row r="43" spans="2:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="15" t="s">
         <v>195</v>
       </c>
@@ -7070,7 +7062,7 @@
       <c r="Z43" s="66"/>
       <c r="AA43" s="66"/>
     </row>
-    <row r="44" spans="2:27" ht="12.75" customHeight="1">
+    <row r="44" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="15" t="s">
         <v>210</v>
       </c>
@@ -7108,7 +7100,7 @@
       <c r="Z44" s="66"/>
       <c r="AA44" s="66"/>
     </row>
-    <row r="45" spans="2:27" ht="12.75" customHeight="1">
+    <row r="45" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="15" t="s">
         <v>88</v>
       </c>
@@ -7144,7 +7136,7 @@
       <c r="Z45" s="66"/>
       <c r="AA45" s="66"/>
     </row>
-    <row r="46" spans="2:27" ht="12.75" customHeight="1">
+    <row r="46" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="15" t="s">
         <v>152</v>
       </c>
@@ -7180,7 +7172,7 @@
       <c r="Z46" s="66"/>
       <c r="AA46" s="66"/>
     </row>
-    <row r="47" spans="2:27" ht="12.75" customHeight="1">
+    <row r="47" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="15" t="s">
         <v>155</v>
       </c>
@@ -7216,7 +7208,7 @@
       <c r="Z47" s="66"/>
       <c r="AA47" s="66"/>
     </row>
-    <row r="48" spans="2:27" ht="12.75" customHeight="1">
+    <row r="48" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="15" t="s">
         <v>17</v>
       </c>
@@ -7246,7 +7238,7 @@
       <c r="Z48" s="66"/>
       <c r="AA48" s="66"/>
     </row>
-    <row r="49" spans="2:27" ht="12.75" customHeight="1">
+    <row r="49" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="15" t="s">
         <v>214</v>
       </c>
@@ -7288,7 +7280,7 @@
       <c r="Z49" s="66"/>
       <c r="AA49" s="66"/>
     </row>
-    <row r="50" spans="2:27" ht="12.75" customHeight="1">
+    <row r="50" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="15" t="s">
         <v>217</v>
       </c>
@@ -7322,7 +7314,7 @@
       <c r="Z50" s="66"/>
       <c r="AA50" s="66"/>
     </row>
-    <row r="51" spans="2:27" ht="12.75" customHeight="1">
+    <row r="51" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="15" t="s">
         <v>219</v>
       </c>
@@ -7356,7 +7348,7 @@
       <c r="Z51" s="66"/>
       <c r="AA51" s="66"/>
     </row>
-    <row r="52" spans="2:27" ht="12.75" customHeight="1">
+    <row r="52" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="15" t="s">
         <v>10</v>
       </c>
@@ -7400,7 +7392,7 @@
       <c r="Z52" s="66"/>
       <c r="AA52" s="66"/>
     </row>
-    <row r="53" spans="2:27" ht="12.75" customHeight="1">
+    <row r="53" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="15" t="s">
         <v>217</v>
       </c>
@@ -7444,7 +7436,7 @@
       <c r="Z53" s="66"/>
       <c r="AA53" s="66"/>
     </row>
-    <row r="54" spans="2:27" ht="12.75" customHeight="1">
+    <row r="54" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="15" t="s">
         <v>88</v>
       </c>
@@ -7489,7 +7481,7 @@
       <c r="Z54" s="66"/>
       <c r="AA54" s="66"/>
     </row>
-    <row r="55" spans="2:27" ht="12.75" customHeight="1">
+    <row r="55" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="15" t="s">
         <v>17</v>
       </c>
@@ -7531,7 +7523,7 @@
       <c r="Z55" s="66"/>
       <c r="AA55" s="66"/>
     </row>
-    <row r="56" spans="2:27" ht="12.75" customHeight="1">
+    <row r="56" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="15" t="s">
         <v>217</v>
       </c>
@@ -7573,7 +7565,7 @@
       <c r="Z56" s="66"/>
       <c r="AA56" s="66"/>
     </row>
-    <row r="57" spans="2:27" ht="12.75" customHeight="1">
+    <row r="57" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="15" t="s">
         <v>139</v>
       </c>
@@ -7613,7 +7605,7 @@
       <c r="Z57" s="66"/>
       <c r="AA57" s="66"/>
     </row>
-    <row r="58" spans="2:27" ht="12.75" customHeight="1">
+    <row r="58" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="15" t="s">
         <v>17</v>
       </c>
@@ -7655,7 +7647,7 @@
       <c r="Z58" s="66"/>
       <c r="AA58" s="66"/>
     </row>
-    <row r="59" spans="2:27" ht="12.75" customHeight="1">
+    <row r="59" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="15" t="s">
         <v>222</v>
       </c>
@@ -7695,7 +7687,7 @@
       <c r="Z59" s="66"/>
       <c r="AA59" s="66"/>
     </row>
-    <row r="60" spans="2:27" ht="12.75" customHeight="1">
+    <row r="60" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="15" t="s">
         <v>217</v>
       </c>
@@ -7737,7 +7729,7 @@
       <c r="Z60" s="66"/>
       <c r="AA60" s="66"/>
     </row>
-    <row r="61" spans="2:27" ht="12.75" customHeight="1">
+    <row r="61" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="15" t="s">
         <v>88</v>
       </c>
@@ -7779,7 +7771,7 @@
       <c r="Z61" s="66"/>
       <c r="AA61" s="66"/>
     </row>
-    <row r="62" spans="2:27" ht="12.75" customHeight="1">
+    <row r="62" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="15" t="s">
         <v>181</v>
       </c>
@@ -7821,7 +7813,7 @@
       <c r="Z62" s="66"/>
       <c r="AA62" s="66"/>
     </row>
-    <row r="63" spans="2:27" ht="12.75" customHeight="1">
+    <row r="63" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="15" t="s">
         <v>139</v>
       </c>
@@ -7863,7 +7855,7 @@
       <c r="Z63" s="66"/>
       <c r="AA63" s="66"/>
     </row>
-    <row r="64" spans="2:27" ht="12.75" customHeight="1">
+    <row r="64" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="60" t="s">
         <v>139</v>
       </c>
@@ -7903,7 +7895,7 @@
       <c r="Z64" s="66"/>
       <c r="AA64" s="66"/>
     </row>
-    <row r="65" spans="2:27" ht="12.75" customHeight="1">
+    <row r="65" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="60" t="s">
         <v>139</v>
       </c>
@@ -7943,7 +7935,7 @@
       <c r="Z65" s="66"/>
       <c r="AA65" s="66"/>
     </row>
-    <row r="66" spans="2:27" ht="12.75" customHeight="1">
+    <row r="66" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="60" t="s">
         <v>230</v>
       </c>
@@ -7983,7 +7975,7 @@
       <c r="Z66" s="66"/>
       <c r="AA66" s="66"/>
     </row>
-    <row r="67" spans="2:27" ht="12.75" customHeight="1">
+    <row r="67" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="60" t="s">
         <v>234</v>
       </c>
@@ -8015,7 +8007,7 @@
       <c r="Z67" s="66"/>
       <c r="AA67" s="66"/>
     </row>
-    <row r="68" spans="2:27" ht="12.75" customHeight="1">
+    <row r="68" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="17" t="s">
         <v>236</v>
       </c>
@@ -8047,7 +8039,7 @@
       <c r="Z68" s="66"/>
       <c r="AA68" s="66"/>
     </row>
-    <row r="69" spans="2:27" ht="12.75" customHeight="1">
+    <row r="69" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="17" t="s">
         <v>238</v>
       </c>
@@ -8077,7 +8069,7 @@
       <c r="Z69" s="66"/>
       <c r="AA69" s="66"/>
     </row>
-    <row r="70" spans="2:27" ht="12.75" customHeight="1">
+    <row r="70" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70" s="60" t="s">
         <v>10</v>
       </c>
@@ -8117,7 +8109,7 @@
       <c r="Z70" s="66"/>
       <c r="AA70" s="66"/>
     </row>
-    <row r="71" spans="2:27" ht="12.75" customHeight="1">
+    <row r="71" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="60" t="s">
         <v>217</v>
       </c>
@@ -8157,7 +8149,7 @@
       <c r="Z71" s="66"/>
       <c r="AA71" s="66"/>
     </row>
-    <row r="72" spans="2:27" ht="12.75" customHeight="1">
+    <row r="72" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="60" t="s">
         <v>240</v>
       </c>
@@ -8185,7 +8177,7 @@
       <c r="Z72" s="66"/>
       <c r="AA72" s="66"/>
     </row>
-    <row r="73" spans="2:27" ht="12.75" customHeight="1">
+    <row r="73" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="60" t="s">
         <v>241</v>
       </c>
@@ -8225,7 +8217,7 @@
       <c r="Z73" s="66"/>
       <c r="AA73" s="66"/>
     </row>
-    <row r="74" spans="2:27" ht="12.75" customHeight="1">
+    <row r="74" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="60" t="s">
         <v>244</v>
       </c>
@@ -8257,7 +8249,7 @@
       <c r="Z74" s="66"/>
       <c r="AA74" s="66"/>
     </row>
-    <row r="75" spans="2:27" ht="12.75" customHeight="1">
+    <row r="75" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B75" s="71" t="s">
         <v>247</v>
       </c>
@@ -8295,7 +8287,7 @@
       <c r="Z75" s="66"/>
       <c r="AA75" s="66"/>
     </row>
-    <row r="76" spans="2:27" ht="12.75" customHeight="1">
+    <row r="76" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="75" t="s">
         <v>249</v>
       </c>
@@ -8333,7 +8325,7 @@
       <c r="Z76" s="66"/>
       <c r="AA76" s="66"/>
     </row>
-    <row r="77" spans="2:27" ht="12.75" customHeight="1">
+    <row r="77" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B77" s="38" t="s">
         <v>251</v>
       </c>
@@ -8373,7 +8365,7 @@
       <c r="Z77" s="66"/>
       <c r="AA77" s="66"/>
     </row>
-    <row r="78" spans="2:27" ht="12.75" customHeight="1">
+    <row r="78" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="62" t="s">
         <v>249</v>
       </c>
@@ -8412,7 +8404,7 @@
       <c r="Z78" s="66"/>
       <c r="AA78" s="66"/>
     </row>
-    <row r="79" spans="2:27" ht="12.75" customHeight="1">
+    <row r="79" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="62" t="s">
         <v>254</v>
       </c>
@@ -8451,7 +8443,7 @@
       <c r="Z79" s="66"/>
       <c r="AA79" s="66"/>
     </row>
-    <row r="80" spans="2:27" ht="12.75" customHeight="1">
+    <row r="80" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B80" s="62" t="s">
         <v>257</v>
       </c>
@@ -8490,7 +8482,7 @@
       <c r="Z80" s="66"/>
       <c r="AA80" s="66"/>
     </row>
-    <row r="81" spans="2:27" ht="12.75" customHeight="1">
+    <row r="81" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B81" s="62" t="s">
         <v>259</v>
       </c>
@@ -8529,7 +8521,7 @@
       <c r="Z81" s="66"/>
       <c r="AA81" s="66"/>
     </row>
-    <row r="82" spans="2:27" ht="12.75" customHeight="1">
+    <row r="82" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="78" t="s">
         <v>262</v>
       </c>
@@ -8562,7 +8554,7 @@
       <c r="Z82" s="66"/>
       <c r="AA82" s="66"/>
     </row>
-    <row r="83" spans="2:27" ht="12.75" customHeight="1">
+    <row r="83" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>264</v>
       </c>
@@ -8601,7 +8593,7 @@
       <c r="Z83" s="66"/>
       <c r="AA83" s="66"/>
     </row>
-    <row r="84" spans="2:27" ht="12.75" customHeight="1">
+    <row r="84" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B84" s="79" t="s">
         <v>267</v>
       </c>
@@ -8640,7 +8632,7 @@
       <c r="Z84" s="66"/>
       <c r="AA84" s="66"/>
     </row>
-    <row r="85" spans="2:27" ht="12.75" customHeight="1">
+    <row r="85" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B85" s="79" t="s">
         <v>268</v>
       </c>
@@ -8685,7 +8677,7 @@
       <c r="Z85" s="66"/>
       <c r="AA85" s="66"/>
     </row>
-    <row r="86" spans="2:27" ht="12.75" customHeight="1">
+    <row r="86" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L86" s="119"/>
       <c r="M86" s="119"/>
       <c r="N86" s="119"/>
@@ -8703,7 +8695,7 @@
       <c r="Z86" s="66"/>
       <c r="AA86" s="66"/>
     </row>
-    <row r="87" spans="2:27" ht="12.75" customHeight="1">
+    <row r="87" spans="2:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L87" s="119"/>
       <c r="M87" s="119"/>
       <c r="N87" s="119"/>
@@ -8790,19 +8782,19 @@
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="43" customWidth="1"/>
-    <col min="5" max="5" width="88.6640625" customWidth="1"/>
+    <col min="5" max="5" width="88.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B2" s="49" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="2:21" ht="12.75" customHeight="1">
+    <row r="3" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="120" t="s">
         <v>271</v>
       </c>
@@ -8826,7 +8818,7 @@
       <c r="T3" s="120"/>
       <c r="U3" s="120"/>
     </row>
-    <row r="4" spans="2:21">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B4" s="120"/>
       <c r="C4" s="120"/>
       <c r="D4" s="120"/>
@@ -8848,7 +8840,7 @@
       <c r="T4" s="120"/>
       <c r="U4" s="120"/>
     </row>
-    <row r="5" spans="2:21">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B5" s="120"/>
       <c r="C5" s="120"/>
       <c r="D5" s="120"/>
@@ -8870,7 +8862,7 @@
       <c r="T5" s="120"/>
       <c r="U5" s="120"/>
     </row>
-    <row r="6" spans="2:21">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B6" s="120"/>
       <c r="C6" s="120"/>
       <c r="D6" s="120"/>
@@ -8892,7 +8884,7 @@
       <c r="T6" s="120"/>
       <c r="U6" s="120"/>
     </row>
-    <row r="7" spans="2:21">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B7" s="120"/>
       <c r="C7" s="120"/>
       <c r="D7" s="120"/>
@@ -8914,7 +8906,7 @@
       <c r="T7" s="120"/>
       <c r="U7" s="120"/>
     </row>
-    <row r="8" spans="2:21">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B8" s="120"/>
       <c r="C8" s="120"/>
       <c r="D8" s="120"/>
@@ -8936,7 +8928,7 @@
       <c r="T8" s="120"/>
       <c r="U8" s="120"/>
     </row>
-    <row r="9" spans="2:21">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B9" s="120"/>
       <c r="C9" s="120"/>
       <c r="D9" s="120"/>
@@ -8958,7 +8950,7 @@
       <c r="T9" s="120"/>
       <c r="U9" s="120"/>
     </row>
-    <row r="10" spans="2:21">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B10" s="120"/>
       <c r="C10" s="120"/>
       <c r="D10" s="120"/>
@@ -8980,7 +8972,7 @@
       <c r="T10" s="120"/>
       <c r="U10" s="120"/>
     </row>
-    <row r="11" spans="2:21">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B11" s="120"/>
       <c r="C11" s="120"/>
       <c r="D11" s="120"/>
@@ -9002,7 +8994,7 @@
       <c r="T11" s="120"/>
       <c r="U11" s="120"/>
     </row>
-    <row r="12" spans="2:21">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B12" s="120"/>
       <c r="C12" s="120"/>
       <c r="D12" s="120"/>
@@ -9024,7 +9016,7 @@
       <c r="T12" s="120"/>
       <c r="U12" s="120"/>
     </row>
-    <row r="15" spans="2:21" ht="12.75" customHeight="1">
+    <row r="15" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>272</v>
       </c>
@@ -9041,7 +9033,7 @@
       <c r="N15" s="119"/>
       <c r="O15" s="119"/>
     </row>
-    <row r="16" spans="2:21">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.2">
       <c r="F16" s="119"/>
       <c r="G16" s="119"/>
       <c r="H16" s="119"/>
@@ -9053,7 +9045,7 @@
       <c r="N16" s="119"/>
       <c r="O16" s="119"/>
     </row>
-    <row r="17" spans="2:15">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F17" s="119"/>
       <c r="G17" s="119"/>
       <c r="H17" s="119"/>
@@ -9065,7 +9057,7 @@
       <c r="N17" s="119"/>
       <c r="O17" s="119"/>
     </row>
-    <row r="18" spans="2:15">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B18" s="49" t="s">
         <v>274</v>
       </c>
@@ -9089,7 +9081,7 @@
       <c r="N18" s="119"/>
       <c r="O18" s="119"/>
     </row>
-    <row r="19" spans="2:15">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>277</v>
       </c>
@@ -9113,7 +9105,7 @@
       <c r="N19" s="119"/>
       <c r="O19" s="119"/>
     </row>
-    <row r="20" spans="2:15">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>280</v>
       </c>
@@ -9134,7 +9126,7 @@
       <c r="N20" s="119"/>
       <c r="O20" s="119"/>
     </row>
-    <row r="21" spans="2:15">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>283</v>
       </c>
@@ -9155,7 +9147,7 @@
       <c r="N21" s="119"/>
       <c r="O21" s="119"/>
     </row>
-    <row r="22" spans="2:15">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>11</v>
       </c>
@@ -9176,7 +9168,7 @@
       <c r="N22" s="119"/>
       <c r="O22" s="119"/>
     </row>
-    <row r="23" spans="2:15">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>287</v>
       </c>
@@ -9194,7 +9186,7 @@
       <c r="N23" s="119"/>
       <c r="O23" s="119"/>
     </row>
-    <row r="24" spans="2:15">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F24" s="119"/>
       <c r="G24" s="119"/>
       <c r="H24" s="119"/>
@@ -9206,7 +9198,7 @@
       <c r="N24" s="119"/>
       <c r="O24" s="119"/>
     </row>
-    <row r="25" spans="2:15">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F25" s="119"/>
       <c r="G25" s="119"/>
       <c r="H25" s="119"/>
@@ -9218,7 +9210,7 @@
       <c r="N25" s="119"/>
       <c r="O25" s="119"/>
     </row>
-    <row r="26" spans="2:15">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F26" s="119"/>
       <c r="G26" s="119"/>
       <c r="H26" s="119"/>
@@ -9230,7 +9222,7 @@
       <c r="N26" s="119"/>
       <c r="O26" s="119"/>
     </row>
-    <row r="27" spans="2:15">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F27" s="119"/>
       <c r="G27" s="119"/>
       <c r="H27" s="119"/>
@@ -9242,7 +9234,7 @@
       <c r="N27" s="119"/>
       <c r="O27" s="119"/>
     </row>
-    <row r="28" spans="2:15">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F28" s="119"/>
       <c r="G28" s="119"/>
       <c r="H28" s="119"/>
@@ -9254,7 +9246,7 @@
       <c r="N28" s="119"/>
       <c r="O28" s="119"/>
     </row>
-    <row r="29" spans="2:15">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F29" s="119"/>
       <c r="G29" s="119"/>
       <c r="H29" s="119"/>
@@ -9266,7 +9258,7 @@
       <c r="N29" s="119"/>
       <c r="O29" s="119"/>
     </row>
-    <row r="30" spans="2:15">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F30" s="119"/>
       <c r="G30" s="119"/>
       <c r="H30" s="119"/>
@@ -9278,7 +9270,7 @@
       <c r="N30" s="119"/>
       <c r="O30" s="119"/>
     </row>
-    <row r="31" spans="2:15">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F31" s="119"/>
       <c r="G31" s="119"/>
       <c r="H31" s="119"/>
@@ -9290,7 +9282,7 @@
       <c r="N31" s="119"/>
       <c r="O31" s="119"/>
     </row>
-    <row r="32" spans="2:15">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F32" s="119"/>
       <c r="G32" s="119"/>
       <c r="H32" s="119"/>
@@ -9302,7 +9294,7 @@
       <c r="N32" s="119"/>
       <c r="O32" s="119"/>
     </row>
-    <row r="33" spans="5:15">
+    <row r="33" spans="5:15" x14ac:dyDescent="0.2">
       <c r="F33" s="119"/>
       <c r="G33" s="119"/>
       <c r="H33" s="119"/>
@@ -9314,7 +9306,7 @@
       <c r="N33" s="119"/>
       <c r="O33" s="119"/>
     </row>
-    <row r="34" spans="5:15">
+    <row r="34" spans="5:15" x14ac:dyDescent="0.2">
       <c r="F34" s="119"/>
       <c r="G34" s="119"/>
       <c r="H34" s="119"/>
@@ -9326,7 +9318,7 @@
       <c r="N34" s="119"/>
       <c r="O34" s="119"/>
     </row>
-    <row r="35" spans="5:15">
+    <row r="35" spans="5:15" x14ac:dyDescent="0.2">
       <c r="F35" s="119"/>
       <c r="G35" s="119"/>
       <c r="H35" s="119"/>
@@ -9338,7 +9330,7 @@
       <c r="N35" s="119"/>
       <c r="O35" s="119"/>
     </row>
-    <row r="36" spans="5:15" ht="14">
+    <row r="36" spans="5:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="E36" s="23" t="s">
         <v>289</v>
       </c>
@@ -9353,7 +9345,7 @@
       <c r="N36" s="119"/>
       <c r="O36" s="119"/>
     </row>
-    <row r="37" spans="5:15" ht="14">
+    <row r="37" spans="5:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="E37" s="23" t="s">
         <v>290</v>
       </c>
@@ -9368,7 +9360,7 @@
       <c r="N37" s="119"/>
       <c r="O37" s="119"/>
     </row>
-    <row r="38" spans="5:15">
+    <row r="38" spans="5:15" x14ac:dyDescent="0.2">
       <c r="F38" s="119"/>
       <c r="G38" s="119"/>
       <c r="H38" s="119"/>
@@ -9380,7 +9372,7 @@
       <c r="N38" s="119"/>
       <c r="O38" s="119"/>
     </row>
-    <row r="39" spans="5:15">
+    <row r="39" spans="5:15" x14ac:dyDescent="0.2">
       <c r="F39" s="119"/>
       <c r="G39" s="119"/>
       <c r="H39" s="119"/>
@@ -9392,7 +9384,7 @@
       <c r="N39" s="119"/>
       <c r="O39" s="119"/>
     </row>
-    <row r="40" spans="5:15">
+    <row r="40" spans="5:15" x14ac:dyDescent="0.2">
       <c r="F40" s="119"/>
       <c r="G40" s="119"/>
       <c r="H40" s="119"/>
@@ -9404,7 +9396,7 @@
       <c r="N40" s="119"/>
       <c r="O40" s="119"/>
     </row>
-    <row r="41" spans="5:15">
+    <row r="41" spans="5:15" x14ac:dyDescent="0.2">
       <c r="F41" s="119"/>
       <c r="G41" s="119"/>
       <c r="H41" s="119"/>
@@ -9416,7 +9408,7 @@
       <c r="N41" s="119"/>
       <c r="O41" s="119"/>
     </row>
-    <row r="42" spans="5:15">
+    <row r="42" spans="5:15" x14ac:dyDescent="0.2">
       <c r="F42" s="119"/>
       <c r="G42" s="119"/>
       <c r="H42" s="119"/>
@@ -9428,7 +9420,7 @@
       <c r="N42" s="119"/>
       <c r="O42" s="119"/>
     </row>
-    <row r="43" spans="5:15">
+    <row r="43" spans="5:15" x14ac:dyDescent="0.2">
       <c r="F43" s="119"/>
       <c r="G43" s="119"/>
       <c r="H43" s="119"/>
@@ -9440,7 +9432,7 @@
       <c r="N43" s="119"/>
       <c r="O43" s="119"/>
     </row>
-    <row r="44" spans="5:15">
+    <row r="44" spans="5:15" x14ac:dyDescent="0.2">
       <c r="F44" s="119"/>
       <c r="G44" s="119"/>
       <c r="H44" s="119"/>
@@ -9452,7 +9444,7 @@
       <c r="N44" s="119"/>
       <c r="O44" s="119"/>
     </row>
-    <row r="45" spans="5:15">
+    <row r="45" spans="5:15" x14ac:dyDescent="0.2">
       <c r="F45" s="119"/>
       <c r="G45" s="119"/>
       <c r="H45" s="119"/>
@@ -9464,7 +9456,7 @@
       <c r="N45" s="119"/>
       <c r="O45" s="119"/>
     </row>
-    <row r="46" spans="5:15">
+    <row r="46" spans="5:15" x14ac:dyDescent="0.2">
       <c r="F46" s="119"/>
       <c r="G46" s="119"/>
       <c r="H46" s="119"/>
@@ -9476,7 +9468,7 @@
       <c r="N46" s="119"/>
       <c r="O46" s="119"/>
     </row>
-    <row r="47" spans="5:15">
+    <row r="47" spans="5:15" x14ac:dyDescent="0.2">
       <c r="F47" s="119"/>
       <c r="G47" s="119"/>
       <c r="H47" s="119"/>
@@ -9488,7 +9480,7 @@
       <c r="N47" s="119"/>
       <c r="O47" s="119"/>
     </row>
-    <row r="48" spans="5:15">
+    <row r="48" spans="5:15" x14ac:dyDescent="0.2">
       <c r="F48" s="119"/>
       <c r="G48" s="119"/>
       <c r="H48" s="119"/>
@@ -9500,7 +9492,7 @@
       <c r="N48" s="119"/>
       <c r="O48" s="119"/>
     </row>
-    <row r="49" spans="6:15">
+    <row r="49" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F49" s="119"/>
       <c r="G49" s="119"/>
       <c r="H49" s="119"/>
@@ -9512,7 +9504,7 @@
       <c r="N49" s="119"/>
       <c r="O49" s="119"/>
     </row>
-    <row r="50" spans="6:15">
+    <row r="50" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F50" s="119"/>
       <c r="G50" s="119"/>
       <c r="H50" s="119"/>
@@ -9524,7 +9516,7 @@
       <c r="N50" s="119"/>
       <c r="O50" s="119"/>
     </row>
-    <row r="51" spans="6:15">
+    <row r="51" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F51" s="119"/>
       <c r="G51" s="119"/>
       <c r="H51" s="119"/>
@@ -9536,7 +9528,7 @@
       <c r="N51" s="119"/>
       <c r="O51" s="119"/>
     </row>
-    <row r="52" spans="6:15">
+    <row r="52" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F52" s="119"/>
       <c r="G52" s="119"/>
       <c r="H52" s="119"/>
@@ -9566,21 +9558,21 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="23.83203125" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="34.1640625" customWidth="1"/>
-    <col min="6" max="6" width="25.5" customWidth="1"/>
-    <col min="7" max="7" width="23.1640625" customWidth="1"/>
-    <col min="8" max="8" width="24.33203125" customWidth="1"/>
-    <col min="9" max="9" width="33.1640625" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" customWidth="1"/>
-    <col min="12" max="12" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="34.140625" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>291</v>
       </c>
@@ -9612,7 +9604,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>293</v>
       </c>
@@ -9630,7 +9622,7 @@
       <c r="K2" s="64"/>
       <c r="L2" s="64"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>295</v>
       </c>
@@ -9662,7 +9654,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4" s="80">
         <v>2</v>
       </c>
@@ -9691,7 +9683,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B5" s="80">
         <v>3</v>
       </c>
@@ -9714,7 +9706,7 @@
       <c r="K5" s="56"/>
       <c r="L5" s="56"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B6" s="80">
         <v>4</v>
       </c>
@@ -9737,7 +9729,7 @@
       <c r="K6" s="56"/>
       <c r="L6" s="56"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B7" s="80">
         <v>5</v>
       </c>
@@ -9760,7 +9752,7 @@
       <c r="K7" s="56"/>
       <c r="L7" s="56"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D8" s="56" t="s">
         <v>109</v>
       </c>
@@ -9774,7 +9766,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D9" s="56" t="s">
         <v>114</v>
       </c>
@@ -9788,7 +9780,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D10" s="56" t="s">
         <v>116</v>
       </c>
@@ -9799,7 +9791,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D11" s="86" t="s">
         <v>466</v>
       </c>
@@ -9810,7 +9802,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D12" s="15" t="s">
         <v>120</v>
       </c>
@@ -9821,7 +9813,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D13" s="15" t="s">
         <v>124</v>
       </c>
@@ -9832,7 +9824,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D14" s="15" t="s">
         <v>127</v>
       </c>
@@ -9840,7 +9832,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D15" s="15" t="s">
         <v>130</v>
       </c>
@@ -9848,7 +9840,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D16" s="15" t="s">
         <v>130</v>
       </c>
@@ -9856,7 +9848,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="17" spans="4:6">
+    <row r="17" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D17" s="15" t="s">
         <v>134</v>
       </c>
@@ -9864,7 +9856,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="18" spans="4:6">
+    <row r="18" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D18" s="15" t="s">
         <v>137</v>
       </c>
@@ -9872,7 +9864,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="19" spans="4:6">
+    <row r="19" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D19" s="15" t="s">
         <v>141</v>
       </c>
@@ -9880,7 +9872,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="20" spans="4:6">
+    <row r="20" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D20" s="15" t="s">
         <v>144</v>
       </c>
@@ -9888,7 +9880,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="21" spans="4:6">
+    <row r="21" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D21" s="15" t="s">
         <v>11</v>
       </c>
@@ -9896,7 +9888,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="22" spans="4:6">
+    <row r="22" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D22" s="15" t="s">
         <v>151</v>
       </c>
@@ -9904,7 +9896,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="23" spans="4:6">
+    <row r="23" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D23" s="15" t="s">
         <v>154</v>
       </c>
@@ -9912,7 +9904,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="24" spans="4:6">
+    <row r="24" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D24" s="15" t="s">
         <v>157</v>
       </c>
@@ -9920,7 +9912,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="25" spans="4:6">
+    <row r="25" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D25" s="15" t="s">
         <v>161</v>
       </c>
@@ -9928,7 +9920,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="4:6">
+    <row r="26" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D26" s="15" t="s">
         <v>165</v>
       </c>
@@ -9936,7 +9928,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="27" spans="4:6">
+    <row r="27" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D27" s="15" t="s">
         <v>169</v>
       </c>
@@ -9944,7 +9936,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="28" spans="4:6">
+    <row r="28" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D28" s="15" t="s">
         <v>172</v>
       </c>
@@ -9952,7 +9944,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="29" spans="4:6">
+    <row r="29" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D29" s="15" t="s">
         <v>175</v>
       </c>
@@ -9960,7 +9952,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="4:6">
+    <row r="30" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D30" s="15" t="s">
         <v>177</v>
       </c>
@@ -9968,7 +9960,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="31" spans="4:6">
+    <row r="31" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D31" s="15" t="s">
         <v>180</v>
       </c>
@@ -9976,7 +9968,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="32" spans="4:6">
+    <row r="32" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D32" s="15" t="s">
         <v>182</v>
       </c>
@@ -9984,7 +9976,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="33" spans="4:6">
+    <row r="33" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D33" s="15" t="s">
         <v>183</v>
       </c>
@@ -9992,7 +9984,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="34" spans="4:6">
+    <row r="34" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D34" s="15" t="s">
         <v>335</v>
       </c>
@@ -10000,7 +9992,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="35" spans="4:6">
+    <row r="35" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D35" s="15" t="s">
         <v>189</v>
       </c>
@@ -10008,7 +10000,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="36" spans="4:6">
+    <row r="36" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D36" s="15" t="s">
         <v>192</v>
       </c>
@@ -10016,7 +10008,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="37" spans="4:6">
+    <row r="37" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D37" s="15" t="s">
         <v>194</v>
       </c>
@@ -10024,7 +10016,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="38" spans="4:6">
+    <row r="38" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D38" s="15" t="s">
         <v>198</v>
       </c>
@@ -10032,7 +10024,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="39" spans="4:6">
+    <row r="39" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D39" s="15" t="s">
         <v>201</v>
       </c>
@@ -10040,7 +10032,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="40" spans="4:6">
+    <row r="40" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D40" s="15" t="s">
         <v>204</v>
       </c>
@@ -10048,7 +10040,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="41" spans="4:6">
+    <row r="41" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D41" s="15" t="s">
         <v>207</v>
       </c>
@@ -10056,547 +10048,547 @@
         <v>344</v>
       </c>
     </row>
-    <row r="42" spans="4:6">
+    <row r="42" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F42" s="15" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="43" spans="4:6">
+    <row r="43" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F43" s="15" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="44" spans="4:6">
+    <row r="44" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F44" s="15" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="45" spans="4:6">
+    <row r="45" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F45" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="4:6">
+    <row r="46" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F46" s="15" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="47" spans="4:6">
+    <row r="47" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F47" s="15" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="48" spans="4:6">
+    <row r="48" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F48" s="15" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="49" spans="6:6">
+    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F49" s="15" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="50" spans="6:6">
+    <row r="50" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F50" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="6:6">
+    <row r="51" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F51" s="15" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="52" spans="6:6">
+    <row r="52" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F52" s="15" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="53" spans="6:6">
+    <row r="53" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F53" s="15" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="54" spans="6:6">
+    <row r="54" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F54" s="15" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="55" spans="6:6">
+    <row r="55" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F55" s="15" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="56" spans="6:6">
+    <row r="56" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F56" s="15" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="57" spans="6:6">
+    <row r="57" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F57" s="15" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="58" spans="6:6">
+    <row r="58" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F58" s="15" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="59" spans="6:6">
+    <row r="59" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F59" s="15" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="60" spans="6:6">
+    <row r="60" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F60" s="15" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="61" spans="6:6">
+    <row r="61" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F61" s="15" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="62" spans="6:6">
+    <row r="62" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F62" s="15" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="63" spans="6:6">
+    <row r="63" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F63" s="15" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="64" spans="6:6">
+    <row r="64" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F64" s="15" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="65" spans="6:6">
+    <row r="65" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F65" s="15" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="66" spans="6:6">
+    <row r="66" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F66" s="15" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="67" spans="6:6">
+    <row r="67" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F67" s="15" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="68" spans="6:6">
+    <row r="68" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F68" s="15" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="69" spans="6:6">
+    <row r="69" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F69" s="15" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="70" spans="6:6">
+    <row r="70" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F70" s="15" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="71" spans="6:6">
+    <row r="71" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F71" s="15" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="72" spans="6:6">
+    <row r="72" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F72" s="15" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="73" spans="6:6">
+    <row r="73" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F73" s="15" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="74" spans="6:6">
+    <row r="74" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F74" s="15" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="75" spans="6:6">
+    <row r="75" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F75" s="15" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="76" spans="6:6">
+    <row r="76" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F76" s="15" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="77" spans="6:6">
+    <row r="77" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F77" s="15" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="78" spans="6:6">
+    <row r="78" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F78" s="15" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="79" spans="6:6">
+    <row r="79" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F79" s="15" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="80" spans="6:6">
+    <row r="80" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F80" s="15" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="81" spans="6:6">
+    <row r="81" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F81" s="15" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="82" spans="6:6">
+    <row r="82" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F82" s="15" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="83" spans="6:6">
+    <row r="83" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F83" s="15" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="84" spans="6:6">
+    <row r="84" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F84" s="15" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="85" spans="6:6">
+    <row r="85" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F85" s="15" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="86" spans="6:6">
+    <row r="86" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F86" s="15" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="87" spans="6:6">
+    <row r="87" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F87" s="15" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="88" spans="6:6">
+    <row r="88" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F88" s="15" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="89" spans="6:6">
+    <row r="89" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F89" s="15" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="90" spans="6:6">
+    <row r="90" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F90" s="15" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="91" spans="6:6">
+    <row r="91" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F91" s="15" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="92" spans="6:6">
+    <row r="92" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F92" s="15" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="93" spans="6:6">
+    <row r="93" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F93" s="15" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="94" spans="6:6">
+    <row r="94" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F94" s="15" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="95" spans="6:6">
+    <row r="95" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F95" s="15" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="96" spans="6:6">
+    <row r="96" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F96" s="15" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="97" spans="6:6">
+    <row r="97" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F97" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="6:6">
+    <row r="98" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F98" s="15" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="99" spans="6:6">
+    <row r="99" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F99" s="15" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="100" spans="6:6">
+    <row r="100" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F100" s="15" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="101" spans="6:6">
+    <row r="101" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F101" s="15" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="102" spans="6:6">
+    <row r="102" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F102" s="15" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="103" spans="6:6">
+    <row r="103" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F103" s="15" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="104" spans="6:6">
+    <row r="104" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F104" s="15" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="105" spans="6:6">
+    <row r="105" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F105" s="15" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="106" spans="6:6">
+    <row r="106" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F106" s="15" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="107" spans="6:6">
+    <row r="107" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F107" s="15" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="108" spans="6:6">
+    <row r="108" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F108" s="15" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="109" spans="6:6">
+    <row r="109" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F109" s="15" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="110" spans="6:6">
+    <row r="110" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F110" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="111" spans="6:6">
+    <row r="111" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F111" s="15" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="112" spans="6:6">
+    <row r="112" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F112" s="15" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="113" spans="6:6">
+    <row r="113" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F113" s="15" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="114" spans="6:6">
+    <row r="114" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F114" s="15" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="115" spans="6:6">
+    <row r="115" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F115" s="15" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="116" spans="6:6">
+    <row r="116" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F116" s="15" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="117" spans="6:6">
+    <row r="117" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F117" s="15" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="118" spans="6:6">
+    <row r="118" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F118" s="15" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="119" spans="6:6">
+    <row r="119" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F119" s="15" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="120" spans="6:6">
+    <row r="120" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F120" s="15" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="121" spans="6:6">
+    <row r="121" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F121" s="15" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="122" spans="6:6">
+    <row r="122" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F122" s="15" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="123" spans="6:6">
+    <row r="123" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F123" s="15" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="124" spans="6:6">
+    <row r="124" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F124" s="15" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="125" spans="6:6">
+    <row r="125" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F125" s="15" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="126" spans="6:6">
+    <row r="126" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F126" s="15" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="127" spans="6:6">
+    <row r="127" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F127" s="15" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="128" spans="6:6">
+    <row r="128" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F128" s="15" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="129" spans="6:6">
+    <row r="129" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F129" s="15" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="130" spans="6:6">
+    <row r="130" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F130" s="15" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="131" spans="6:6">
+    <row r="131" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F131" s="15" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="132" spans="6:6">
+    <row r="132" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F132" s="15" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="133" spans="6:6">
+    <row r="133" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F133" s="15" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="134" spans="6:6">
+    <row r="134" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F134" s="15" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="135" spans="6:6">
+    <row r="135" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F135" s="15" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="136" spans="6:6">
+    <row r="136" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F136" s="15" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="137" spans="6:6">
+    <row r="137" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F137" s="15" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="138" spans="6:6">
+    <row r="138" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F138" s="15" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="139" spans="6:6">
+    <row r="139" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F139" s="15" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="140" spans="6:6">
+    <row r="140" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F140" s="15" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="141" spans="6:6">
+    <row r="141" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F141" s="15" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="142" spans="6:6">
+    <row r="142" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F142" s="15" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="143" spans="6:6">
+    <row r="143" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F143" s="15" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="144" spans="6:6">
+    <row r="144" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F144" s="15" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="145" spans="6:6">
+    <row r="145" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F145" s="15" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="146" spans="6:6">
+    <row r="146" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F146" s="15" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="147" spans="6:6">
+    <row r="147" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F147" s="15" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="148" spans="6:6">
+    <row r="148" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F148" s="15" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="149" spans="6:6">
+    <row r="149" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F149" s="15" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="150" spans="6:6">
+    <row r="150" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F150" s="15" t="s">
         <v>112</v>
       </c>
@@ -10615,108 +10607,108 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="92.6640625" customWidth="1"/>
+    <col min="1" max="1" width="92.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="85" t="s">
         <v>447</v>
       </c>
       <c r="B1" s="48"/>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>465</v>
       </c>

</xml_diff>